<commit_message>
fixed SQL behind Excel output, cleaned up some stuff
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -52,6 +52,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -356,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C92"/>
+  <dimension ref="A2:D120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
@@ -388,10 +456,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>45880</v>
+        <v>26184</v>
       </c>
       <c r="C4" t="n">
-        <v>35891</v>
+        <v>19952</v>
+      </c>
+      <c r="D4" t="n">
+        <v>19952</v>
       </c>
     </row>
     <row r="5">
@@ -408,10 +479,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1615</v>
+        <v>1052</v>
       </c>
       <c r="C6" t="n">
-        <v>1328</v>
+        <v>869</v>
+      </c>
+      <c r="D6" t="n">
+        <v>869</v>
       </c>
     </row>
     <row r="7">
@@ -424,991 +498,1619 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>cash and cash equivalents</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>19384</v>
-      </c>
-      <c r="C8" t="n">
-        <v>6268</v>
+          <t>adjustments to reconcile net income (loss) to net cash provided by operating activities:</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>total automotive revenues</t>
+          <t>cash and cash equivalents</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>27236</v>
+        <v>19384</v>
       </c>
       <c r="C9" t="n">
-        <v>20821</v>
+        <v>6268</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6268</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>accounts receivable net</t>
+          <t>total automotive revenues</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1886</v>
+        <v>27236</v>
       </c>
       <c r="C10" t="n">
-        <v>1324</v>
+        <v>20821</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20821</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>energy generation and storage</t>
+          <t>accounts receivable net</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3970</v>
+        <v>1886</v>
       </c>
       <c r="C11" t="n">
-        <v>2872</v>
+        <v>1324</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1324</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>inventory</t>
+          <t>depreciation amortization and impairment</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4101</v>
+        <v>2322</v>
       </c>
       <c r="C12" t="n">
-        <v>3552</v>
+        <v>2154</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2154</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>services and other</t>
+          <t>energy generation and storage</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4977</v>
+        <v>1994</v>
       </c>
       <c r="C13" t="n">
-        <v>4996</v>
+        <v>1531</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1531</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>stock-based compensation</t>
+          <t>inventory</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1734</v>
+        <v>4101</v>
       </c>
       <c r="C14" t="n">
-        <v>898</v>
+        <v>3552</v>
+      </c>
+      <c r="D14" t="n">
+        <v>3552</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>amortization of debt discounts and issuance costs</t>
+          <t>services and other</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>180</v>
+        <v>2306</v>
       </c>
       <c r="C15" t="n">
-        <v>188</v>
+        <v>2226</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2226</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>prepaid expenses and other current assets</t>
+          <t>stock-based compensation</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1346</v>
+        <v>1734</v>
       </c>
       <c r="C16" t="n">
-        <v>959</v>
+        <v>898</v>
+      </c>
+      <c r="D16" t="n">
+        <v>898</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>total revenues</t>
+          <t>amortization of debt discounts and issuance costs</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>31536</v>
+        <v>180</v>
       </c>
       <c r="C17" t="n">
-        <v>24578</v>
+        <v>188</v>
+      </c>
+      <c r="D17" t="n">
+        <v>188</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>cost of revenues</t>
-        </is>
+          <t>prepaid expenses and other current assets</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1346</v>
+      </c>
+      <c r="C18" t="n">
+        <v>959</v>
+      </c>
+      <c r="D18" t="n">
+        <v>959</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>inventory and purchase commitments write-downs</t>
+          <t>total revenues</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>202</v>
+        <v>31536</v>
       </c>
       <c r="C19" t="n">
-        <v>193</v>
+        <v>24578</v>
+      </c>
+      <c r="D19" t="n">
+        <v>24578</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>total current assets</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>26717</v>
-      </c>
-      <c r="C20" t="n">
-        <v>12103</v>
+          <t>cost of revenues</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>operating lease vehicles net</t>
+          <t>inventory and purchase commitments write-downs</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3091</v>
+        <v>202</v>
       </c>
       <c r="C21" t="n">
-        <v>2447</v>
+        <v>193</v>
+      </c>
+      <c r="D21" t="n">
+        <v>193</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>solar energy systems net</t>
+          <t>total current assets</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5979</v>
+        <v>26717</v>
       </c>
       <c r="C22" t="n">
-        <v>6138</v>
+        <v>12103</v>
+      </c>
+      <c r="D22" t="n">
+        <v>12103</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>property plant and equipment net</t>
+          <t>automotive sales</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>12747</v>
+        <v>19696</v>
       </c>
       <c r="C23" t="n">
-        <v>10396</v>
+        <v>15939</v>
+      </c>
+      <c r="D23" t="n">
+        <v>15939</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>total automotive cost of revenues</t>
+          <t>loss on disposals of fixed assets</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>20259</v>
+        <v>17</v>
       </c>
       <c r="C24" t="n">
-        <v>16398</v>
+        <v>146</v>
+      </c>
+      <c r="D24" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>operating lease right-of-use assets</t>
+          <t>operating lease vehicles net</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1558</v>
+        <v>3091</v>
       </c>
       <c r="C25" t="n">
-        <v>1218</v>
+        <v>2447</v>
+      </c>
+      <c r="D25" t="n">
+        <v>2447</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>intangible assets net</t>
+          <t>automotive leasing</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>313</v>
+        <v>563</v>
       </c>
       <c r="C26" t="n">
-        <v>339</v>
+        <v>459</v>
+      </c>
+      <c r="D26" t="n">
+        <v>459</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>accounts receivable</t>
+          <t>foreign currency transaction net loss (gain)</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>114</v>
       </c>
       <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>goodwill</t>
+          <t>solar energy systems net</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>207</v>
+        <v>5979</v>
       </c>
       <c r="C28" t="n">
-        <v>198</v>
+        <v>6138</v>
+      </c>
+      <c r="D28" t="n">
+        <v>6138</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>total cost of revenues</t>
+          <t>non-cash interest and other operating activities</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>24906</v>
+        <v>228</v>
       </c>
       <c r="C29" t="n">
-        <v>20509</v>
+        <v>186</v>
+      </c>
+      <c r="D29" t="n">
+        <v>186</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>gross profit</t>
+          <t>property plant and equipment net</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>6630</v>
+        <v>12747</v>
       </c>
       <c r="C30" t="n">
-        <v>4069</v>
+        <v>10396</v>
+      </c>
+      <c r="D30" t="n">
+        <v>10396</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>other non-current assets</t>
+          <t>total automotive cost of revenues</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2182</v>
+        <v>20259</v>
       </c>
       <c r="C31" t="n">
-        <v>1585</v>
+        <v>16398</v>
+      </c>
+      <c r="D31" t="n">
+        <v>16398</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>operating expenses</t>
-        </is>
+          <t>energy generation and storage</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1976</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1341</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1341</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>operating lease vehicles</t>
+          <t>operating cash flow related to repayment of discounted convertible senior notes</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>0</v>
       </c>
       <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>total assets</t>
+          <t>operating lease right-of-use assets</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>52148</v>
+        <v>1558</v>
       </c>
       <c r="C34" t="n">
-        <v>34309</v>
+        <v>1218</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1218</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>liabilities</t>
+          <t>changes in operating assets and liabilities net of effect of business combinations:</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>research and development</t>
+          <t>intangible assets net</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1491</v>
+        <v>313</v>
       </c>
       <c r="C36" t="n">
-        <v>1343</v>
+        <v>339</v>
+      </c>
+      <c r="D36" t="n">
+        <v>339</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>current liabilities</t>
-        </is>
+          <t>services and other</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2671</v>
+      </c>
+      <c r="C37" t="n">
+        <v>2770</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2770</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>selling general and administrative</t>
+          <t>accounts receivable</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>3145</v>
+        <v>0</v>
       </c>
       <c r="C38" t="n">
-        <v>2646</v>
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>accounts payable</t>
+          <t>goodwill</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>6051</v>
+        <v>207</v>
       </c>
       <c r="C39" t="n">
-        <v>3771</v>
+        <v>198</v>
+      </c>
+      <c r="D39" t="n">
+        <v>198</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>restructuring and other</t>
+          <t>total cost of revenues</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0</v>
+        <v>24906</v>
       </c>
       <c r="C40" t="n">
-        <v>149</v>
+        <v>20509</v>
+      </c>
+      <c r="D40" t="n">
+        <v>20509</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>accrued liabilities and other</t>
+          <t>gross profit</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3855</v>
+        <v>6630</v>
       </c>
       <c r="C41" t="n">
-        <v>3222</v>
+        <v>4069</v>
+      </c>
+      <c r="D41" t="n">
+        <v>4069</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>total operating expenses</t>
+          <t>other non-current assets</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4636</v>
+        <v>1536</v>
       </c>
       <c r="C42" t="n">
-        <v>4138</v>
+        <v>1470</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1470</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>deferred revenue</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>1458</v>
-      </c>
-      <c r="C43" t="n">
-        <v>1163</v>
+          <t>operating expenses</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>income (loss) from operations</t>
+          <t>total assets</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1994</v>
+        <v>52148</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>34309</v>
+      </c>
+      <c r="D44" t="n">
+        <v>34309</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>customer deposits</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>752</v>
-      </c>
-      <c r="C45" t="n">
-        <v>726</v>
+          <t>liabilities</t>
+        </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>interest income</t>
+          <t>prepaid expenses and other current assets</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C46" t="n">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>other long-term liabilities 5)</t>
+          <t>research and development</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>5943</v>
+        <v>1491</v>
       </c>
       <c r="C47" t="n">
-        <v>495</v>
+        <v>1343</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1343</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>current portion of debt and finance leases</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>2132</v>
-      </c>
-      <c r="C48" t="n">
-        <v>1785</v>
+          <t>current liabilities</t>
+        </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>interest expense</t>
+          <t>other non-current assets</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>0</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>115</v>
+      </c>
+      <c r="D49" t="n">
+        <v>115</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>cash flows from investing activities (3157) (1327)</t>
-        </is>
+          <t>selling general and administrative</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>3145</v>
+      </c>
+      <c r="C50" t="n">
+        <v>2646</v>
+      </c>
+      <c r="D50" t="n">
+        <v>2646</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>other (expense) income net</t>
+          <t>accounts payable</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0</v>
+        <v>6051</v>
       </c>
       <c r="C51" t="n">
-        <v>45</v>
+        <v>3771</v>
+      </c>
+      <c r="D51" t="n">
+        <v>3771</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>total current liabilities</t>
+          <t>accounts payable and accrued liabilities</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>14248</v>
+        <v>2102</v>
       </c>
       <c r="C52" t="n">
-        <v>10667</v>
+        <v>646</v>
+      </c>
+      <c r="D52" t="n">
+        <v>646</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>debt and finance leases net of current portion</t>
+          <t>restructuring and other</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>9556</v>
+        <v>0</v>
       </c>
       <c r="C53" t="n">
-        <v>11634</v>
+        <v>149</v>
+      </c>
+      <c r="D53" t="n">
+        <v>149</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>deferred revenue net of current portion</t>
+          <t>accrued liabilities and other</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1284</v>
+        <v>3855</v>
       </c>
       <c r="C54" t="n">
-        <v>1207</v>
+        <v>3222</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3222</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>provision for income taxes</t>
+          <t>deferred revenue</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>292</v>
+        <v>321</v>
       </c>
       <c r="C55" t="n">
-        <v>110</v>
+        <v>801</v>
+      </c>
+      <c r="D55" t="n">
+        <v>801</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>other long-term liabilities</t>
+          <t>total operating expenses</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3330</v>
+        <v>4636</v>
       </c>
       <c r="C56" t="n">
-        <v>2691</v>
+        <v>4138</v>
+      </c>
+      <c r="D56" t="n">
+        <v>4138</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>receipt of government grants</t>
+          <t>customer deposits</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="C57" t="n">
-        <v>46</v>
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>net income (loss) attributable to noncontrolling interests and</t>
-        </is>
+          <t>deferred revenue</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1458</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1163</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1163</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>total liabilities</t>
+          <t>income (loss) from operations</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>28418</v>
+        <v>1994</v>
       </c>
       <c r="C59" t="n">
-        <v>26199</v>
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>commitments and contingencies (note 16)</t>
-        </is>
+          <t>customer deposits</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>752</v>
+      </c>
+      <c r="C60" t="n">
+        <v>726</v>
+      </c>
+      <c r="D60" t="n">
+        <v>726</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>net cash used in investing activities (2337)</t>
-        </is>
+          <t>interest income</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>30</v>
+      </c>
+      <c r="C61" t="n">
+        <v>44</v>
+      </c>
+      <c r="D61" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>net income (loss) attributable to common stockholders</t>
+          <t>current portion of debt and finance leases</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>721</v>
+        <v>2132</v>
       </c>
       <c r="C62" t="n">
-        <v>0</v>
+        <v>1785</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1785</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>redeemable noncontrolling interests in subsidiaries</t>
+          <t>interest expense</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>745</v>
+        <v>0</v>
       </c>
       <c r="C63" t="n">
-        <v>730</v>
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>cash flows from financing activities</t>
-        </is>
+          <t>net cash provided by operating activities</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>5943</v>
+      </c>
+      <c r="C64" t="n">
+        <v>2405</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2405</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>less: buy-out of noncontrolling interest</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>31</v>
-      </c>
-      <c r="C65" t="n">
-        <v>8</v>
+          <t>cash flows from investing activities</t>
+        </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>equity</t>
-        </is>
+          <t>other (expense) income net</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" t="n">
+        <v>45</v>
+      </c>
+      <c r="D66" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>net income (loss) used in computing net</t>
-        </is>
+          <t>total current liabilities</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>14248</v>
+      </c>
+      <c r="C67" t="n">
+        <v>10667</v>
+      </c>
+      <c r="D67" t="n">
+        <v>10667</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>income (loss) per share of common stock</t>
+          <t>debt and finance leases net of current portion</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>690</v>
+        <v>9556</v>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>11634</v>
+      </c>
+      <c r="D68" t="n">
+        <v>11634</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>stockholders' equity</t>
+          <t>purchases of property and equipment excluding finance leases net of sales (3157) (1327) (2101)</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>net income (loss) per share of common stock attributable</t>
-        </is>
+          <t>deferred revenue net of current portion</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1284</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1207</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1207</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>preferred stock; par value; shares authorized;</t>
+          <t>provision for income taxes</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.001</v>
+        <v>292</v>
       </c>
       <c r="C71" t="n">
-        <v>100</v>
+        <v>110</v>
+      </c>
+      <c r="D71" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>repayments of convertible and other debt (5247)</t>
-        </is>
+          <t>purchases of solar energy systems net of sales</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>no shares issued and outstanding</t>
-        </is>
+          <t>other long-term liabilities</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>3330</v>
+      </c>
+      <c r="C73" t="n">
+        <v>2691</v>
+      </c>
+      <c r="D73" t="n">
+        <v>2691</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>basic</t>
+          <t>receipt of government grants</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>933.74</v>
+        <v>123</v>
       </c>
       <c r="C74" t="n">
-        <v>887</v>
+        <v>46</v>
+      </c>
+      <c r="D74" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>diluted</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>1083.64</v>
-      </c>
-      <c r="C75" t="n">
-        <v>887</v>
+          <t>net income (loss) attributable to noncontrolling interests and</t>
+        </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>proceeds from exercises of stock options and other stock issuances</t>
+          <t>total liabilities</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>417</v>
+        <v>28418</v>
       </c>
       <c r="C76" t="n">
-        <v>263</v>
+        <v>26199</v>
+      </c>
+      <c r="D76" t="n">
+        <v>26199</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>principal payments on finance leases</t>
+          <t>business combinations net of cash acquired</t>
         </is>
       </c>
       <c r="B77" t="n">
         <v>0</v>
       </c>
       <c r="C77" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>weighted average shares used in computing net</t>
+          <t>commitments and contingencies (note 16)</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>accumulated other comprehensive income (loss)</t>
+          <t>redeemable noncontrolling interests in subsidiaries</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>363</v>
+        <v>141</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>87</v>
+      </c>
+      <c r="D79" t="n">
+        <v>87</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>purchase of convertible note hedges</t>
+          <t>net income (loss) attributable to common stockholders</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0</v>
+        <v>721</v>
       </c>
       <c r="C80" t="n">
-        <v>174</v>
+        <v>0</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>accumulated deficit (5399) (6083)</t>
-        </is>
+          <t>redeemable noncontrolling interests in subsidiaries</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>604</v>
+      </c>
+      <c r="C81" t="n">
+        <v>643</v>
+      </c>
+      <c r="D81" t="n">
+        <v>643</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>_ prior overview period results for details. have the been accompanying adjusted to reflect the five-for-one integral stock of split these effected consolidated in the form financial of a stock dividend in august see note</t>
-        </is>
-      </c>
-      <c r="B82" t="n">
-        <v>0</v>
-      </c>
-      <c r="C82" t="n">
-        <v>1</v>
+          <t>cash flows from financing activities</t>
+        </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>proceeds from investments by noncontrolling interests in subsidiaries</t>
+          <t>less: buy-out of noncontrolling interest</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C83" t="n">
-        <v>279</v>
+        <v>8</v>
+      </c>
+      <c r="D83" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>total stockholders' equity</t>
-        </is>
-      </c>
-      <c r="B84" t="n">
-        <v>22225</v>
-      </c>
-      <c r="C84" t="n">
-        <v>6618</v>
+          <t>equity</t>
+        </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>noncontrolling interests in subsidiaries</t>
-        </is>
-      </c>
-      <c r="B85" t="n">
-        <v>850</v>
-      </c>
-      <c r="C85" t="n">
-        <v>849</v>
+          <t>net income (loss) used in computing net</t>
+        </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>total liabilities and equity</t>
+          <t>proceeds from issuances of common stock in public offerings net of issuance costs</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>52148</v>
+        <v>12269</v>
       </c>
       <c r="C86" t="n">
-        <v>34309</v>
+        <v>848</v>
+      </c>
+      <c r="D86" t="n">
+        <v>848</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>effect exchange rate changes on cash and cash equivalents and restricted cash</t>
+          <t>income (loss) per share of common stock</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>13118</v>
+        <v>690</v>
       </c>
       <c r="C87" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>cash and cash equivalents and restricted cash end period § §</t>
+          <t>proceeds from issuances of convertible and other debt</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>19901</v>
+        <v>9713</v>
       </c>
       <c r="C88" t="n">
-        <v>6.783</v>
+        <v>10669</v>
+      </c>
+      <c r="D88" t="n">
+        <v>10669</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>supplemental non-cash investing and financing activities</t>
+          <t>stockholders' equity</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>acquisitions of property and equipment included in liabilities</t>
-        </is>
-      </c>
-      <c r="B90" t="n">
-        <v>1088</v>
-      </c>
-      <c r="C90" t="n">
-        <v>562</v>
+          <t>net income (loss) per share of common stock attributable</t>
+        </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>supplemental disclosures</t>
-        </is>
+          <t>preferred stock; par value; shares authorized;</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="C91" t="n">
+        <v>100</v>
+      </c>
+      <c r="D91" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>cash paid during the period for interest net of of amounts capitalized</t>
-        </is>
-      </c>
-      <c r="B92" t="n">
+          <t>repayments of convertible and other debt (11623) (9161) (5247)</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>no shares issued and outstanding</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>basic</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="C94" t="n">
+        <v>0</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>collateralized lease repayments</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>0</v>
+      </c>
+      <c r="C95" t="n">
+        <v>0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>diluted</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="C96" t="n">
+        <v>0</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>proceeds from exercises of stock options and other stock issuances</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>417</v>
+      </c>
+      <c r="C97" t="n">
+        <v>263</v>
+      </c>
+      <c r="D97" t="n">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>principal payments on finance leases</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>0</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>weighted average shares used in computing net</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>accumulated other comprehensive income (loss)</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>363</v>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>basic</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>933</v>
+      </c>
+      <c r="C101" t="n">
+        <v>887</v>
+      </c>
+      <c r="D101" t="n">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>purchase of convertible note hedges</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0</v>
+      </c>
+      <c r="C102" t="n">
+        <v>0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>accumulated deficit (5399) (6083)</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>diluted</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>1083</v>
+      </c>
+      <c r="C104" t="n">
+        <v>887</v>
+      </c>
+      <c r="D104" t="n">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>proceeds from issuance of warrants.</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0</v>
+      </c>
+      <c r="C105" t="n">
+        <v>174</v>
+      </c>
+      <c r="D105" t="n">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>prior overview period results for details. have the been accompanying adjusted to reflect the five-for-one integral stock of split these effected consolidated in the form financial of a stock dividend in august see note</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>0</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>proceeds from investments by noncontrolling interests in subsidiaries</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>24</v>
+      </c>
+      <c r="C107" t="n">
+        <v>279</v>
+      </c>
+      <c r="D107" t="n">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>total stockholders' equity</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>22225</v>
+      </c>
+      <c r="C108" t="n">
+        <v>6618</v>
+      </c>
+      <c r="D108" t="n">
+        <v>6618</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>distributions paid to noncontrolling interests in subsidiaries</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>0</v>
+      </c>
+      <c r="C109" t="n">
+        <v>0</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>noncontrolling interests in subsidiaries</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>850</v>
+      </c>
+      <c r="C110" t="n">
+        <v>849</v>
+      </c>
+      <c r="D110" t="n">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>total liabilities and equity</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>52148</v>
+      </c>
+      <c r="C111" t="n">
+        <v>34309</v>
+      </c>
+      <c r="D111" t="n">
+        <v>34309</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>net cash provided by financing activities</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>9973</v>
+      </c>
+      <c r="C112" t="n">
+        <v>1529</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>effect of exchange rate changes on cash and cash equivalents and restricted cash</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>334</v>
+      </c>
+      <c r="C113" t="n">
+        <v>8</v>
+      </c>
+      <c r="D113" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>net increase in cash and cash equivalents and restricted cash</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>13118</v>
+      </c>
+      <c r="C114" t="n">
+        <v>2506</v>
+      </c>
+      <c r="D114" t="n">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>cash and cash equivalents and restricted cash beginning of period</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>6783</v>
+      </c>
+      <c r="C115" t="n">
+        <v>4277</v>
+      </c>
+      <c r="D115" t="n">
+        <v>4277</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>cash and cash equivalents and restricted cash end of period § §</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>19901</v>
+      </c>
+      <c r="C116" t="n">
+        <v>6.783</v>
+      </c>
+      <c r="D116" t="n">
+        <v>6.783</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>supplemental non-cash investing and financing activities</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>acquisitions of property and equipment included in liabilities</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>1088</v>
+      </c>
+      <c r="C118" t="n">
+        <v>562</v>
+      </c>
+      <c r="D118" t="n">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>supplemental disclosures</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>cash paid during the period for interest net of amounts capitalized</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
         <v>444</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C120" t="n">
+        <v>455</v>
+      </c>
+      <c r="D120" t="n">
         <v>455</v>
       </c>
     </row>

</xml_diff>

<commit_message>
still untangling the logic
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -438,357 +438,348 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>revenues</t>
+          <t>cash flows from operating activities</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>assets</t>
+          <t>adjustments to reconcile net income (loss) to net cash provided by operating activities:</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>automotive sales</t>
+          <t>depreciation amortization and impairment</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>26184</v>
+        <v>2322</v>
       </c>
       <c r="C4" t="n">
-        <v>19952</v>
+        <v>2154</v>
       </c>
       <c r="D4" t="n">
-        <v>19952</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cash flows from operating activities</t>
-        </is>
+          <t>stock-based compensation</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1734</v>
+      </c>
+      <c r="C5" t="n">
+        <v>898</v>
+      </c>
+      <c r="D5" t="n">
+        <v>898</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>automotive leasing</t>
+          <t>amortization of debt discounts and issuance costs</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1052</v>
+        <v>180</v>
       </c>
       <c r="C6" t="n">
-        <v>869</v>
+        <v>188</v>
       </c>
       <c r="D6" t="n">
-        <v>869</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>current assets</t>
-        </is>
+          <t>inventory and purchase commitments write-downs</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>202</v>
+      </c>
+      <c r="C7" t="n">
+        <v>193</v>
+      </c>
+      <c r="D7" t="n">
+        <v>193</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>adjustments to reconcile net income (loss) to net cash provided by operating activities:</t>
-        </is>
+          <t>loss on disposals of fixed assets</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>117</v>
+      </c>
+      <c r="C8" t="n">
+        <v>146</v>
+      </c>
+      <c r="D8" t="n">
+        <v>146</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cash and cash equivalents</t>
+          <t>foreign currency transaction net loss (gain)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>19384</v>
+        <v>114</v>
       </c>
       <c r="C9" t="n">
-        <v>6268</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>6268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>total automotive revenues</t>
+          <t>non-cash interest and other operating activities</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27236</v>
+        <v>228</v>
       </c>
       <c r="C10" t="n">
-        <v>20821</v>
+        <v>186</v>
       </c>
       <c r="D10" t="n">
-        <v>20821</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>accounts receivable net</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>1886</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1324</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1324</v>
+          <t>changes in operating assets and liabilities net of effect of business combinations:</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>depreciation amortization and impairment</t>
+          <t>prepaid expenses and other current assets</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2322</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>2154</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>2154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>energy generation and storage</t>
+          <t>accounts payable and accrued liabilities</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1994</v>
+        <v>2102</v>
       </c>
       <c r="C13" t="n">
-        <v>1531</v>
+        <v>646</v>
       </c>
       <c r="D13" t="n">
-        <v>1531</v>
+        <v>646</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>inventory</t>
+          <t>deferred revenue</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4101</v>
+        <v>321</v>
       </c>
       <c r="C14" t="n">
-        <v>3552</v>
+        <v>801</v>
       </c>
       <c r="D14" t="n">
-        <v>3552</v>
+        <v>801</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>services and other</t>
+          <t>customer deposits</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2306</v>
+        <v>7</v>
       </c>
       <c r="C15" t="n">
-        <v>2226</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>2226</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>stock-based compensation</t>
+          <t>other long-term liabilities</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1734</v>
+        <v>495</v>
       </c>
       <c r="C16" t="n">
-        <v>898</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>amortization of debt discounts and issuance costs</t>
+          <t>net cash provided by operating activities</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>180</v>
+        <v>5.943</v>
       </c>
       <c r="C17" t="n">
-        <v>188</v>
+        <v>2.405</v>
       </c>
       <c r="D17" t="n">
-        <v>188</v>
+        <v>2.405</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>prepaid expenses and other current assets</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>1346</v>
-      </c>
-      <c r="C18" t="n">
-        <v>959</v>
-      </c>
-      <c r="D18" t="n">
-        <v>959</v>
+          <t>cash flows from investing activities</t>
+        </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>total revenues</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>31536</v>
-      </c>
-      <c r="C19" t="n">
-        <v>24578</v>
-      </c>
-      <c r="D19" t="n">
-        <v>24578</v>
+          <t>purchases of property and equipment excluding finance leases net of sales 3157) (1327) (2101)</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>cost of revenues</t>
-        </is>
+          <t>receipt of government grants</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>123</v>
+      </c>
+      <c r="C20" t="n">
+        <v>46</v>
+      </c>
+      <c r="D20" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>inventory and purchase commitments write-downs</t>
+          <t>purchase of intangible assets</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>total current assets</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>26717</v>
-      </c>
-      <c r="C22" t="n">
-        <v>12103</v>
-      </c>
-      <c r="D22" t="n">
-        <v>12103</v>
+          <t>cash flows from financing activities</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>automotive sales</t>
+          <t>proceeds from issuances of convertible and other debt</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>19696</v>
+        <v>9713</v>
       </c>
       <c r="C23" t="n">
-        <v>15939</v>
+        <v>10669</v>
       </c>
       <c r="D23" t="n">
-        <v>15939</v>
+        <v>10669</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>loss on disposals of fixed assets</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>17</v>
-      </c>
-      <c r="C24" t="n">
-        <v>146</v>
-      </c>
-      <c r="D24" t="n">
-        <v>146</v>
+          <t>repayments of convertible and other debt (11623) (9161) (5247)</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>operating lease vehicles net</t>
+          <t>collateralized lease repayments</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3091</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>2447</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>2447</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>automotive leasing</t>
+          <t>proceeds from exercises of stock options and other stock issuances</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>563</v>
+        <v>417</v>
       </c>
       <c r="C26" t="n">
-        <v>459</v>
+        <v>263</v>
       </c>
       <c r="D26" t="n">
-        <v>459</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>foreign currency transaction net loss (gain)</t>
+          <t>purchase of convertible note hedges</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -800,152 +791,143 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>solar energy systems net</t>
+          <t>proceeds from investments by noncontrolling interests in subsidiaries</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5979</v>
+        <v>24</v>
       </c>
       <c r="C28" t="n">
-        <v>6138</v>
+        <v>279</v>
       </c>
       <c r="D28" t="n">
-        <v>6138</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>non-cash interest and other operating activities</t>
+          <t>net cash provided by financing activities</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>228</v>
+        <v>9.973000000000001</v>
       </c>
       <c r="C29" t="n">
-        <v>186</v>
+        <v>1529</v>
       </c>
       <c r="D29" t="n">
-        <v>186</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>property plant and equipment net</t>
+          <t>effect of exchange rate changes on cash and cash equivalents and restricted cash</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>12747</v>
+        <v>334</v>
       </c>
       <c r="C30" t="n">
-        <v>10396</v>
+        <v>8</v>
       </c>
       <c r="D30" t="n">
-        <v>10396</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>total automotive cost of revenues</t>
+          <t>net increase in cash and cash equivalents and restricted cash</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>20259</v>
+        <v>13118</v>
       </c>
       <c r="C31" t="n">
-        <v>16398</v>
+        <v>2506</v>
       </c>
       <c r="D31" t="n">
-        <v>16398</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>energy generation and storage</t>
+          <t>cash and cash equivalents and restricted cash beginning of period</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1976</v>
+        <v>6.783</v>
       </c>
       <c r="C32" t="n">
-        <v>1341</v>
+        <v>4277</v>
       </c>
       <c r="D32" t="n">
-        <v>1341</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>operating cash flow related to repayment of discounted convertible senior notes</t>
+          <t>cash and cash equivalents and restricted cash end of period</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>19.901</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>6.783</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>6.783</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>operating lease right-of-use assets</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>1558</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1218</v>
-      </c>
-      <c r="D34" t="n">
-        <v>1218</v>
+          <t>supplemental non-cash investing and financing activities</t>
+        </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>changes in operating assets and liabilities net of effect of business combinations:</t>
-        </is>
+          <t>acquisitions property and equipment included in liabilities</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1088</v>
+      </c>
+      <c r="C35" t="n">
+        <v>562</v>
+      </c>
+      <c r="D35" t="n">
+        <v>562</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>intangible assets net</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>313</v>
-      </c>
-      <c r="C36" t="n">
-        <v>339</v>
-      </c>
-      <c r="D36" t="n">
-        <v>339</v>
+          <t>supplemental disclosures</t>
+        </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>services and other</t>
+          <t>cash paid during the period for taxes net of the refunds accompanying notes are an integral part of these consolidated financial us statements. os</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2671</v>
+        <v>58</v>
       </c>
       <c r="C37" t="n">
-        <v>2770</v>
+        <v>54</v>
       </c>
       <c r="D37" t="n">
-        <v>2770</v>
+        <v>54</v>
       </c>
     </row>
     <row r="38">

</xml_diff>

<commit_message>
fixed a couple bugs
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -462,7 +462,7 @@
         <v>2154</v>
       </c>
       <c r="D4" t="n">
-        <v>2154</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="5">
@@ -478,7 +478,7 @@
         <v>898</v>
       </c>
       <c r="D5" t="n">
-        <v>898</v>
+        <v>749</v>
       </c>
     </row>
     <row r="6">
@@ -494,7 +494,7 @@
         <v>188</v>
       </c>
       <c r="D6" t="n">
-        <v>188</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7">
@@ -510,7 +510,7 @@
         <v>193</v>
       </c>
       <c r="D7" t="n">
-        <v>193</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8">
@@ -526,7 +526,7 @@
         <v>146</v>
       </c>
       <c r="D8" t="n">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9">
@@ -558,7 +558,7 @@
         <v>186</v>
       </c>
       <c r="D10" t="n">
-        <v>186</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         <v>646</v>
       </c>
       <c r="D13" t="n">
-        <v>646</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="14">
@@ -613,7 +613,7 @@
         <v>801</v>
       </c>
       <c r="D14" t="n">
-        <v>801</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15">
@@ -661,7 +661,7 @@
         <v>2.405</v>
       </c>
       <c r="D17" t="n">
-        <v>2.405</v>
+        <v>2.098</v>
       </c>
     </row>
     <row r="18">
@@ -691,7 +691,7 @@
         <v>46</v>
       </c>
       <c r="D20" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -730,7 +730,7 @@
         <v>10669</v>
       </c>
       <c r="D23" t="n">
-        <v>10669</v>
+        <v>6176</v>
       </c>
     </row>
     <row r="24">
@@ -769,7 +769,7 @@
         <v>263</v>
       </c>
       <c r="D26" t="n">
-        <v>263</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27">
@@ -801,7 +801,7 @@
         <v>279</v>
       </c>
       <c r="D28" t="n">
-        <v>279</v>
+        <v>437</v>
       </c>
     </row>
     <row r="29">
@@ -817,7 +817,7 @@
         <v>1529</v>
       </c>
       <c r="D29" t="n">
-        <v>1529</v>
+        <v>574</v>
       </c>
     </row>
     <row r="30">
@@ -833,7 +833,7 @@
         <v>8</v>
       </c>
       <c r="D30" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -849,7 +849,7 @@
         <v>2506</v>
       </c>
       <c r="D31" t="n">
-        <v>2506</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32">
@@ -865,7 +865,7 @@
         <v>4277</v>
       </c>
       <c r="D32" t="n">
-        <v>4277</v>
+        <v>3965</v>
       </c>
     </row>
     <row r="33">
@@ -881,7 +881,7 @@
         <v>6.783</v>
       </c>
       <c r="D33" t="n">
-        <v>6.783</v>
+        <v>4.277</v>
       </c>
     </row>
     <row r="34">
@@ -904,7 +904,7 @@
         <v>562</v>
       </c>
       <c r="D35" t="n">
-        <v>562</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36">
@@ -927,7 +927,7 @@
         <v>54</v>
       </c>
       <c r="D37" t="n">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38">

</xml_diff>

<commit_message>
making sure its up to date
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -438,512 +438,413 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>cash flows from operating activities</t>
+          <t xml:space="preserve"> depreciation and amortization</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>adjustments to reconcile net income (loss) to net cash provided by operating activities:</t>
+          <t xml:space="preserve"> stock-based compensation expense</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>depreciation amortization and impairment</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2322</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2154</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1901</v>
+          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>stock-based compensation</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1734</v>
-      </c>
-      <c r="C5" t="n">
-        <v>898</v>
-      </c>
-      <c r="D5" t="n">
-        <v>749</v>
+          <t xml:space="preserve"> other</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>amortization of debt discounts and issuance costs</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>180</v>
-      </c>
-      <c r="C6" t="n">
-        <v>188</v>
-      </c>
-      <c r="D6" t="n">
-        <v>159</v>
+          <t xml:space="preserve"> trade and other accounts receivable net</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>inventory and purchase commitments write-downs</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>202</v>
-      </c>
-      <c r="C7" t="n">
-        <v>193</v>
-      </c>
-      <c r="D7" t="n">
-        <v>85</v>
+          <t xml:space="preserve"> inventories</t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>loss on disposals of fixed assets</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>117</v>
-      </c>
-      <c r="C8" t="n">
-        <v>146</v>
-      </c>
-      <c r="D8" t="n">
-        <v>162</v>
+          <t xml:space="preserve"> prepaid expenses and other</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>foreign currency transaction net loss (gain)</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>114</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
+          <t xml:space="preserve"> deposits and other</t>
+        </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>non-cash interest and other operating activities</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>228</v>
-      </c>
-      <c r="C10" t="n">
-        <v>186</v>
-      </c>
-      <c r="D10" t="n">
-        <v>49</v>
+          <t xml:space="preserve"> accounts payable</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>changes in operating assets and liabilities net of effect of business combinations:</t>
+          <t xml:space="preserve"> accrued expenses</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>prepaid expenses and other current assets</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
+          <t xml:space="preserve"> deferred rent</t>
+        </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>accounts payable and accrued liabilities</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>2102</v>
-      </c>
-      <c r="C13" t="n">
-        <v>646</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1797</v>
+          <t xml:space="preserve"> other net long-term cash provided liabilities by operating activities</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>deferred revenue</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>321</v>
-      </c>
-      <c r="C14" t="n">
-        <v>801</v>
-      </c>
-      <c r="D14" t="n">
-        <v>406</v>
+          <t xml:space="preserve"> additions to property and equipment</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>customer deposits</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>7</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
+          <t xml:space="preserve"> proceeds net from cash sale-leaseback used in investing transactions activities</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>other long-term liabilities</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>495</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
+          <t xml:space="preserve"> exercise of employee stock options</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>net cash provided by operating activities</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>5.943</v>
-      </c>
-      <c r="C17" t="n">
-        <v>2.405</v>
-      </c>
-      <c r="D17" t="n">
-        <v>2.098</v>
+          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
+        </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>cash flows from investing activities</t>
+          <t xml:space="preserve"> proceeds net from cash issuance used in financing of common activities stock under employee benefit plans</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>purchases of property and equipment excluding finance leases net of sales 3157) (1327) (2101)</t>
+          <t xml:space="preserve"> net increase (decrease) in cash and cash equivalents</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>receipt of government grants</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>123</v>
-      </c>
-      <c r="C20" t="n">
-        <v>46</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
+          <t xml:space="preserve"> cash and cash equivalents at beginning of period</t>
+        </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>purchase of intangible assets</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
+          <t xml:space="preserve"> cash and cash equivalents at end of the period accompanying notes are an integral part of the consolidated financial statements.</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>cash flows from financing activities</t>
-        </is>
+          <t xml:space="preserve"> business combinations net of cash acquired</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-13</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-45</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>proceeds from issuances of convertible and other debt</t>
+          <t xml:space="preserve"> net cash used in investing activities</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>9713</v>
+        <v>-3132</v>
       </c>
       <c r="C23" t="n">
-        <v>10669</v>
+        <v>-1436</v>
       </c>
       <c r="D23" t="n">
-        <v>6176</v>
+        <v>-2337</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>repayments of convertible and other debt (11623) (9161) (5247)</t>
-        </is>
+          <t xml:space="preserve"> proceeds from issuances of convertible and other debt</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>9713</v>
+      </c>
+      <c r="C24" t="n">
+        <v>10669</v>
+      </c>
+      <c r="D24" t="n">
+        <v>6176</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>collateralized lease repayments</t>
+          <t xml:space="preserve"> repayments of convertible and other debt</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>-11623</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>-9161</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>-5247</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>proceeds from exercises of stock options and other stock issuances</t>
+          <t xml:space="preserve"> collateralized lease repayments</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>417</v>
+        <v>-240</v>
       </c>
       <c r="C26" t="n">
-        <v>263</v>
+        <v>-389</v>
       </c>
       <c r="D26" t="n">
-        <v>296</v>
+        <v>-559</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>purchase of convertible note hedges</t>
+          <t xml:space="preserve"> proceeds from exercises of stock options and other stock issuances</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>417</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>263</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>proceeds from investments by noncontrolling interests in subsidiaries</t>
+          <t xml:space="preserve"> principal payments on finance leases</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>24</v>
+        <v>-338</v>
       </c>
       <c r="C28" t="n">
-        <v>279</v>
+        <v>-321</v>
       </c>
       <c r="D28" t="n">
-        <v>437</v>
+        <v>-181</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>net cash provided by financing activities</t>
+          <t xml:space="preserve"> debt issuance costs</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>9.973000000000001</v>
+        <v>-6</v>
       </c>
       <c r="C29" t="n">
-        <v>1529</v>
+        <v>-37</v>
       </c>
       <c r="D29" t="n">
-        <v>574</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>effect of exchange rate changes on cash and cash equivalents and restricted cash</t>
+          <t xml:space="preserve"> proceeds from investments by noncontrolling interests in subsidiaries</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>334</v>
+        <v>24</v>
       </c>
       <c r="C30" t="n">
-        <v>8</v>
+        <v>279</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>net increase in cash and cash equivalents and restricted cash</t>
+          <t xml:space="preserve"> distributions paid to noncontrolling interests in subsidiaries gl)</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>13118</v>
+        <v>-208</v>
       </c>
       <c r="C31" t="n">
-        <v>2506</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>312</v>
+        <v>-227</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>cash and cash equivalents and restricted cash beginning of period</t>
+          <t xml:space="preserve"> payments for buy-outs of noncontrolling interests in subsidiaries</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>6.783</v>
+        <v>-35</v>
       </c>
       <c r="C32" t="n">
-        <v>4277</v>
+        <v>-9</v>
       </c>
       <c r="D32" t="n">
-        <v>3965</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>cash and cash equivalents and restricted cash end of period</t>
+          <t xml:space="preserve"> net cash provided by financing activities</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>19.901</v>
+        <v>9973</v>
       </c>
       <c r="C33" t="n">
-        <v>6.783</v>
+        <v>1529</v>
       </c>
       <c r="D33" t="n">
-        <v>4.277</v>
+        <v>574</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>supplemental non-cash investing and financing activities</t>
-        </is>
+          <t xml:space="preserve"> effect of exchange rate changes on cash and cash equivalents and restricted cash</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>334</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-23</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>acquisitions property and equipment included in liabilities</t>
+          <t xml:space="preserve"> net increase in cash and cash equivalents and restricted cash</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1088</v>
+        <v>13118</v>
       </c>
       <c r="C35" t="n">
-        <v>562</v>
+        <v>2506</v>
       </c>
       <c r="D35" t="n">
-        <v>249</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>supplemental disclosures</t>
-        </is>
+          <t xml:space="preserve"> cash and cash equivalents and restricted cash beginning of period</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>6783</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4277</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3965</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>cash paid during the period for taxes net of the refunds accompanying notes are an integral part of these consolidated financial us statements. os</t>
+          <t xml:space="preserve"> cash and cash equivalents and restricted cash end of period</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>58</v>
+        <v>19901</v>
       </c>
       <c r="C37" t="n">
-        <v>54</v>
+        <v>6783</v>
       </c>
       <c r="D37" t="n">
-        <v>35</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>accounts receivable</t>
+          <t xml:space="preserve"> acquisitions of property and equipment included in liabilities</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1088</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>562</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>249</v>
       </c>
     </row>
     <row r="39">

</xml_diff>

<commit_message>
working on improving column recognition
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -466,273 +466,192 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> trade and other accounts receivable net</t>
+          <t xml:space="preserve"> inventories</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> inventories</t>
+          <t xml:space="preserve"> prepaid expenses and other</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> prepaid expenses and other</t>
+          <t xml:space="preserve"> deposits and other</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deposits and other</t>
+          <t xml:space="preserve"> accounts payable</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable</t>
+          <t xml:space="preserve"> accrued expenses</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accrued expenses</t>
+          <t xml:space="preserve"> deferred rent</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred rent</t>
+          <t xml:space="preserve"> other net long-term cash provided liabilities by operating activities</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other net long-term cash provided liabilities by operating activities</t>
+          <t xml:space="preserve"> additions to property and equipment</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> additions to property and equipment</t>
+          <t xml:space="preserve"> proceeds net from cash sale-leaseback used in investing transactions activities</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds net from cash sale-leaseback used in investing transactions activities</t>
+          <t xml:space="preserve"> exercise of employee stock options</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> exercise of employee stock options</t>
+          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
+          <t xml:space="preserve"> cash and cash equivalents at end of the period accompanying notes are an integral part of the consolidated financial statements.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds net from cash issuance used in financing of common activities stock under employee benefit plans</t>
+          <t xml:space="preserve"> net cash provided by operating activities</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> net increase (decrease) in cash and cash equivalents</t>
+          <t xml:space="preserve"> purchases of solar energy systems net of sales</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents at beginning of period</t>
+          <t xml:space="preserve"> business combinations net of cash acquired</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents at end of the period accompanying notes are an integral part of the consolidated financial statements.</t>
+          <t xml:space="preserve"> net cash used in investing activities</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> business combinations net of cash acquired</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>-13</v>
-      </c>
-      <c r="C22" t="n">
-        <v>-45</v>
-      </c>
-      <c r="D22" t="n">
-        <v>-18</v>
+          <t xml:space="preserve"> proceeds from issuances of convertible and other debt</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> net cash used in investing activities</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>-3132</v>
-      </c>
-      <c r="C23" t="n">
-        <v>-1436</v>
-      </c>
-      <c r="D23" t="n">
-        <v>-2337</v>
+          <t xml:space="preserve"> repayments of convertible and other debt</t>
+        </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds from issuances of convertible and other debt</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>9713</v>
-      </c>
-      <c r="C24" t="n">
-        <v>10669</v>
-      </c>
-      <c r="D24" t="n">
-        <v>6176</v>
+          <t xml:space="preserve"> collateralized lease repayments</t>
+        </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> repayments of convertible and other debt</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>-11623</v>
-      </c>
-      <c r="C25" t="n">
-        <v>-9161</v>
-      </c>
-      <c r="D25" t="n">
-        <v>-5247</v>
+          <t xml:space="preserve"> principal payments on finance leases</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> collateralized lease repayments</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>-240</v>
-      </c>
-      <c r="C26" t="n">
-        <v>-389</v>
-      </c>
-      <c r="D26" t="n">
-        <v>-559</v>
+          <t xml:space="preserve"> debt issuance costs</t>
+        </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds from exercises of stock options and other stock issuances</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>417</v>
-      </c>
-      <c r="C27" t="n">
-        <v>263</v>
-      </c>
-      <c r="D27" t="n">
-        <v>296</v>
+          <t xml:space="preserve"> distributions paid to noncontrolling interests in subsidiaries gl)</t>
+        </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> principal payments on finance leases</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>-338</v>
-      </c>
-      <c r="C28" t="n">
-        <v>-321</v>
-      </c>
-      <c r="D28" t="n">
-        <v>-181</v>
+          <t xml:space="preserve"> payments for buy-outs of noncontrolling interests in subsidiaries</t>
+        </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> debt issuance costs</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>-6</v>
-      </c>
-      <c r="C29" t="n">
-        <v>-37</v>
-      </c>
-      <c r="D29" t="n">
-        <v>-15</v>
+          <t xml:space="preserve"> net cash provided by financing activities</t>
+        </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds from investments by noncontrolling interests in subsidiaries</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>24</v>
-      </c>
-      <c r="C30" t="n">
-        <v>279</v>
-      </c>
-      <c r="D30" t="n">
-        <v>437</v>
+          <t xml:space="preserve"> net increase in cash and cash equivalents and restricted cash</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> distributions paid to noncontrolling interests in subsidiaries gl)</t>
+          <t xml:space="preserve"> net increase in cash and cash equivalents and restricted cash</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-208</v>
+        <v>13118</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>2506</v>
       </c>
       <c r="D31" t="n">
-        <v>-227</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32">

</xml_diff>

<commit_message>
gets column headers properly from Tesla and Panera public statements
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -438,190 +438,280 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
+          <t xml:space="preserve"> net income</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> stock-based compensation expense</t>
+          <t xml:space="preserve"> depreciation and amortization</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
+          <t xml:space="preserve"> stock-based compensation expense</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other</t>
+          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> inventories</t>
+          <t xml:space="preserve"> other</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> prepaid expenses and other</t>
+          <t xml:space="preserve"> inventories</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deposits and other</t>
+          <t xml:space="preserve"> prepaid expenses and other</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable</t>
+          <t xml:space="preserve"> deposits and other</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accrued expenses</t>
+          <t xml:space="preserve"> accounts payable</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred rent</t>
+          <t xml:space="preserve"> accrued expenses</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other net long-term cash provided liabilities by operating activities</t>
+          <t xml:space="preserve"> deferred rent</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> additions to property and equipment</t>
+          <t xml:space="preserve"> other net long-term cash provided liabilities by operating activities</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds net from cash sale-leaseback used in investing transactions activities</t>
+          <t xml:space="preserve"> additions to property and equipment</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> exercise of employee stock options</t>
+          <t xml:space="preserve"> proceeds net from cash sale-leaseback used in investing transactions activities</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
+          <t xml:space="preserve"> exercise of employee stock options</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents at end of the period accompanying notes are an integral part of the consolidated financial statements.</t>
+          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> net cash provided by operating activities</t>
+          <t xml:space="preserve"> cash and cash equivalents at end of the period accompanying notes are an integral part of the consolidated financial statements.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> purchases of solar energy systems net of sales</t>
-        </is>
+          <t xml:space="preserve"> net cash provided by operating activities</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>5943</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2405</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2098</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> business combinations net of cash acquired</t>
-        </is>
+          <t xml:space="preserve"> purchases of solar energy systems net of sales</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-75</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-105</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-218</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> net cash used in investing activities</t>
-        </is>
+          <t xml:space="preserve"> business combinations net of cash acquired</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-13</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-45</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds from issuances of convertible and other debt</t>
-        </is>
+          <t xml:space="preserve"> net cash used in investing activities</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-3132</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-1436</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-2337</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> repayments of convertible and other debt</t>
-        </is>
+          <t xml:space="preserve"> proceeds from issuances of convertible and other debt</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>9713</v>
+      </c>
+      <c r="C23" t="n">
+        <v>10669</v>
+      </c>
+      <c r="D23" t="n">
+        <v>6176</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> collateralized lease repayments</t>
-        </is>
+          <t xml:space="preserve"> repayments of convertible and other debt</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-11623</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-9161</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-5247</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> principal payments on finance leases</t>
-        </is>
+          <t xml:space="preserve"> collateralized lease repayments</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>-240</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-389</v>
+      </c>
+      <c r="D25" t="n">
+        <v>-559</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> debt issuance costs</t>
-        </is>
+          <t xml:space="preserve"> principal payments on finance leases</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-338</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-321</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-181</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> distributions paid to noncontrolling interests in subsidiaries gl)</t>
-        </is>
+          <t xml:space="preserve"> debt issuance costs</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-6</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-37</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-15</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> payments for buy-outs of noncontrolling interests in subsidiaries</t>
-        </is>
+          <t xml:space="preserve"> distributions paid to noncontrolling interests in subsidiaries gl)</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>-208</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-227</v>
       </c>
     </row>
     <row r="29">
@@ -630,28 +720,40 @@
           <t xml:space="preserve"> net cash provided by financing activities</t>
         </is>
       </c>
+      <c r="B29" t="n">
+        <v>9973</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1529</v>
+      </c>
+      <c r="D29" t="n">
+        <v>574</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> net increase in cash and cash equivalents and restricted cash</t>
-        </is>
+          <t xml:space="preserve"> noncontrolling interests in subsidiaries</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>850</v>
+      </c>
+      <c r="C30" t="n">
+        <v>849</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> net increase in cash and cash equivalents and restricted cash</t>
+          <t xml:space="preserve"> total liabilities and equity </t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>13118</v>
+        <v>52148</v>
       </c>
       <c r="C31" t="n">
-        <v>2506</v>
-      </c>
-      <c r="D31" t="n">
-        <v>312</v>
+        <v>34309</v>
       </c>
     </row>
     <row r="32">

</xml_diff>

<commit_message>
almost done fixing known issues
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -438,120 +438,273 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> net income</t>
-        </is>
+          <t xml:space="preserve"> net income (loss)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>862</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-775</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-1063</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
-        </is>
+          <t xml:space="preserve"> depreciation amortization and impairment</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2322</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2154</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1901</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> stock-based compensation expense</t>
-        </is>
+          <t xml:space="preserve"> stock-based compensation</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1734</v>
+      </c>
+      <c r="C4" t="n">
+        <v>898</v>
+      </c>
+      <c r="D4" t="n">
+        <v>749</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
+          <t xml:space="preserve"> amortization of debt discounts and issuance costs</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>180</v>
+      </c>
+      <c r="C5" t="n">
+        <v>188</v>
+      </c>
+      <c r="D5" t="n">
+        <v>159</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other</t>
-        </is>
+          <t xml:space="preserve"> inventory and purchase commitments write-downs</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>202</v>
+      </c>
+      <c r="C6" t="n">
+        <v>193</v>
+      </c>
+      <c r="D6" t="n">
+        <v>85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> inventories</t>
-        </is>
+          <t xml:space="preserve"> loss on disposals of fixed assets</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>117</v>
+      </c>
+      <c r="C7" t="n">
+        <v>146</v>
+      </c>
+      <c r="D7" t="n">
+        <v>162</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> prepaid expenses and other</t>
-        </is>
+          <t xml:space="preserve"> foreign currency transaction net loss (gain)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>114</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-48</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deposits and other</t>
-        </is>
+          <t xml:space="preserve"> non-cash interest and other operating activities</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>228</v>
+      </c>
+      <c r="C9" t="n">
+        <v>186</v>
+      </c>
+      <c r="D9" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable</t>
-        </is>
+          <t xml:space="preserve"> accounts receivable</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>-652</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-367</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-497</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accrued expenses</t>
-        </is>
+          <t xml:space="preserve"> inventory</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-422</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-429</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-1023</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred rent</t>
-        </is>
+          <t xml:space="preserve"> operating lease vehicles</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>-1072</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-764</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-215</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other net long-term cash provided liabilities by operating activities</t>
-        </is>
+          <t xml:space="preserve"> prepaid expenses and other current assets</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-251</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-288</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-82</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> additions to property and equipment</t>
-        </is>
+          <t xml:space="preserve"> other non-current assets.</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>-344</v>
+      </c>
+      <c r="C14" t="n">
+        <v>115</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-207</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> proceeds net from cash sale-leaseback used in investing transactions activities</t>
-        </is>
+          <t xml:space="preserve"> accounts payable and accrued liabilities</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2102</v>
+      </c>
+      <c r="C15" t="n">
+        <v>646</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1797</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> exercise of employee stock options</t>
-        </is>
+          <t xml:space="preserve"> deferred revenue</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>321</v>
+      </c>
+      <c r="C16" t="n">
+        <v>801</v>
+      </c>
+      <c r="D16" t="n">
+        <v>406</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
+          <t xml:space="preserve"> customer deposits</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-58</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-96</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents at end of the period accompanying notes are an integral part of the consolidated financial statements.</t>
-        </is>
+          <t xml:space="preserve"> other long-term liabilities</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>495</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-25</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
got it down to 624 lines
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -491,17 +491,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>december 29, 2015</t>
+          <t>september 29,</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>december 30, 2014</t>
+          <t>september 30, 2017</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>september 24,</t>
         </is>
       </c>
     </row>
@@ -510,20 +510,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents</t>
+          <t xml:space="preserve"> net income</t>
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>241886</v>
+        <v>59531</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>196493</v>
+        <v>48351</v>
       </c>
-      <c r="F2" s="3" t="n"/>
+      <c r="F2" s="3" t="n">
+        <v>45687</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -534,34 +536,36 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> trade accounts receivable net</t>
+          <t xml:space="preserve"> respectively</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>38211</v>
+        <v>-525</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>36584</v>
+        <v>224</v>
       </c>
-      <c r="F3" s="3" t="n"/>
+      <c r="F3" s="3" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other accounts receivable</t>
+          <t xml:space="preserve"> (478) and (7) respectively</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>77575</v>
+        <v>523</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>70069</v>
+        <v>1315</v>
       </c>
       <c r="F4" s="3" t="n"/>
     </row>
@@ -570,1896 +574,540 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> inventories</t>
+          <t xml:space="preserve"> of tax</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>22482</v>
+        <v>905</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>22811</v>
+        <v>-162</v>
       </c>
-      <c r="F5" s="3" t="n"/>
+      <c r="F5" s="3" t="n">
+        <v>-734</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> prepaid and other</t>
+          <t xml:space="preserve"> and (863) respectively</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>59457</v>
+        <v>-3407</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>51588</v>
+        <v>-782</v>
       </c>
-      <c r="F6" s="3" t="n"/>
+      <c r="F6" s="3" t="n">
+        <v>1582</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> veferred income taxes</t>
+          <t xml:space="preserve"> tax</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>34479</v>
+        <v>-3406</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>28621</v>
+        <v>-846</v>
       </c>
-      <c r="F7" s="3" t="n"/>
+      <c r="F7" s="3" t="n">
+        <v>1638</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> assets held for sale</t>
+          <t xml:space="preserve"> total other cuniprehensive incuine/(loss)</t>
         </is>
       </c>
       <c r="D8" s="3" t="n">
-        <v>28699</v>
+        <v>-3026</v>
       </c>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="n"/>
+      <c r="E8" s="3" t="n">
+        <v>-784</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>979</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current assets</t>
+          <t xml:space="preserve"> total comprehensive income see accompanying apple notes inc. to | consolidated fun 10-k financial | statements</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>502789</v>
+        <v>56505</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>406166</v>
+        <v>47567</v>
       </c>
-      <c r="F9" s="3" t="n"/>
+      <c r="F9" s="3" t="n">
+        <v>46666</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" t="n">
-        <v>12</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> property and equipment net</t>
-        </is>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>776248</v>
-      </c>
-      <c r="E10" s="3" t="n">
-        <v>787294</v>
-      </c>
+      <c r="D10" s="3" t="n"/>
+      <c r="E10" s="3" t="n"/>
       <c r="F10" s="3" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" t="n">
-        <v>14</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> goodwill</t>
-        </is>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>121791</v>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>120778</v>
-      </c>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="3" t="n"/>
       <c r="F11" s="3" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" t="n">
-        <v>15</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other intangible assets net</t>
-        </is>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>63877</v>
-      </c>
-      <c r="E12" s="3" t="n">
-        <v>70940</v>
-      </c>
+      <c r="D12" s="3" t="n"/>
+      <c r="E12" s="3" t="n"/>
       <c r="F12" s="3" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" t="n">
-        <v>16</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deposits and other</t>
-        </is>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>10613</v>
-      </c>
-      <c r="E13" s="3" t="n">
-        <v>5508</v>
-      </c>
+      <c r="D13" s="3" t="n"/>
+      <c r="E13" s="3" t="n"/>
       <c r="F13" s="3" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" t="n">
-        <v>17</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total other assets</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>196281</v>
-      </c>
-      <c r="E14" s="3" t="n">
-        <v>197226</v>
-      </c>
+      <c r="D14" s="3" t="n"/>
+      <c r="E14" s="3" t="n"/>
       <c r="F14" s="3" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" t="n">
-        <v>18</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total assets</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>1475318</v>
-      </c>
-      <c r="E15" s="3" t="n">
-        <v>1390686</v>
-      </c>
+      <c r="D15" s="3" t="n"/>
+      <c r="E15" s="3" t="n"/>
       <c r="F15" s="3" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" t="n">
-        <v>21</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accounts payable</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>19805</v>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>19511</v>
-      </c>
+      <c r="D16" s="3" t="n"/>
+      <c r="E16" s="3" t="n"/>
       <c r="F16" s="3" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" t="n">
-        <v>22</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accrued expenses</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>359464</v>
-      </c>
-      <c r="E17" s="3" t="n">
-        <v>333201</v>
-      </c>
+      <c r="D17" s="3" t="n"/>
+      <c r="E17" s="3" t="n"/>
       <c r="F17" s="3" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" t="n">
-        <v>1</v>
-      </c>
-      <c r="B18" t="n">
-        <v>23</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cunent portion of long-term debt</t>
-        </is>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>17229</v>
-      </c>
+      <c r="D18" s="3" t="n"/>
       <c r="E18" s="3" t="n"/>
       <c r="F18" s="3" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" t="n">
-        <v>24</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> liabilities associated with assets held for sale</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>2945</v>
-      </c>
+      <c r="D19" s="3" t="n"/>
       <c r="E19" s="3" t="n"/>
       <c r="F19" s="3" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" t="n">
-        <v>25</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total current liabilities</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>399443</v>
-      </c>
-      <c r="E20" s="3" t="n">
-        <v>352712</v>
-      </c>
+      <c r="D20" s="3" t="n"/>
+      <c r="E20" s="3" t="n"/>
       <c r="F20" s="3" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" t="n">
-        <v>1</v>
-      </c>
-      <c r="B21" t="n">
-        <v>26</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> long-term debt</t>
-        </is>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>388971</v>
-      </c>
-      <c r="E21" s="3" t="n">
-        <v>99784</v>
-      </c>
+      <c r="D21" s="3" t="n"/>
+      <c r="E21" s="3" t="n"/>
       <c r="F21" s="3" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B22" t="n">
-        <v>27</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred rent</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>62610</v>
-      </c>
-      <c r="E22" s="3" t="n">
-        <v>67390</v>
-      </c>
+      <c r="D22" s="3" t="n"/>
+      <c r="E22" s="3" t="n"/>
       <c r="F22" s="3" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" t="n">
-        <v>1</v>
-      </c>
-      <c r="B23" t="n">
-        <v>28</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred income taxes</t>
-        </is>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>70447</v>
-      </c>
-      <c r="E23" s="3" t="n">
-        <v>76589</v>
-      </c>
+      <c r="D23" s="3" t="n"/>
+      <c r="E23" s="3" t="n"/>
       <c r="F23" s="3" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" t="n">
-        <v>1</v>
-      </c>
-      <c r="B24" t="n">
-        <v>29</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
-        </is>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>52566</v>
-      </c>
-      <c r="E24" s="3" t="n">
-        <v>58027</v>
-      </c>
+      <c r="D24" s="3" t="n"/>
+      <c r="E24" s="3" t="n"/>
       <c r="F24" s="3" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" t="n">
-        <v>1</v>
-      </c>
-      <c r="B25" t="n">
-        <v>30</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total liabilities</t>
-        </is>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>974037</v>
-      </c>
-      <c r="E25" s="3" t="n">
-        <v>654502</v>
-      </c>
+      <c r="D25" s="3" t="n"/>
+      <c r="E25" s="3" t="n"/>
       <c r="F25" s="3" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" t="n">
-        <v>32</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> redeemable noncontrolling interest</t>
-        </is>
-      </c>
-      <c r="D26" s="3" t="n">
-        <v>3981</v>
-      </c>
+      <c r="D26" s="3" t="n"/>
       <c r="E26" s="3" t="n"/>
       <c r="F26" s="3" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>1</v>
-      </c>
-      <c r="B27" t="n">
-        <v>39</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> treasury stock carried at cost; shares at december and shares at</t>
-        </is>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>-1111586</v>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>-706073</v>
-      </c>
+      <c r="D27" s="3" t="n"/>
+      <c r="E27" s="3" t="n"/>
       <c r="F27" s="3" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" t="n">
-        <v>43</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> additional paid-in capital</t>
-        </is>
-      </c>
-      <c r="D28" s="3" t="n">
-        <v>235393</v>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>214437</v>
-      </c>
+      <c r="D28" s="3" t="n"/>
+      <c r="E28" s="3" t="n"/>
       <c r="F28" s="3" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" t="n">
-        <v>44</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accumulated other comprehensive income (loss)</t>
-        </is>
-      </c>
-      <c r="D29" s="3" t="n">
-        <v>-5029</v>
-      </c>
-      <c r="E29" s="3" t="n">
-        <v>-1360</v>
-      </c>
+      <c r="D29" s="3" t="n"/>
+      <c r="E29" s="3" t="n"/>
       <c r="F29" s="3" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" t="n">
-        <v>45</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> retained ca:uings</t>
-        </is>
-      </c>
-      <c r="D30" s="3" t="n">
-        <v>1378519</v>
-      </c>
-      <c r="E30" s="3" t="n">
-        <v>1229177</v>
-      </c>
+      <c r="D30" s="3" t="n"/>
+      <c r="E30" s="3" t="n"/>
       <c r="F30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" t="n">
-        <v>46</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total stockholders' equity</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="n">
-        <v>497300</v>
-      </c>
-      <c r="E31" s="3" t="n">
-        <v>736184</v>
-      </c>
+      <c r="D31" s="3" t="n"/>
+      <c r="E31" s="3" t="n"/>
       <c r="F31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" t="n">
-        <v>47</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total liabilities redeemable the accompanying noncontrolling notes interest are an and integral stockholders' part of equity the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>1475318</v>
-      </c>
-      <c r="E32" s="3" t="n">
-        <v>1390686</v>
-      </c>
+      <c r="D32" s="3" t="n"/>
+      <c r="E32" s="3" t="n"/>
       <c r="F32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>2</v>
-      </c>
-      <c r="B33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> bakery-cafe sales net</t>
-        </is>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>2358794</v>
-      </c>
-      <c r="E33" s="3" t="n">
-        <v>2230370</v>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>2108908</v>
-      </c>
+      <c r="D33" s="3" t="n"/>
+      <c r="E33" s="3" t="n"/>
+      <c r="F33" s="3" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>2</v>
-      </c>
-      <c r="B34" t="n">
-        <v>3</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> franchise royalties and fees</t>
-        </is>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>138563</v>
-      </c>
-      <c r="E34" s="3" t="n">
-        <v>123686</v>
-      </c>
-      <c r="F34" s="3" t="n">
-        <v>112641</v>
-      </c>
+      <c r="D34" s="3" t="n"/>
+      <c r="E34" s="3" t="n"/>
+      <c r="F34" s="3" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>2</v>
-      </c>
-      <c r="B35" t="n">
-        <v>4</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> fresh dough and other product sales to franchisees</t>
-        </is>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>184223</v>
-      </c>
-      <c r="E35" s="3" t="n">
-        <v>175139</v>
-      </c>
-      <c r="F35" s="3" t="n">
-        <v>163453</v>
-      </c>
+      <c r="D35" s="3" t="n"/>
+      <c r="E35" s="3" t="n"/>
+      <c r="F35" s="3" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>2</v>
-      </c>
-      <c r="B36" t="n">
-        <v>5</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total</t>
-        </is>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>2681580</v>
-      </c>
-      <c r="E36" s="3" t="n">
-        <v>2529195</v>
-      </c>
-      <c r="F36" s="3" t="n">
-        <v>2385002</v>
-      </c>
+      <c r="D36" s="3" t="n"/>
+      <c r="E36" s="3" t="n"/>
+      <c r="F36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>2</v>
-      </c>
-      <c r="B37" t="n">
-        <v>10</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cost of food and paper products</t>
-        </is>
-      </c>
-      <c r="D37" s="3" t="n">
-        <v>715502</v>
-      </c>
-      <c r="E37" s="3" t="n">
-        <v>669860</v>
-      </c>
-      <c r="F37" s="3" t="n">
-        <v>625622</v>
-      </c>
+      <c r="D37" s="3" t="n"/>
+      <c r="E37" s="3" t="n"/>
+      <c r="F37" s="3" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>2</v>
-      </c>
-      <c r="B38" t="n">
-        <v>11</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> labor</t>
-        </is>
-      </c>
-      <c r="D38" s="3" t="n">
-        <v>754646</v>
-      </c>
-      <c r="E38" s="3" t="n">
-        <v>685576</v>
-      </c>
-      <c r="F38" s="3" t="n">
-        <v>625457</v>
-      </c>
+      <c r="D38" s="3" t="n"/>
+      <c r="E38" s="3" t="n"/>
+      <c r="F38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>2</v>
-      </c>
-      <c r="B39" t="n">
-        <v>12</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> occupancy</t>
-        </is>
-      </c>
-      <c r="D39" s="3" t="n">
-        <v>169998</v>
-      </c>
-      <c r="E39" s="3" t="n">
-        <v>159794</v>
-      </c>
-      <c r="F39" s="3" t="n">
-        <v>148816</v>
-      </c>
+      <c r="D39" s="3" t="n"/>
+      <c r="E39" s="3" t="n"/>
+      <c r="F39" s="3" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>2</v>
-      </c>
-      <c r="B40" t="n">
-        <v>13</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other operating expenses</t>
-        </is>
-      </c>
-      <c r="D40" s="3" t="n">
-        <v>334635</v>
-      </c>
-      <c r="E40" s="3" t="n">
-        <v>314879</v>
-      </c>
-      <c r="F40" s="3" t="n">
-        <v>295539</v>
-      </c>
+      <c r="D40" s="3" t="n"/>
+      <c r="E40" s="3" t="n"/>
+      <c r="F40" s="3" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>2</v>
-      </c>
-      <c r="B41" t="n">
-        <v>14</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total bakery-cafe expenses</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="n">
-        <v>1974781</v>
-      </c>
-      <c r="E41" s="3" t="n">
-        <v>1830109</v>
-      </c>
-      <c r="F41" s="3" t="n">
-        <v>1695434</v>
-      </c>
+      <c r="D41" s="3" t="n"/>
+      <c r="E41" s="3" t="n"/>
+      <c r="F41" s="3" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>2</v>
-      </c>
-      <c r="B42" t="n">
-        <v>15</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> fresh dough and other product cost of sales to franchisees</t>
-        </is>
-      </c>
-      <c r="D42" s="3" t="n">
-        <v>160706</v>
-      </c>
-      <c r="E42" s="3" t="n">
-        <v>152267</v>
-      </c>
-      <c r="F42" s="3" t="n">
-        <v>142160</v>
-      </c>
+      <c r="D42" s="3" t="n"/>
+      <c r="E42" s="3" t="n"/>
+      <c r="F42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>2</v>
-      </c>
-      <c r="B43" t="n">
-        <v>16</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
-        </is>
-      </c>
-      <c r="D43" s="3" t="n">
-        <v>135398</v>
-      </c>
-      <c r="E43" s="3" t="n">
-        <v>124109</v>
-      </c>
-      <c r="F43" s="3" t="n">
-        <v>106523</v>
-      </c>
+      <c r="D43" s="3" t="n"/>
+      <c r="E43" s="3" t="n"/>
+      <c r="F43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>2</v>
-      </c>
-      <c r="B44" t="n">
-        <v>17</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> general and administrative expenses</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="n">
-        <v>142904</v>
-      </c>
-      <c r="E44" s="3" t="n">
-        <v>138060</v>
-      </c>
-      <c r="F44" s="3" t="n">
-        <v>123335</v>
-      </c>
+      <c r="D44" s="3" t="n"/>
+      <c r="E44" s="3" t="n"/>
+      <c r="F44" s="3" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>2</v>
-      </c>
-      <c r="B45" t="n">
-        <v>18</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> pre-opening expenses</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="n">
-        <v>9089</v>
-      </c>
-      <c r="E45" s="3" t="n">
-        <v>8707</v>
-      </c>
-      <c r="F45" s="3" t="n">
-        <v>7794</v>
-      </c>
+      <c r="D45" s="3" t="n"/>
+      <c r="E45" s="3" t="n"/>
+      <c r="F45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>2</v>
-      </c>
-      <c r="B46" t="n">
-        <v>19</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> refranchising loss</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="n">
-        <v>17108</v>
-      </c>
+      <c r="D46" s="3" t="n"/>
       <c r="E46" s="3" t="n"/>
       <c r="F46" s="3" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>2</v>
-      </c>
-      <c r="B47" t="n">
-        <v>20</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total costs and expenses</t>
-        </is>
-      </c>
-      <c r="D47" s="3" t="n">
-        <v>2439986</v>
-      </c>
-      <c r="E47" s="3" t="n">
-        <v>2253252</v>
-      </c>
-      <c r="F47" s="3" t="n">
-        <v>2075246</v>
-      </c>
+      <c r="D47" s="3" t="n"/>
+      <c r="E47" s="3" t="n"/>
+      <c r="F47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>2</v>
-      </c>
-      <c r="B48" t="n">
-        <v>21</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> operating profit</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="n">
-        <v>241594</v>
-      </c>
-      <c r="E48" s="3" t="n">
-        <v>275943</v>
-      </c>
-      <c r="F48" s="3" t="n">
-        <v>309756</v>
-      </c>
+      <c r="D48" s="3" t="n"/>
+      <c r="E48" s="3" t="n"/>
+      <c r="F48" s="3" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>2</v>
-      </c>
-      <c r="B49" t="n">
-        <v>22</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> interest</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="n">
-        <v>3830</v>
-      </c>
-      <c r="E49" s="3" t="n">
-        <v>1824</v>
-      </c>
-      <c r="F49" s="3" t="n">
-        <v>1053</v>
-      </c>
+      <c r="D49" s="3" t="n"/>
+      <c r="E49" s="3" t="n"/>
+      <c r="F49" s="3" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>2</v>
-      </c>
-      <c r="B50" t="n">
-        <v>24</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other (income) expense net</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="n">
-        <v>1192</v>
-      </c>
-      <c r="E50" s="3" t="n">
-        <v>-3175</v>
-      </c>
-      <c r="F50" s="3" t="n">
-        <v>-4017</v>
-      </c>
+      <c r="D50" s="3" t="n"/>
+      <c r="E50" s="3" t="n"/>
+      <c r="F50" s="3" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>2</v>
-      </c>
-      <c r="B51" t="n">
-        <v>25</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> income before income taxes</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="n">
-        <v>236572</v>
-      </c>
-      <c r="E51" s="3" t="n">
-        <v>277294</v>
-      </c>
-      <c r="F51" s="3" t="n">
-        <v>312720</v>
-      </c>
+      <c r="D51" s="3" t="n"/>
+      <c r="E51" s="3" t="n"/>
+      <c r="F51" s="3" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>2</v>
-      </c>
-      <c r="B52" t="n">
-        <v>26</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> income taxes</t>
-        </is>
-      </c>
-      <c r="D52" s="3" t="n">
-        <v>87247</v>
-      </c>
-      <c r="E52" s="3" t="n">
-        <v>98001</v>
-      </c>
-      <c r="F52" s="3" t="n">
-        <v>116551</v>
-      </c>
+      <c r="D52" s="3" t="n"/>
+      <c r="E52" s="3" t="n"/>
+      <c r="F52" s="3" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>2</v>
-      </c>
-      <c r="B53" t="n">
-        <v>27</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="n">
-        <v>149325</v>
-      </c>
-      <c r="E53" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F53" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D53" s="3" t="n"/>
+      <c r="E53" s="3" t="n"/>
+      <c r="F53" s="3" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>2</v>
-      </c>
-      <c r="B54" t="n">
-        <v>28</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> less: net loss attributable to noncontrolling interest</t>
-        </is>
-      </c>
-      <c r="D54" s="3" t="n">
-        <v>-17</v>
-      </c>
+      <c r="D54" s="3" t="n"/>
       <c r="E54" s="3" t="n"/>
       <c r="F54" s="3" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>2</v>
-      </c>
-      <c r="B55" t="n">
-        <v>29</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income attributable to panera bread company</t>
-        </is>
-      </c>
-      <c r="D55" s="3" t="n">
-        <v>149342</v>
-      </c>
-      <c r="E55" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F55" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D55" s="3" t="n"/>
+      <c r="E55" s="3" t="n"/>
+      <c r="F55" s="3" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>2</v>
-      </c>
-      <c r="B56" t="n">
-        <v>32</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> basic</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="n">
-        <v>5.81</v>
-      </c>
-      <c r="E56" s="3" t="n">
-        <v>6.67</v>
-      </c>
-      <c r="F56" s="3" t="n">
-        <v>6.85</v>
-      </c>
+      <c r="D56" s="3" t="n"/>
+      <c r="E56" s="3" t="n"/>
+      <c r="F56" s="3" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>2</v>
-      </c>
-      <c r="B57" t="n">
-        <v>33</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> diluted</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="n">
-        <v>5.79</v>
-      </c>
-      <c r="E57" s="3" t="n">
-        <v>6.64</v>
-      </c>
-      <c r="F57" s="3" t="n">
-        <v>6.81</v>
-      </c>
+      <c r="D57" s="3" t="n"/>
+      <c r="E57" s="3" t="n"/>
+      <c r="F57" s="3" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>2</v>
-      </c>
-      <c r="B58" t="n">
-        <v>36</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> basic</t>
-        </is>
-      </c>
-      <c r="D58" s="3" t="n">
-        <v>25685</v>
-      </c>
-      <c r="E58" s="3" t="n">
-        <v>26881</v>
-      </c>
-      <c r="F58" s="3" t="n">
-        <v>28629</v>
-      </c>
+      <c r="D58" s="3" t="n"/>
+      <c r="E58" s="3" t="n"/>
+      <c r="F58" s="3" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>2</v>
-      </c>
-      <c r="B59" t="n">
-        <v>37</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> viluted 1he accompanying notes are an integral part of the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="n">
-        <v>25788</v>
-      </c>
-      <c r="E59" s="3" t="n">
-        <v>26999</v>
-      </c>
-      <c r="F59" s="3" t="n">
-        <v>28794</v>
-      </c>
+      <c r="D59" s="3" t="n"/>
+      <c r="E59" s="3" t="n"/>
+      <c r="F59" s="3" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>3</v>
-      </c>
-      <c r="B60" t="n">
-        <v>2</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income</t>
-        </is>
-      </c>
-      <c r="D60" s="3" t="n">
-        <v>149325</v>
-      </c>
-      <c r="E60" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F60" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D60" s="3" t="n"/>
+      <c r="E60" s="3" t="n"/>
+      <c r="F60" s="3" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>3</v>
-      </c>
-      <c r="B61" t="n">
-        <v>4</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="n">
-        <v>135398</v>
-      </c>
-      <c r="E61" s="3" t="n">
-        <v>124109</v>
-      </c>
-      <c r="F61" s="3" t="n">
-        <v>106523</v>
-      </c>
+      <c r="D61" s="3" t="n"/>
+      <c r="E61" s="3" t="n"/>
+      <c r="F61" s="3" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>3</v>
-      </c>
-      <c r="B62" t="n">
-        <v>5</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> stock-based compensation expense</t>
-        </is>
-      </c>
-      <c r="D62" s="3" t="n">
-        <v>15086</v>
-      </c>
-      <c r="E62" s="3" t="n">
-        <v>10077</v>
-      </c>
-      <c r="F62" s="3" t="n">
-        <v>10703</v>
-      </c>
+      <c r="D62" s="3" t="n"/>
+      <c r="E62" s="3" t="n"/>
+      <c r="F62" s="3" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>3</v>
-      </c>
-      <c r="B63" t="n">
-        <v>6</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
-      </c>
-      <c r="D63" s="3" t="n">
-        <v>-2057</v>
-      </c>
-      <c r="E63" s="3" t="n">
-        <v>-3089</v>
-      </c>
-      <c r="F63" s="3" t="n">
-        <v>-8100</v>
-      </c>
+      <c r="D63" s="3" t="n"/>
+      <c r="E63" s="3" t="n"/>
+      <c r="F63" s="3" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>3</v>
-      </c>
-      <c r="B64" t="n">
-        <v>7</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred income taxes</t>
-        </is>
-      </c>
-      <c r="D64" s="3" t="n">
-        <v>-10991</v>
-      </c>
-      <c r="E64" s="3" t="n">
-        <v>10459</v>
-      </c>
-      <c r="F64" s="3" t="n">
-        <v>10356</v>
-      </c>
+      <c r="D64" s="3" t="n"/>
+      <c r="E64" s="3" t="n"/>
+      <c r="F64" s="3" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>3</v>
-      </c>
-      <c r="B65" t="n">
-        <v>8</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> refranchising loss</t>
-        </is>
-      </c>
-      <c r="D65" s="3" t="n">
-        <v>12942</v>
-      </c>
+      <c r="D65" s="3" t="n"/>
       <c r="E65" s="3" t="n"/>
       <c r="F65" s="3" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>3</v>
-      </c>
-      <c r="B66" t="n">
-        <v>9</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other</t>
-        </is>
-      </c>
-      <c r="D66" s="3" t="n">
-        <v>3505</v>
-      </c>
-      <c r="E66" s="3" t="n">
-        <v>4617</v>
-      </c>
-      <c r="F66" s="3" t="n">
-        <v>6353</v>
-      </c>
+      <c r="D66" s="3" t="n"/>
+      <c r="E66" s="3" t="n"/>
+      <c r="F66" s="3" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>3</v>
-      </c>
-      <c r="B67" t="n">
-        <v>12</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> trade and other accounts receivable net</t>
-        </is>
-      </c>
-      <c r="D67" s="3" t="n">
-        <v>-3605</v>
-      </c>
-      <c r="E67" s="3" t="n">
-        <v>-22139</v>
-      </c>
-      <c r="F67" s="3" t="n">
-        <v>3021</v>
-      </c>
+      <c r="D67" s="3" t="n"/>
+      <c r="E67" s="3" t="n"/>
+      <c r="F67" s="3" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>3</v>
-      </c>
-      <c r="B68" t="n">
-        <v>13</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> inventories</t>
-        </is>
-      </c>
-      <c r="D68" s="3" t="n">
-        <v>-1698</v>
-      </c>
-      <c r="E68" s="3" t="n">
-        <v>-895</v>
-      </c>
-      <c r="F68" s="3" t="n">
-        <v>-2186</v>
-      </c>
+      <c r="D68" s="3" t="n"/>
+      <c r="E68" s="3" t="n"/>
+      <c r="F68" s="3" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>3</v>
-      </c>
-      <c r="B69" t="n">
-        <v>14</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> prepaid expenses and other</t>
-        </is>
-      </c>
-      <c r="D69" s="3" t="n">
-        <v>-7191</v>
-      </c>
-      <c r="E69" s="3" t="n">
-        <v>-8524</v>
-      </c>
-      <c r="F69" s="3" t="n">
-        <v>-841</v>
-      </c>
+      <c r="D69" s="3" t="n"/>
+      <c r="E69" s="3" t="n"/>
+      <c r="F69" s="3" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>3</v>
-      </c>
-      <c r="B70" t="n">
-        <v>15</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deposits and other</t>
-        </is>
-      </c>
-      <c r="D70" s="3" t="n">
-        <v>-455</v>
-      </c>
-      <c r="E70" s="3" t="n">
-        <v>239</v>
-      </c>
-      <c r="F70" s="3" t="n">
-        <v>1449</v>
-      </c>
+      <c r="D70" s="3" t="n"/>
+      <c r="E70" s="3" t="n"/>
+      <c r="F70" s="3" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>3</v>
-      </c>
-      <c r="B71" t="n">
-        <v>16</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accounts payable</t>
-        </is>
-      </c>
-      <c r="D71" s="3" t="n">
-        <v>-183</v>
-      </c>
-      <c r="E71" s="3" t="n">
-        <v>1978</v>
-      </c>
-      <c r="F71" s="3" t="n">
-        <v>8162</v>
-      </c>
+      <c r="D71" s="3" t="n"/>
+      <c r="E71" s="3" t="n"/>
+      <c r="F71" s="3" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>3</v>
-      </c>
-      <c r="B72" t="n">
-        <v>17</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accrued expenses</t>
-        </is>
-      </c>
-      <c r="D72" s="3" t="n">
-        <v>31169</v>
-      </c>
-      <c r="E72" s="3" t="n">
-        <v>35288</v>
-      </c>
-      <c r="F72" s="3" t="n">
-        <v>13372</v>
-      </c>
+      <c r="D72" s="3" t="n"/>
+      <c r="E72" s="3" t="n"/>
+      <c r="F72" s="3" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>3</v>
-      </c>
-      <c r="B73" t="n">
-        <v>18</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred rent</t>
-        </is>
-      </c>
-      <c r="D73" s="3" t="n">
-        <v>3751</v>
-      </c>
-      <c r="E73" s="3" t="n">
-        <v>1067</v>
-      </c>
-      <c r="F73" s="3" t="n">
-        <v>5868</v>
-      </c>
+      <c r="D73" s="3" t="n"/>
+      <c r="E73" s="3" t="n"/>
+      <c r="F73" s="3" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>3</v>
-      </c>
-      <c r="B74" t="n">
-        <v>19</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
-        </is>
-      </c>
-      <c r="D74" s="3" t="n">
-        <v>-6951</v>
-      </c>
-      <c r="E74" s="3" t="n">
-        <v>2599</v>
-      </c>
-      <c r="F74" s="3" t="n">
-        <v>-2432</v>
-      </c>
+      <c r="D74" s="3" t="n"/>
+      <c r="E74" s="3" t="n"/>
+      <c r="F74" s="3" t="n"/>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>3</v>
-      </c>
-      <c r="B75" t="n">
-        <v>20</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash provided by operating activities</t>
-        </is>
-      </c>
-      <c r="D75" s="3" t="n">
-        <v>318045</v>
-      </c>
-      <c r="E75" s="3" t="n">
-        <v>335079</v>
-      </c>
-      <c r="F75" s="3" t="n">
-        <v>348417</v>
-      </c>
+      <c r="D75" s="3" t="n"/>
+      <c r="E75" s="3" t="n"/>
+      <c r="F75" s="3" t="n"/>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>3</v>
-      </c>
-      <c r="B76" t="n">
-        <v>22</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> additions to property and equipment</t>
-        </is>
-      </c>
-      <c r="D76" s="3" t="n">
-        <v>-223932</v>
-      </c>
-      <c r="E76" s="3" t="n">
-        <v>-224217</v>
-      </c>
-      <c r="F76" s="3" t="n">
-        <v>-192010</v>
-      </c>
+      <c r="D76" s="3" t="n"/>
+      <c r="E76" s="3" t="n"/>
+      <c r="F76" s="3" t="n"/>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>3</v>
-      </c>
-      <c r="B77" t="n">
-        <v>23</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> acquisitions net of cash acquired</t>
-        </is>
-      </c>
       <c r="D77" s="3" t="n"/>
       <c r="E77" s="3" t="n"/>
-      <c r="F77" s="3" t="n">
-        <v>-2446</v>
-      </c>
+      <c r="F77" s="3" t="n"/>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>3</v>
-      </c>
-      <c r="B78" t="n">
-        <v>24</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> purchase of investments</t>
-        </is>
-      </c>
       <c r="D78" s="3" t="n"/>
       <c r="E78" s="3" t="n"/>
-      <c r="F78" s="3" t="n">
-        <v>-97919</v>
-      </c>
+      <c r="F78" s="3" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" t="n">
-        <v>3</v>
-      </c>
-      <c r="B79" t="n">
-        <v>25</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale of investments</t>
-        </is>
-      </c>
       <c r="D79" s="3" t="n"/>
       <c r="E79" s="3" t="n"/>
-      <c r="F79" s="3" t="n">
-        <v>97936</v>
-      </c>
+      <c r="F79" s="3" t="n"/>
     </row>
     <row r="80">
-      <c r="A80" t="n">
-        <v>3</v>
-      </c>
-      <c r="B80" t="n">
-        <v>26</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from refranchising</t>
-        </is>
-      </c>
-      <c r="D80" s="3" t="n">
-        <v>46869</v>
-      </c>
+      <c r="D80" s="3" t="n"/>
       <c r="E80" s="3" t="n"/>
       <c r="F80" s="3" t="n"/>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>3</v>
-      </c>
-      <c r="B81" t="n">
-        <v>27</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale of property and equipment</t>
-        </is>
-      </c>
-      <c r="D81" s="3" t="n">
-        <v>1553</v>
-      </c>
+      <c r="D81" s="3" t="n"/>
       <c r="E81" s="3" t="n"/>
       <c r="F81" s="3" t="n"/>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>3</v>
-      </c>
-      <c r="B82" t="n">
-        <v>28</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale-leaseback transactions</t>
-        </is>
-      </c>
-      <c r="D82" s="3" t="n">
-        <v>10095</v>
-      </c>
-      <c r="E82" s="3" t="n">
-        <v>12900</v>
-      </c>
-      <c r="F82" s="3" t="n">
-        <v>6132</v>
-      </c>
+      <c r="D82" s="3" t="n"/>
+      <c r="E82" s="3" t="n"/>
+      <c r="F82" s="3" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>3</v>
-      </c>
-      <c r="B83" t="n">
-        <v>29</v>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash used in investing activities</t>
-        </is>
-      </c>
-      <c r="D83" s="3" t="n">
-        <v>-165415</v>
-      </c>
-      <c r="E83" s="3" t="n">
-        <v>-211317</v>
-      </c>
-      <c r="F83" s="3" t="n">
-        <v>-188307</v>
-      </c>
+      <c r="D83" s="3" t="n"/>
+      <c r="E83" s="3" t="n"/>
+      <c r="F83" s="3" t="n"/>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>3</v>
-      </c>
-      <c r="B84" t="n">
-        <v>31</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from issuance of long-term debt</t>
-        </is>
-      </c>
-      <c r="D84" s="3" t="n">
-        <v>299070</v>
-      </c>
-      <c r="E84" s="3" t="n">
-        <v>100000</v>
-      </c>
+      <c r="D84" s="3" t="n"/>
+      <c r="E84" s="3" t="n"/>
       <c r="F84" s="3" t="n"/>
     </row>
     <row r="85">
-      <c r="A85" t="n">
-        <v>3</v>
-      </c>
-      <c r="B85" t="n">
-        <v>32</v>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> repayments of long-term debt</t>
-        </is>
-      </c>
-      <c r="D85" s="3" t="n">
-        <v>-6301</v>
-      </c>
+      <c r="D85" s="3" t="n"/>
       <c r="E85" s="3" t="n"/>
       <c r="F85" s="3" t="n"/>
     </row>
     <row r="86">
-      <c r="A86" t="n">
-        <v>3</v>
-      </c>
-      <c r="B86" t="n">
-        <v>33</v>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> capitalized debt issuance costs</t>
-        </is>
-      </c>
-      <c r="D86" s="3" t="n">
-        <v>-363</v>
-      </c>
-      <c r="E86" s="3" t="n">
-        <v>-193</v>
-      </c>
+      <c r="D86" s="3" t="n"/>
+      <c r="E86" s="3" t="n"/>
       <c r="F86" s="3" t="n"/>
     </row>
     <row r="87">
-      <c r="A87" t="n">
-        <v>3</v>
-      </c>
-      <c r="B87" t="n">
-        <v>34</v>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> payment of deferred acquisition holdback</t>
-        </is>
-      </c>
       <c r="D87" s="3" t="n"/>
-      <c r="E87" s="3" t="n">
-        <v>-270</v>
-      </c>
-      <c r="F87" s="3" t="n">
-        <v>-4112</v>
-      </c>
+      <c r="E87" s="3" t="n"/>
+      <c r="F87" s="3" t="n"/>
     </row>
     <row r="88">
-      <c r="A88" t="n">
-        <v>3</v>
-      </c>
-      <c r="B88" t="n">
-        <v>35</v>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> repurchase of common stock</t>
-        </is>
-      </c>
-      <c r="D88" s="3" t="n">
-        <v>-405513</v>
-      </c>
-      <c r="E88" s="3" t="n">
-        <v>-159503</v>
-      </c>
-      <c r="F88" s="3" t="n">
-        <v>-339409</v>
-      </c>
+      <c r="D88" s="3" t="n"/>
+      <c r="E88" s="3" t="n"/>
+      <c r="F88" s="3" t="n"/>
     </row>
     <row r="89">
-      <c r="A89" t="n">
-        <v>3</v>
-      </c>
-      <c r="B89" t="n">
-        <v>36</v>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> exercise of employee stock options</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="n">
-        <v>288</v>
-      </c>
-      <c r="E89" s="3" t="n">
-        <v>1116</v>
-      </c>
-      <c r="F89" s="3" t="n">
-        <v>573</v>
-      </c>
+      <c r="D89" s="3" t="n"/>
+      <c r="E89" s="3" t="n"/>
+      <c r="F89" s="3" t="n"/>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>3</v>
-      </c>
-      <c r="B90" t="n">
-        <v>37</v>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
-      </c>
-      <c r="D90" s="3" t="n">
-        <v>2057</v>
-      </c>
-      <c r="E90" s="3" t="n">
-        <v>3089</v>
-      </c>
-      <c r="F90" s="3" t="n">
-        <v>8100</v>
-      </c>
+      <c r="D90" s="3" t="n"/>
+      <c r="E90" s="3" t="n"/>
+      <c r="F90" s="3" t="n"/>
     </row>
     <row r="91">
-      <c r="A91" t="n">
-        <v>3</v>
-      </c>
-      <c r="B91" t="n">
-        <v>38</v>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from issuance of common stock under employee benefit plans</t>
-        </is>
-      </c>
-      <c r="D91" s="3" t="n">
-        <v>3525</v>
-      </c>
-      <c r="E91" s="3" t="n">
-        <v>3247</v>
-      </c>
-      <c r="F91" s="3" t="n">
-        <v>2842</v>
-      </c>
+      <c r="D91" s="3" t="n"/>
+      <c r="E91" s="3" t="n"/>
+      <c r="F91" s="3" t="n"/>
     </row>
     <row r="92">
-      <c r="A92" t="n">
-        <v>3</v>
-      </c>
-      <c r="B92" t="n">
-        <v>39</v>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash used in financing activities</t>
-        </is>
-      </c>
-      <c r="D92" s="3" t="n">
-        <v>-107237</v>
-      </c>
-      <c r="E92" s="3" t="n">
-        <v>-52514</v>
-      </c>
-      <c r="F92" s="3" t="n">
-        <v>-332006</v>
-      </c>
+      <c r="D92" s="3" t="n"/>
+      <c r="E92" s="3" t="n"/>
+      <c r="F92" s="3" t="n"/>
     </row>
     <row r="93">
-      <c r="A93" t="n">
-        <v>3</v>
-      </c>
-      <c r="B93" t="n">
-        <v>40</v>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net increase (decrease) in cash and cash equivalents</t>
-        </is>
-      </c>
-      <c r="D93" s="3" t="n">
-        <v>45393</v>
-      </c>
-      <c r="E93" s="3" t="n">
-        <v>71248</v>
-      </c>
-      <c r="F93" s="3" t="n">
-        <v>-171896</v>
-      </c>
+      <c r="D93" s="3" t="n"/>
+      <c r="E93" s="3" t="n"/>
+      <c r="F93" s="3" t="n"/>
     </row>
     <row r="94">
-      <c r="A94" t="n">
-        <v>3</v>
-      </c>
-      <c r="B94" t="n">
-        <v>41</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cash and cash equivalents at beginning of period</t>
-        </is>
-      </c>
-      <c r="D94" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="E94" s="3" t="n">
-        <v>125245</v>
-      </c>
-      <c r="F94" s="3" t="n">
-        <v>297141</v>
-      </c>
+      <c r="D94" s="3" t="n"/>
+      <c r="E94" s="3" t="n"/>
+      <c r="F94" s="3" t="n"/>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>3</v>
-      </c>
-      <c r="B95" t="n">
-        <v>42</v>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cash and cash equivalents at end of 1he period accompanying notes are an integral part of the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D95" s="3" t="n">
-        <v>241886</v>
-      </c>
-      <c r="E95" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="F95" s="3" t="n">
-        <v>125245</v>
-      </c>
+      <c r="D95" s="3" t="n"/>
+      <c r="E95" s="3" t="n"/>
+      <c r="F95" s="3" t="n"/>
     </row>
     <row r="96">
       <c r="D96" s="3" t="n"/>

</xml_diff>

<commit_message>
brought together detect columns functions
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="3255" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="3255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,8 +16,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="164"/>
+    <numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="165"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -68,24 +68,24 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="44"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="4" name="Currency" xfId="1"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -460,19 +460,19 @@
   </sheetPr>
   <dimension ref="A1:M4269"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="110">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col width="11.3125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="10.1875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="50.9375" customWidth="1" min="3" max="3"/>
-    <col width="20.4375" bestFit="1" customWidth="1" min="4" max="9"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="11.3125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="10.1875"/>
+    <col customWidth="1" max="3" min="3" width="50.9375"/>
+    <col bestFit="1" customWidth="1" max="9" min="4" width="20.4375"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customFormat="1" customHeight="1" s="2">
+    <row customFormat="1" customHeight="1" ht="18" r="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>page_num</t>
@@ -490,12 +490,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>december 31. 2020</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>december 31. 2020:1</t>
         </is>
       </c>
       <c r="F1" s="1" t="n"/>
@@ -516,10 +516,10 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>19384</v>
+        <v>384344</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>6268</v>
+        <v>27872</v>
       </c>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
@@ -531,18 +531,18 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts receivable net</t>
+          <t xml:space="preserve"> and respectively</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>1886</v>
+        <v>176617</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>1324</v>
+        <v>148855</v>
       </c>
       <c r="F3" s="3" t="n"/>
       <c r="G3" s="3" t="n"/>
@@ -554,18 +554,18 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> inventory</t>
+          <t xml:space="preserve"> prepaid and other</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>4101</v>
+        <v>63224</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>3552</v>
+        <v>52161</v>
       </c>
       <c r="F4" s="3" t="n"/>
       <c r="G4" s="3" t="n"/>
@@ -577,18 +577,18 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> expenses current assets</t>
+          <t xml:space="preserve"> total current assets</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>1346</v>
+        <v>624185</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>959</v>
+        <v>228888</v>
       </c>
       <c r="F5" s="3" t="n"/>
       <c r="G5" s="3" t="n"/>
@@ -600,18 +600,18 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current assets</t>
+          <t xml:space="preserve"> fixed assets net</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>26717</v>
+        <v>628757</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>12103</v>
+        <v>636153</v>
       </c>
       <c r="F6" s="3" t="n"/>
       <c r="G6" s="3" t="n"/>
@@ -623,18 +623,18 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> operating lease vehicles net</t>
+          <t xml:space="preserve"> goodwill</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>3091</v>
+        <v>1431967</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>2447</v>
+        <v>1412873</v>
       </c>
       <c r="F7" s="3" t="n"/>
       <c r="G7" s="3" t="n"/>
@@ -650,14 +650,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> energy systems net</t>
+          <t xml:space="preserve"> other intangible asse*s net</t>
         </is>
       </c>
       <c r="D8" s="3" t="n">
-        <v>5979</v>
+        <v>274620</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>6138</v>
+        <v>304673</v>
       </c>
       <c r="F8" s="3" t="n"/>
       <c r="G8" s="3" t="n"/>
@@ -673,14 +673,14 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> property plant and equipment net</t>
+          <t xml:space="preserve"> operating lease right-of-use assets</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>12747</v>
+        <v>717821</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>10396</v>
+        <v>700956</v>
       </c>
       <c r="F9" s="3" t="n"/>
       <c r="G9" s="3" t="n"/>
@@ -696,14 +696,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> operating lease right-of-use assets</t>
+          <t xml:space="preserve"> other assets</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
-        <v>1558</v>
+        <v>49298</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>1218</v>
+        <v>46877</v>
       </c>
       <c r="F10" s="3" t="n"/>
       <c r="G10" s="3" t="n"/>
@@ -719,14 +719,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> intangible assets net</t>
+          <t xml:space="preserve"> total assets</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>313</v>
+        <v>3726648</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>339</v>
+        <v>3330420</v>
       </c>
       <c r="F11" s="3" t="n"/>
       <c r="G11" s="3" t="n"/>
@@ -738,18 +738,18 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> goodwill</t>
+          <t xml:space="preserve"> current portion of long-term debt</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>207</v>
+        <v>10750</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>198</v>
+        <v>10750</v>
       </c>
       <c r="F12" s="3" t="n"/>
       <c r="G12" s="3" t="n"/>
@@ -761,18 +761,18 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other non-current assets</t>
+          <t xml:space="preserve"> accounts payable and accrued expenses</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>1536</v>
+        <v>194551</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>1470</v>
+        <v>167059</v>
       </c>
       <c r="F13" s="3" t="n"/>
       <c r="G13" s="3" t="n"/>
@@ -784,18 +784,18 @@
         <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total assets</t>
+          <t xml:space="preserve"> current portion of operating lease liabilities</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>52148</v>
+        <v>87181</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>34309</v>
+        <v>83123</v>
       </c>
       <c r="F14" s="3" t="n"/>
       <c r="G14" s="3" t="n"/>
@@ -811,14 +811,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable</t>
+          <t xml:space="preserve"> deferred</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>6051</v>
+        <v>197939</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>3771</v>
+        <v>191117</v>
       </c>
       <c r="F15" s="3" t="n"/>
       <c r="G15" s="3" t="n"/>
@@ -830,18 +830,18 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accrued liabilities and other</t>
+          <t xml:space="preserve"> other current liabilities</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>3855</v>
+        <v>40393</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>3222</v>
+        <v>31241</v>
       </c>
       <c r="F16" s="3" t="n"/>
       <c r="G16" s="3" t="n"/>
@@ -853,18 +853,18 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred</t>
+          <t xml:space="preserve"> total current liabilities</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>1458</v>
+        <v>530814</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>1163</v>
+        <v>483290</v>
       </c>
       <c r="F17" s="3" t="n"/>
       <c r="G17" s="3" t="n"/>
@@ -880,14 +880,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> customer deposits</t>
+          <t xml:space="preserve"> long-iciu debt net</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>752</v>
+        <v>1020137</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>726</v>
+        <v>1028049</v>
       </c>
       <c r="F18" s="3" t="n"/>
       <c r="G18" s="3" t="n"/>
@@ -903,14 +903,14 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> current portion of debt and finance leases</t>
+          <t xml:space="preserve"> operating lease liabilities</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>2132</v>
+        <v>729754</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>1785</v>
+        <v>685910</v>
       </c>
       <c r="F19" s="3" t="n"/>
       <c r="G19" s="3" t="n"/>
@@ -926,14 +926,14 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current liabilities</t>
+          <t xml:space="preserve"> other long-term liabilities</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
-        <v>14248</v>
+        <v>105980</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>10667</v>
+        <v>92865</v>
       </c>
       <c r="F20" s="3" t="n"/>
       <c r="G20" s="3" t="n"/>
@@ -949,14 +949,14 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> debt and finance leases net of current portion</t>
+          <t xml:space="preserve"> deferred</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>9556</v>
+        <v>10215</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>11634</v>
+        <v>10098</v>
       </c>
       <c r="F21" s="3" t="n"/>
       <c r="G21" s="3" t="n"/>
@@ -968,18 +968,18 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred of portion</t>
+          <t xml:space="preserve"> deferred income taxes</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
-        <v>1284</v>
+        <v>45951</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>1207</v>
+        <v>58940</v>
       </c>
       <c r="F22" s="3" t="n"/>
       <c r="G22" s="3" t="n"/>
@@ -995,14 +995,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
+          <t xml:space="preserve"> total liabilities</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>3330</v>
+        <v>2442851</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>2691</v>
+        <v>2359152</v>
       </c>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
@@ -1014,18 +1014,18 @@
         <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total liabilities</t>
+          <t xml:space="preserve"> issued and outstanding at december and respectively</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
-        <v>28418</v>
+        <v>60</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>26199</v>
+        <v>58</v>
       </c>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
@@ -1037,18 +1037,18 @@
         <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> redeemable noncontrolling interests in subsidiaries</t>
+          <t xml:space="preserve"> additional paid-in capital</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>604</v>
+        <v>910304</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>643</v>
+        <v>648031</v>
       </c>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
@@ -1060,17 +1060,19 @@
         <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> convertible senior notes (note 12)</t>
+          <t xml:space="preserve"> accumulated other comprehensive loss</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
-        <v>51</v>
-      </c>
-      <c r="E26" s="3" t="n"/>
+        <v>-27069</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>-50331</v>
+      </c>
       <c r="F26" s="3" t="n"/>
       <c r="G26" s="3" t="n"/>
       <c r="H26" s="3" t="n"/>
@@ -1081,18 +1083,18 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> respectively</t>
+          <t xml:space="preserve"> retained earnings</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>1</v>
+        <v>400502</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>1</v>
+        <v>373510</v>
       </c>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
@@ -1104,18 +1106,18 @@
         <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> additional paid-in capital</t>
+          <t xml:space="preserve"> total stockholders’ equity</t>
         </is>
       </c>
       <c r="D28" s="3" t="n">
-        <v>27260</v>
+        <v>1283797</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>12736</v>
+        <v>971268</v>
       </c>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
@@ -1127,18 +1129,18 @@
         <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accumulated other comprehensive income (loss)</t>
+          <t xml:space="preserve"> total liabilities and stockholders’ equity see accompanying notes to consolidated financial statements.</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>363</v>
+        <v>3726648</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-36</v>
+        <v>3330420</v>
       </c>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
@@ -1146,92 +1148,32 @@
       <c r="I29" s="3" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" t="n">
-        <v>44</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accumulated deficit</t>
-        </is>
-      </c>
-      <c r="D30" s="3" t="n">
-        <v>-5399</v>
-      </c>
-      <c r="E30" s="3" t="n">
-        <v>-6083</v>
-      </c>
+      <c r="D30" s="3" t="n"/>
+      <c r="E30" s="3" t="n"/>
       <c r="F30" s="3" t="n"/>
       <c r="G30" s="3" t="n"/>
       <c r="H30" s="3" t="n"/>
       <c r="I30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" t="n">
-        <v>45</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total stockholders’ equity</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="n">
-        <v>22225</v>
-      </c>
-      <c r="E31" s="3" t="n">
-        <v>6618</v>
-      </c>
+      <c r="D31" s="3" t="n"/>
+      <c r="E31" s="3" t="n"/>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="3" t="n"/>
       <c r="I31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" t="n">
-        <v>46</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> noncontrolling interests in subsidiaries</t>
-        </is>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>850</v>
-      </c>
-      <c r="E32" s="3" t="n">
-        <v>849</v>
-      </c>
+      <c r="D32" s="3" t="n"/>
+      <c r="E32" s="3" t="n"/>
       <c r="F32" s="3" t="n"/>
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="3" t="n"/>
       <c r="I32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>1</v>
-      </c>
-      <c r="B33" t="n">
-        <v>47</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total liabilities and equity</t>
-        </is>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>52148</v>
-      </c>
-      <c r="E33" s="3" t="n">
-        <v>34309</v>
-      </c>
+      <c r="D33" s="3" t="n"/>
+      <c r="E33" s="3" t="n"/>
       <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="3" t="n"/>
@@ -8631,7 +8573,7 @@
     <row r="4268"/>
     <row r="4269"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
still working on column logic, reduced to 554 lines of code from high of 840
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="3255"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="3255" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,8 +16,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="164"/>
-    <numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -68,24 +68,24 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="4" name="Currency" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -460,19 +460,19 @@
   </sheetPr>
   <dimension ref="A1:M4269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="110">
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="11.3125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="10.1875"/>
-    <col customWidth="1" max="3" min="3" width="50.9375"/>
-    <col bestFit="1" customWidth="1" max="9" min="4" width="20.4375"/>
+    <col width="11.3125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10.1875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="50.9375" customWidth="1" min="3" max="3"/>
+    <col width="20.4375" bestFit="1" customWidth="1" min="4" max="9"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="18" r="1" s="2">
+    <row r="1" ht="18" customFormat="1" customHeight="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>page_num</t>
@@ -490,15 +490,19 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>december 31. 2020</t>
+          <t>december 30. 2015</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>december 31. 2020:1</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="n"/>
+          <t>december 30. 2014</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
+      </c>
       <c r="G1" s="1" t="n"/>
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
@@ -516,10 +520,10 @@
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>384344</v>
+        <v>241886</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>27872</v>
+        <v>196493</v>
       </c>
       <c r="F2" s="3" t="n"/>
       <c r="G2" s="3" t="n"/>
@@ -531,18 +535,18 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> and respectively</t>
+          <t xml:space="preserve"> trade accounts receivable net</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>176617</v>
+        <v>38211</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>148855</v>
+        <v>36584</v>
       </c>
       <c r="F3" s="3" t="n"/>
       <c r="G3" s="3" t="n"/>
@@ -554,18 +558,18 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> prepaid and other</t>
+          <t xml:space="preserve"> other accounts receivable</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>63224</v>
+        <v>77575</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>52161</v>
+        <v>70069</v>
       </c>
       <c r="F4" s="3" t="n"/>
       <c r="G4" s="3" t="n"/>
@@ -577,18 +581,18 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current assets</t>
+          <t xml:space="preserve"> inventories</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>624185</v>
+        <v>22482</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>228888</v>
+        <v>22811</v>
       </c>
       <c r="F5" s="3" t="n"/>
       <c r="G5" s="3" t="n"/>
@@ -600,18 +604,18 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fixed assets net</t>
+          <t xml:space="preserve"> prepaid and other</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>628757</v>
+        <v>59457</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>636153</v>
+        <v>51588</v>
       </c>
       <c r="F6" s="3" t="n"/>
       <c r="G6" s="3" t="n"/>
@@ -623,18 +627,18 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> goodwill</t>
+          <t xml:space="preserve"> veferred income taxes</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1431967</v>
+        <v>34479</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>1412873</v>
+        <v>28621</v>
       </c>
       <c r="F7" s="3" t="n"/>
       <c r="G7" s="3" t="n"/>
@@ -646,19 +650,17 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other intangible asse*s net</t>
+          <t xml:space="preserve"> assets held for sale</t>
         </is>
       </c>
       <c r="D8" s="3" t="n">
-        <v>274620</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>304673</v>
-      </c>
+        <v>28699</v>
+      </c>
+      <c r="E8" s="3" t="n"/>
       <c r="F8" s="3" t="n"/>
       <c r="G8" s="3" t="n"/>
       <c r="H8" s="3" t="n"/>
@@ -669,18 +671,18 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> operating lease right-of-use assets</t>
+          <t xml:space="preserve"> total current assets</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>717821</v>
+        <v>502789</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>700956</v>
+        <v>406166</v>
       </c>
       <c r="F9" s="3" t="n"/>
       <c r="G9" s="3" t="n"/>
@@ -692,18 +694,18 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other assets</t>
+          <t xml:space="preserve"> property and equipment net</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
-        <v>49298</v>
+        <v>776248</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>46877</v>
+        <v>787294</v>
       </c>
       <c r="F10" s="3" t="n"/>
       <c r="G10" s="3" t="n"/>
@@ -719,14 +721,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total assets</t>
+          <t xml:space="preserve"> goodwill</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>3726648</v>
+        <v>121791</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>3330420</v>
+        <v>120778</v>
       </c>
       <c r="F11" s="3" t="n"/>
       <c r="G11" s="3" t="n"/>
@@ -738,18 +740,18 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> current portion of long-term debt</t>
+          <t xml:space="preserve"> other intangible assets net</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>10750</v>
+        <v>63877</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>10750</v>
+        <v>70940</v>
       </c>
       <c r="F12" s="3" t="n"/>
       <c r="G12" s="3" t="n"/>
@@ -761,18 +763,18 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable and accrued expenses</t>
+          <t xml:space="preserve"> deposits and other</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>194551</v>
+        <v>10613</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>167059</v>
+        <v>5508</v>
       </c>
       <c r="F13" s="3" t="n"/>
       <c r="G13" s="3" t="n"/>
@@ -784,18 +786,18 @@
         <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> current portion of operating lease liabilities</t>
+          <t xml:space="preserve"> total other assets</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>87181</v>
+        <v>196281</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>83123</v>
+        <v>197226</v>
       </c>
       <c r="F14" s="3" t="n"/>
       <c r="G14" s="3" t="n"/>
@@ -807,18 +809,18 @@
         <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred</t>
+          <t xml:space="preserve"> total assets</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>197939</v>
+        <v>1475318</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>191117</v>
+        <v>1390686</v>
       </c>
       <c r="F15" s="3" t="n"/>
       <c r="G15" s="3" t="n"/>
@@ -830,18 +832,18 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other current liabilities</t>
+          <t xml:space="preserve"> accounts payable</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>40393</v>
+        <v>19805</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>31241</v>
+        <v>19511</v>
       </c>
       <c r="F16" s="3" t="n"/>
       <c r="G16" s="3" t="n"/>
@@ -853,18 +855,18 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current liabilities</t>
+          <t xml:space="preserve"> accrued</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>530814</v>
+        <v>359464</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>483290</v>
+        <v>333201</v>
       </c>
       <c r="F17" s="3" t="n"/>
       <c r="G17" s="3" t="n"/>
@@ -880,15 +882,13 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> long-iciu debt net</t>
+          <t xml:space="preserve"> cunent portion of long-term debt</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>1020137</v>
-      </c>
-      <c r="E18" s="3" t="n">
-        <v>1028049</v>
-      </c>
+        <v>17229</v>
+      </c>
+      <c r="E18" s="3" t="n"/>
       <c r="F18" s="3" t="n"/>
       <c r="G18" s="3" t="n"/>
       <c r="H18" s="3" t="n"/>
@@ -903,15 +903,13 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> operating lease liabilities</t>
+          <t xml:space="preserve"> liabilities associated with assets held for sale</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>729754</v>
-      </c>
-      <c r="E19" s="3" t="n">
-        <v>685910</v>
-      </c>
+        <v>2945</v>
+      </c>
+      <c r="E19" s="3" t="n"/>
       <c r="F19" s="3" t="n"/>
       <c r="G19" s="3" t="n"/>
       <c r="H19" s="3" t="n"/>
@@ -926,14 +924,14 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
+          <t xml:space="preserve"> total current liabilities</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
-        <v>105980</v>
+        <v>399443</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>92865</v>
+        <v>352712</v>
       </c>
       <c r="F20" s="3" t="n"/>
       <c r="G20" s="3" t="n"/>
@@ -949,14 +947,14 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred</t>
+          <t xml:space="preserve"> long-term debt</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>10215</v>
+        <v>388971</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>10098</v>
+        <v>99784</v>
       </c>
       <c r="F21" s="3" t="n"/>
       <c r="G21" s="3" t="n"/>
@@ -968,18 +966,18 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred income taxes</t>
+          <t xml:space="preserve"> deferred rent</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
-        <v>45951</v>
+        <v>62610</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>58940</v>
+        <v>67390</v>
       </c>
       <c r="F22" s="3" t="n"/>
       <c r="G22" s="3" t="n"/>
@@ -991,18 +989,18 @@
         <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total liabilities</t>
+          <t xml:space="preserve"> deferred income taxes</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>2442851</v>
+        <v>70447</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>2359152</v>
+        <v>76589</v>
       </c>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
@@ -1014,18 +1012,18 @@
         <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> issued and outstanding at december and respectively</t>
+          <t xml:space="preserve"> other long-term liabilities</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
-        <v>60</v>
+        <v>52566</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>58</v>
+        <v>58027</v>
       </c>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
@@ -1037,18 +1035,18 @@
         <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> additional paid-in capital</t>
+          <t xml:space="preserve"> total liabilities</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>910304</v>
+        <v>974037</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>648031</v>
+        <v>654502</v>
       </c>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
@@ -1060,19 +1058,17 @@
         <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accumulated other comprehensive loss</t>
+          <t xml:space="preserve"> redeemable noncontrolling interest</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
-        <v>-27069</v>
-      </c>
-      <c r="E26" s="3" t="n">
-        <v>-50331</v>
-      </c>
+        <v>3981</v>
+      </c>
+      <c r="E26" s="3" t="n"/>
       <c r="F26" s="3" t="n"/>
       <c r="G26" s="3" t="n"/>
       <c r="H26" s="3" t="n"/>
@@ -1083,18 +1079,18 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> retained earnings</t>
+          <t xml:space="preserve"> treasury stock carried at cost; shares at december and shares at</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>400502</v>
+        <v>-1111586</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>373510</v>
+        <v>-706073</v>
       </c>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
@@ -1106,18 +1102,18 @@
         <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total stockholders’ equity</t>
+          <t xml:space="preserve"> additional paid-in capital</t>
         </is>
       </c>
       <c r="D28" s="3" t="n">
-        <v>1283797</v>
+        <v>235393</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>971268</v>
+        <v>214437</v>
       </c>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
@@ -1129,18 +1125,18 @@
         <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total liabilities and stockholders’ equity see accompanying notes to consolidated financial statements.</t>
+          <t xml:space="preserve"> accumulated other comprehensive income (loss)</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>3726648</v>
+        <v>-5029</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>3330420</v>
+        <v>-1360</v>
       </c>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
@@ -1148,135 +1144,414 @@
       <c r="I29" s="3" t="n"/>
     </row>
     <row r="30">
-      <c r="D30" s="3" t="n"/>
-      <c r="E30" s="3" t="n"/>
+      <c r="A30" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="n">
+        <v>46</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> retained ca:uings</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>1378519</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>1229177</v>
+      </c>
       <c r="F30" s="3" t="n"/>
       <c r="G30" s="3" t="n"/>
       <c r="H30" s="3" t="n"/>
       <c r="I30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="D31" s="3" t="n"/>
-      <c r="E31" s="3" t="n"/>
+      <c r="A31" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" t="n">
+        <v>47</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> total stockholders' equity</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>497300</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>736184</v>
+      </c>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="3" t="n"/>
       <c r="I31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="D32" s="3" t="n"/>
-      <c r="E32" s="3" t="n"/>
+      <c r="A32" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" t="n">
+        <v>48</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> total liabilities redeemable the accompanying noncontrolling notes interest are an and integral stockholders' part of equity the consolidated financial statements.</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>1475318</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>1390686</v>
+      </c>
       <c r="F32" s="3" t="n"/>
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="3" t="n"/>
       <c r="I32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="D33" s="3" t="n"/>
-      <c r="E33" s="3" t="n"/>
-      <c r="F33" s="3" t="n"/>
+      <c r="A33" t="n">
+        <v>2</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> bakery-cafe sales net</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>2358794</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <v>2230370</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>2108908</v>
+      </c>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="3" t="n"/>
       <c r="I33" s="3" t="n"/>
     </row>
     <row r="34">
-      <c r="D34" s="3" t="n"/>
-      <c r="E34" s="3" t="n"/>
-      <c r="F34" s="3" t="n"/>
+      <c r="A34" t="n">
+        <v>2</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> franchise royalties and fees</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>138563</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>123686</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>112641</v>
+      </c>
       <c r="G34" s="3" t="n"/>
       <c r="H34" s="3" t="n"/>
       <c r="I34" s="3" t="n"/>
     </row>
     <row r="35">
-      <c r="D35" s="3" t="n"/>
-      <c r="E35" s="3" t="n"/>
-      <c r="F35" s="3" t="n"/>
+      <c r="A35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B35" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> fresh dough and other product sales to franchisees</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>184223</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>175139</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>163453</v>
+      </c>
       <c r="G35" s="3" t="n"/>
       <c r="H35" s="3" t="n"/>
       <c r="I35" s="3" t="n"/>
     </row>
     <row r="36">
-      <c r="D36" s="3" t="n"/>
-      <c r="E36" s="3" t="n"/>
-      <c r="F36" s="3" t="n"/>
+      <c r="A36" t="n">
+        <v>2</v>
+      </c>
+      <c r="B36" t="n">
+        <v>5</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> total</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>2681580</v>
+      </c>
+      <c r="E36" s="3" t="n">
+        <v>2529195</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>2385002</v>
+      </c>
       <c r="G36" s="3" t="n"/>
       <c r="H36" s="3" t="n"/>
       <c r="I36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="D37" s="3" t="n"/>
-      <c r="E37" s="3" t="n"/>
-      <c r="F37" s="3" t="n"/>
+      <c r="A37" t="n">
+        <v>2</v>
+      </c>
+      <c r="B37" t="n">
+        <v>11</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cost of food and paper products</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>715502</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>669860</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>625622</v>
+      </c>
       <c r="G37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="I37" s="3" t="n"/>
     </row>
     <row r="38">
-      <c r="D38" s="3" t="n"/>
-      <c r="E38" s="3" t="n"/>
-      <c r="F38" s="3" t="n"/>
+      <c r="A38" t="n">
+        <v>2</v>
+      </c>
+      <c r="B38" t="n">
+        <v>12</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> labor</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>754646</v>
+      </c>
+      <c r="E38" s="3" t="n">
+        <v>685576</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>625457</v>
+      </c>
       <c r="G38" s="3" t="n"/>
       <c r="H38" s="3" t="n"/>
       <c r="I38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="D39" s="3" t="n"/>
-      <c r="E39" s="3" t="n"/>
-      <c r="F39" s="3" t="n"/>
+      <c r="A39" t="n">
+        <v>2</v>
+      </c>
+      <c r="B39" t="n">
+        <v>13</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> occupancy</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>169998</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>159794</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>148816</v>
+      </c>
       <c r="G39" s="3" t="n"/>
       <c r="H39" s="3" t="n"/>
       <c r="I39" s="3" t="n"/>
     </row>
     <row r="40">
-      <c r="D40" s="3" t="n"/>
-      <c r="E40" s="3" t="n"/>
-      <c r="F40" s="3" t="n"/>
+      <c r="A40" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" t="n">
+        <v>14</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> other operating expenses</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>334635</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>314879</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>295539</v>
+      </c>
       <c r="G40" s="3" t="n"/>
       <c r="H40" s="3" t="n"/>
       <c r="I40" s="3" t="n"/>
     </row>
     <row r="41">
-      <c r="D41" s="3" t="n"/>
-      <c r="E41" s="3" t="n"/>
-      <c r="F41" s="3" t="n"/>
+      <c r="A41" t="n">
+        <v>2</v>
+      </c>
+      <c r="B41" t="n">
+        <v>15</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> total bakery-cafe expenses</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>1974781</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>1830109</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>1695434</v>
+      </c>
       <c r="G41" s="3" t="n"/>
       <c r="H41" s="3" t="n"/>
       <c r="I41" s="3" t="n"/>
     </row>
     <row r="42">
-      <c r="D42" s="3" t="n"/>
-      <c r="E42" s="3" t="n"/>
-      <c r="F42" s="3" t="n"/>
+      <c r="A42" t="n">
+        <v>2</v>
+      </c>
+      <c r="B42" t="n">
+        <v>16</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> fresh dough and other product cost of sales to franchisees</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>160706</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>152267</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>142160</v>
+      </c>
       <c r="G42" s="3" t="n"/>
       <c r="H42" s="3" t="n"/>
       <c r="I42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="D43" s="3" t="n"/>
-      <c r="E43" s="3" t="n"/>
-      <c r="F43" s="3" t="n"/>
+      <c r="A43" t="n">
+        <v>2</v>
+      </c>
+      <c r="B43" t="n">
+        <v>17</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> depreciation and amortization</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>135398</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>124109</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>106523</v>
+      </c>
       <c r="G43" s="3" t="n"/>
       <c r="H43" s="3" t="n"/>
       <c r="I43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="D44" s="3" t="n"/>
-      <c r="E44" s="3" t="n"/>
-      <c r="F44" s="3" t="n"/>
+      <c r="A44" t="n">
+        <v>2</v>
+      </c>
+      <c r="B44" t="n">
+        <v>18</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> general and administrative expenses</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>142904</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>138060</v>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>123335</v>
+      </c>
       <c r="G44" s="3" t="n"/>
       <c r="H44" s="3" t="n"/>
       <c r="I44" s="3" t="n"/>
     </row>
     <row r="45">
-      <c r="D45" s="3" t="n"/>
-      <c r="E45" s="3" t="n"/>
-      <c r="F45" s="3" t="n"/>
+      <c r="A45" t="n">
+        <v>2</v>
+      </c>
+      <c r="B45" t="n">
+        <v>19</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> pre-opening</t>
+        </is>
+      </c>
+      <c r="D45" s="3" t="n">
+        <v>9089</v>
+      </c>
+      <c r="E45" s="3" t="n">
+        <v>8707</v>
+      </c>
+      <c r="F45" s="3" t="n">
+        <v>7794</v>
+      </c>
       <c r="G45" s="3" t="n"/>
       <c r="H45" s="3" t="n"/>
       <c r="I45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="D46" s="3" t="n"/>
+      <c r="A46" t="n">
+        <v>2</v>
+      </c>
+      <c r="B46" t="n">
+        <v>21</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> refranchising loss</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>17108</v>
+      </c>
       <c r="E46" s="3" t="n"/>
       <c r="F46" s="3" t="n"/>
       <c r="G46" s="3" t="n"/>
@@ -1284,63 +1559,195 @@
       <c r="I46" s="3" t="n"/>
     </row>
     <row r="47">
-      <c r="D47" s="3" t="n"/>
-      <c r="E47" s="3" t="n"/>
-      <c r="F47" s="3" t="n"/>
+      <c r="A47" t="n">
+        <v>2</v>
+      </c>
+      <c r="B47" t="n">
+        <v>22</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> total and</t>
+        </is>
+      </c>
+      <c r="D47" s="3" t="n">
+        <v>2439986</v>
+      </c>
+      <c r="E47" s="3" t="n">
+        <v>2253252</v>
+      </c>
+      <c r="F47" s="3" t="n">
+        <v>2075246</v>
+      </c>
       <c r="G47" s="3" t="n"/>
       <c r="H47" s="3" t="n"/>
       <c r="I47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="D48" s="3" t="n"/>
-      <c r="E48" s="3" t="n"/>
-      <c r="F48" s="3" t="n"/>
+      <c r="A48" t="n">
+        <v>2</v>
+      </c>
+      <c r="B48" t="n">
+        <v>24</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> operating profit</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>241594</v>
+      </c>
+      <c r="E48" s="3" t="n">
+        <v>275943</v>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>309756</v>
+      </c>
       <c r="G48" s="3" t="n"/>
       <c r="H48" s="3" t="n"/>
       <c r="I48" s="3" t="n"/>
     </row>
     <row r="49">
-      <c r="D49" s="3" t="n"/>
-      <c r="E49" s="3" t="n"/>
-      <c r="F49" s="3" t="n"/>
+      <c r="A49" t="n">
+        <v>2</v>
+      </c>
+      <c r="B49" t="n">
+        <v>25</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> interest</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>3830</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>1824</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>1053</v>
+      </c>
       <c r="G49" s="3" t="n"/>
       <c r="H49" s="3" t="n"/>
       <c r="I49" s="3" t="n"/>
     </row>
     <row r="50">
-      <c r="D50" s="3" t="n"/>
-      <c r="E50" s="3" t="n"/>
-      <c r="F50" s="3" t="n"/>
+      <c r="A50" t="n">
+        <v>2</v>
+      </c>
+      <c r="B50" t="n">
+        <v>27</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> other (income)</t>
+        </is>
+      </c>
+      <c r="D50" s="3" t="n">
+        <v>1192</v>
+      </c>
+      <c r="E50" s="3" t="n">
+        <v>-3175</v>
+      </c>
+      <c r="F50" s="3" t="n">
+        <v>-4017</v>
+      </c>
       <c r="G50" s="3" t="n"/>
       <c r="H50" s="3" t="n"/>
       <c r="I50" s="3" t="n"/>
     </row>
     <row r="51">
-      <c r="D51" s="3" t="n"/>
-      <c r="E51" s="3" t="n"/>
-      <c r="F51" s="3" t="n"/>
+      <c r="A51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" t="n">
+        <v>29</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> income before income taxes</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="n">
+        <v>236572</v>
+      </c>
+      <c r="E51" s="3" t="n">
+        <v>277294</v>
+      </c>
+      <c r="F51" s="3" t="n">
+        <v>312720</v>
+      </c>
       <c r="G51" s="3" t="n"/>
       <c r="H51" s="3" t="n"/>
       <c r="I51" s="3" t="n"/>
     </row>
     <row r="52">
-      <c r="D52" s="3" t="n"/>
-      <c r="E52" s="3" t="n"/>
-      <c r="F52" s="3" t="n"/>
+      <c r="A52" t="n">
+        <v>2</v>
+      </c>
+      <c r="B52" t="n">
+        <v>30</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> income taxes</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="n">
+        <v>87247</v>
+      </c>
+      <c r="E52" s="3" t="n">
+        <v>98001</v>
+      </c>
+      <c r="F52" s="3" t="n">
+        <v>116551</v>
+      </c>
       <c r="G52" s="3" t="n"/>
       <c r="H52" s="3" t="n"/>
       <c r="I52" s="3" t="n"/>
     </row>
     <row r="53">
-      <c r="D53" s="3" t="n"/>
-      <c r="E53" s="3" t="n"/>
-      <c r="F53" s="3" t="n"/>
+      <c r="A53" t="n">
+        <v>2</v>
+      </c>
+      <c r="B53" t="n">
+        <v>31</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net income</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="n">
+        <v>149325</v>
+      </c>
+      <c r="E53" s="3" t="n">
+        <v>179293</v>
+      </c>
+      <c r="F53" s="3" t="n">
+        <v>196169</v>
+      </c>
       <c r="G53" s="3" t="n"/>
       <c r="H53" s="3" t="n"/>
       <c r="I53" s="3" t="n"/>
     </row>
     <row r="54">
-      <c r="D54" s="3" t="n"/>
+      <c r="A54" t="n">
+        <v>2</v>
+      </c>
+      <c r="B54" t="n">
+        <v>32</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> less: net loss attributable to noncontrolling interest</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="n">
+        <v>-17</v>
+      </c>
       <c r="E54" s="3" t="n"/>
       <c r="F54" s="3" t="n"/>
       <c r="G54" s="3" t="n"/>
@@ -1348,87 +1755,270 @@
       <c r="I54" s="3" t="n"/>
     </row>
     <row r="55">
-      <c r="D55" s="3" t="n"/>
-      <c r="E55" s="3" t="n"/>
-      <c r="F55" s="3" t="n"/>
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="n">
+        <v>33</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net income attributable to panera bread company</t>
+        </is>
+      </c>
+      <c r="D55" s="3" t="n">
+        <v>149342</v>
+      </c>
+      <c r="E55" s="3" t="n">
+        <v>179293</v>
+      </c>
+      <c r="F55" s="3" t="n">
+        <v>196169</v>
+      </c>
       <c r="G55" s="3" t="n"/>
       <c r="H55" s="3" t="n"/>
       <c r="I55" s="3" t="n"/>
     </row>
     <row r="56">
-      <c r="D56" s="3" t="n"/>
-      <c r="E56" s="3" t="n"/>
-      <c r="F56" s="3" t="n"/>
+      <c r="A56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" t="n">
+        <v>36</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> basic</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="F56" s="3" t="n">
+        <v>6.85</v>
+      </c>
       <c r="G56" s="3" t="n"/>
       <c r="H56" s="3" t="n"/>
       <c r="I56" s="3" t="n"/>
     </row>
     <row r="57">
-      <c r="D57" s="3" t="n"/>
-      <c r="E57" s="3" t="n"/>
-      <c r="F57" s="3" t="n"/>
+      <c r="A57" t="n">
+        <v>2</v>
+      </c>
+      <c r="B57" t="n">
+        <v>37</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> diluted</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="E57" s="3" t="n">
+        <v>6.64</v>
+      </c>
+      <c r="F57" s="3" t="n">
+        <v>6.81</v>
+      </c>
       <c r="G57" s="3" t="n"/>
       <c r="H57" s="3" t="n"/>
       <c r="I57" s="3" t="n"/>
     </row>
     <row r="58">
-      <c r="D58" s="3" t="n"/>
-      <c r="E58" s="3" t="n"/>
-      <c r="F58" s="3" t="n"/>
+      <c r="A58" t="n">
+        <v>2</v>
+      </c>
+      <c r="B58" t="n">
+        <v>40</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> basic</t>
+        </is>
+      </c>
+      <c r="D58" s="3" t="n">
+        <v>25685</v>
+      </c>
+      <c r="E58" s="3" t="n">
+        <v>26881</v>
+      </c>
+      <c r="F58" s="3" t="n">
+        <v>28629</v>
+      </c>
       <c r="G58" s="3" t="n"/>
       <c r="H58" s="3" t="n"/>
       <c r="I58" s="3" t="n"/>
     </row>
     <row r="59">
-      <c r="D59" s="3" t="n"/>
-      <c r="E59" s="3" t="n"/>
-      <c r="F59" s="3" t="n"/>
+      <c r="A59" t="n">
+        <v>2</v>
+      </c>
+      <c r="B59" t="n">
+        <v>41</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> viluted 1he accompanying notes are an integral part of the consolidated financial statements.</t>
+        </is>
+      </c>
+      <c r="D59" s="3" t="n">
+        <v>25788</v>
+      </c>
+      <c r="E59" s="3" t="n">
+        <v>26999</v>
+      </c>
+      <c r="F59" s="3" t="n">
+        <v>28794</v>
+      </c>
       <c r="G59" s="3" t="n"/>
       <c r="H59" s="3" t="n"/>
       <c r="I59" s="3" t="n"/>
     </row>
     <row r="60">
-      <c r="D60" s="3" t="n"/>
-      <c r="E60" s="3" t="n"/>
-      <c r="F60" s="3" t="n"/>
+      <c r="A60" t="n">
+        <v>3</v>
+      </c>
+      <c r="B60" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net income</t>
+        </is>
+      </c>
+      <c r="D60" s="3" t="n">
+        <v>149325</v>
+      </c>
+      <c r="E60" s="3" t="n">
+        <v>179293</v>
+      </c>
+      <c r="F60" s="3" t="n">
+        <v>196169</v>
+      </c>
       <c r="G60" s="3" t="n"/>
       <c r="H60" s="3" t="n"/>
       <c r="I60" s="3" t="n"/>
     </row>
     <row r="61">
-      <c r="D61" s="3" t="n"/>
-      <c r="E61" s="3" t="n"/>
-      <c r="F61" s="3" t="n"/>
+      <c r="A61" t="n">
+        <v>3</v>
+      </c>
+      <c r="B61" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> depreciation and amortization</t>
+        </is>
+      </c>
+      <c r="D61" s="3" t="n">
+        <v>135398</v>
+      </c>
+      <c r="E61" s="3" t="n">
+        <v>124109</v>
+      </c>
+      <c r="F61" s="3" t="n">
+        <v>106523</v>
+      </c>
       <c r="G61" s="3" t="n"/>
       <c r="H61" s="3" t="n"/>
       <c r="I61" s="3" t="n"/>
     </row>
     <row r="62">
-      <c r="D62" s="3" t="n"/>
-      <c r="E62" s="3" t="n"/>
-      <c r="F62" s="3" t="n"/>
+      <c r="A62" t="n">
+        <v>3</v>
+      </c>
+      <c r="B62" t="n">
+        <v>5</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> stock-based compensation expense</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="n">
+        <v>15086</v>
+      </c>
+      <c r="E62" s="3" t="n">
+        <v>10077</v>
+      </c>
+      <c r="F62" s="3" t="n">
+        <v>10703</v>
+      </c>
       <c r="G62" s="3" t="n"/>
       <c r="H62" s="3" t="n"/>
       <c r="I62" s="3" t="n"/>
     </row>
     <row r="63">
-      <c r="D63" s="3" t="n"/>
-      <c r="E63" s="3" t="n"/>
-      <c r="F63" s="3" t="n"/>
+      <c r="A63" t="n">
+        <v>3</v>
+      </c>
+      <c r="B63" t="n">
+        <v>6</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="n">
+        <v>-2057</v>
+      </c>
+      <c r="E63" s="3" t="n">
+        <v>-3089</v>
+      </c>
+      <c r="F63" s="3" t="n">
+        <v>-8100</v>
+      </c>
       <c r="G63" s="3" t="n"/>
       <c r="H63" s="3" t="n"/>
       <c r="I63" s="3" t="n"/>
     </row>
     <row r="64">
-      <c r="D64" s="3" t="n"/>
-      <c r="E64" s="3" t="n"/>
-      <c r="F64" s="3" t="n"/>
+      <c r="A64" t="n">
+        <v>3</v>
+      </c>
+      <c r="B64" t="n">
+        <v>7</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> deferred income taxes</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="n">
+        <v>-10991</v>
+      </c>
+      <c r="E64" s="3" t="n">
+        <v>10459</v>
+      </c>
+      <c r="F64" s="3" t="n">
+        <v>10356</v>
+      </c>
       <c r="G64" s="3" t="n"/>
       <c r="H64" s="3" t="n"/>
       <c r="I64" s="3" t="n"/>
     </row>
     <row r="65">
-      <c r="D65" s="3" t="n"/>
+      <c r="A65" t="n">
+        <v>3</v>
+      </c>
+      <c r="B65" t="n">
+        <v>8</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> refranchising loss</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="n">
+        <v>12942</v>
+      </c>
       <c r="E65" s="3" t="n"/>
       <c r="F65" s="3" t="n"/>
       <c r="G65" s="3" t="n"/>
@@ -1436,119 +2026,358 @@
       <c r="I65" s="3" t="n"/>
     </row>
     <row r="66">
-      <c r="D66" s="3" t="n"/>
-      <c r="E66" s="3" t="n"/>
-      <c r="F66" s="3" t="n"/>
+      <c r="A66" t="n">
+        <v>3</v>
+      </c>
+      <c r="B66" t="n">
+        <v>9</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> other</t>
+        </is>
+      </c>
+      <c r="D66" s="3" t="n">
+        <v>3505</v>
+      </c>
+      <c r="E66" s="3" t="n">
+        <v>4617</v>
+      </c>
+      <c r="F66" s="3" t="n">
+        <v>6353</v>
+      </c>
       <c r="G66" s="3" t="n"/>
       <c r="H66" s="3" t="n"/>
       <c r="I66" s="3" t="n"/>
     </row>
     <row r="67">
-      <c r="D67" s="3" t="n"/>
-      <c r="E67" s="3" t="n"/>
-      <c r="F67" s="3" t="n"/>
+      <c r="A67" t="n">
+        <v>3</v>
+      </c>
+      <c r="B67" t="n">
+        <v>12</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> trade and other accounts receivable net</t>
+        </is>
+      </c>
+      <c r="D67" s="3" t="n">
+        <v>-3605</v>
+      </c>
+      <c r="E67" s="3" t="n">
+        <v>-22139</v>
+      </c>
+      <c r="F67" s="3" t="n">
+        <v>3021</v>
+      </c>
       <c r="G67" s="3" t="n"/>
       <c r="H67" s="3" t="n"/>
       <c r="I67" s="3" t="n"/>
     </row>
     <row r="68">
-      <c r="D68" s="3" t="n"/>
-      <c r="E68" s="3" t="n"/>
-      <c r="F68" s="3" t="n"/>
+      <c r="A68" t="n">
+        <v>3</v>
+      </c>
+      <c r="B68" t="n">
+        <v>13</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> inventories</t>
+        </is>
+      </c>
+      <c r="D68" s="3" t="n">
+        <v>-1698</v>
+      </c>
+      <c r="E68" s="3" t="n">
+        <v>-895</v>
+      </c>
+      <c r="F68" s="3" t="n">
+        <v>-2186</v>
+      </c>
       <c r="G68" s="3" t="n"/>
       <c r="H68" s="3" t="n"/>
       <c r="I68" s="3" t="n"/>
     </row>
     <row r="69">
-      <c r="D69" s="3" t="n"/>
-      <c r="E69" s="3" t="n"/>
-      <c r="F69" s="3" t="n"/>
+      <c r="A69" t="n">
+        <v>3</v>
+      </c>
+      <c r="B69" t="n">
+        <v>14</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> prepaid and other</t>
+        </is>
+      </c>
+      <c r="D69" s="3" t="n">
+        <v>-7191</v>
+      </c>
+      <c r="E69" s="3" t="n">
+        <v>-8524</v>
+      </c>
+      <c r="F69" s="3" t="n">
+        <v>-841</v>
+      </c>
       <c r="G69" s="3" t="n"/>
       <c r="H69" s="3" t="n"/>
       <c r="I69" s="3" t="n"/>
     </row>
     <row r="70">
-      <c r="D70" s="3" t="n"/>
-      <c r="E70" s="3" t="n"/>
-      <c r="F70" s="3" t="n"/>
+      <c r="A70" t="n">
+        <v>3</v>
+      </c>
+      <c r="B70" t="n">
+        <v>16</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> deposits and other</t>
+        </is>
+      </c>
+      <c r="D70" s="3" t="n">
+        <v>-455</v>
+      </c>
+      <c r="E70" s="3" t="n">
+        <v>239</v>
+      </c>
+      <c r="F70" s="3" t="n">
+        <v>1449</v>
+      </c>
       <c r="G70" s="3" t="n"/>
       <c r="H70" s="3" t="n"/>
       <c r="I70" s="3" t="n"/>
     </row>
     <row r="71">
-      <c r="D71" s="3" t="n"/>
-      <c r="E71" s="3" t="n"/>
-      <c r="F71" s="3" t="n"/>
+      <c r="A71" t="n">
+        <v>3</v>
+      </c>
+      <c r="B71" t="n">
+        <v>17</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> accounts payable</t>
+        </is>
+      </c>
+      <c r="D71" s="3" t="n">
+        <v>-183</v>
+      </c>
+      <c r="E71" s="3" t="n">
+        <v>1978</v>
+      </c>
+      <c r="F71" s="3" t="n">
+        <v>8162</v>
+      </c>
       <c r="G71" s="3" t="n"/>
       <c r="H71" s="3" t="n"/>
       <c r="I71" s="3" t="n"/>
     </row>
     <row r="72">
-      <c r="D72" s="3" t="n"/>
-      <c r="E72" s="3" t="n"/>
-      <c r="F72" s="3" t="n"/>
+      <c r="A72" t="n">
+        <v>3</v>
+      </c>
+      <c r="B72" t="n">
+        <v>18</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> accrued</t>
+        </is>
+      </c>
+      <c r="D72" s="3" t="n">
+        <v>31169</v>
+      </c>
+      <c r="E72" s="3" t="n">
+        <v>35288</v>
+      </c>
+      <c r="F72" s="3" t="n">
+        <v>13372</v>
+      </c>
       <c r="G72" s="3" t="n"/>
       <c r="H72" s="3" t="n"/>
       <c r="I72" s="3" t="n"/>
     </row>
     <row r="73">
-      <c r="D73" s="3" t="n"/>
-      <c r="E73" s="3" t="n"/>
-      <c r="F73" s="3" t="n"/>
+      <c r="A73" t="n">
+        <v>3</v>
+      </c>
+      <c r="B73" t="n">
+        <v>20</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> deferred rent</t>
+        </is>
+      </c>
+      <c r="D73" s="3" t="n">
+        <v>3751</v>
+      </c>
+      <c r="E73" s="3" t="n">
+        <v>1067</v>
+      </c>
+      <c r="F73" s="3" t="n">
+        <v>5868</v>
+      </c>
       <c r="G73" s="3" t="n"/>
       <c r="H73" s="3" t="n"/>
       <c r="I73" s="3" t="n"/>
     </row>
     <row r="74">
-      <c r="D74" s="3" t="n"/>
-      <c r="E74" s="3" t="n"/>
-      <c r="F74" s="3" t="n"/>
+      <c r="A74" t="n">
+        <v>3</v>
+      </c>
+      <c r="B74" t="n">
+        <v>21</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> other long-term liabilities</t>
+        </is>
+      </c>
+      <c r="D74" s="3" t="n">
+        <v>-6951</v>
+      </c>
+      <c r="E74" s="3" t="n">
+        <v>2599</v>
+      </c>
+      <c r="F74" s="3" t="n">
+        <v>-2432</v>
+      </c>
       <c r="G74" s="3" t="n"/>
       <c r="H74" s="3" t="n"/>
       <c r="I74" s="3" t="n"/>
     </row>
     <row r="75">
-      <c r="D75" s="3" t="n"/>
-      <c r="E75" s="3" t="n"/>
-      <c r="F75" s="3" t="n"/>
+      <c r="A75" t="n">
+        <v>3</v>
+      </c>
+      <c r="B75" t="n">
+        <v>22</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net cash provided by operating activities</t>
+        </is>
+      </c>
+      <c r="D75" s="3" t="n">
+        <v>318045</v>
+      </c>
+      <c r="E75" s="3" t="n">
+        <v>335079</v>
+      </c>
+      <c r="F75" s="3" t="n">
+        <v>348417</v>
+      </c>
       <c r="G75" s="3" t="n"/>
       <c r="H75" s="3" t="n"/>
       <c r="I75" s="3" t="n"/>
     </row>
     <row r="76">
-      <c r="D76" s="3" t="n"/>
-      <c r="E76" s="3" t="n"/>
-      <c r="F76" s="3" t="n"/>
+      <c r="A76" t="n">
+        <v>3</v>
+      </c>
+      <c r="B76" t="n">
+        <v>24</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> additions to property and equipment</t>
+        </is>
+      </c>
+      <c r="D76" s="3" t="n">
+        <v>-223932</v>
+      </c>
+      <c r="E76" s="3" t="n">
+        <v>-224217</v>
+      </c>
+      <c r="F76" s="3" t="n">
+        <v>-192010</v>
+      </c>
       <c r="G76" s="3" t="n"/>
       <c r="H76" s="3" t="n"/>
       <c r="I76" s="3" t="n"/>
     </row>
     <row r="77">
+      <c r="A77" t="n">
+        <v>3</v>
+      </c>
+      <c r="B77" t="n">
+        <v>25</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> acquisitions net of cash acquired</t>
+        </is>
+      </c>
       <c r="D77" s="3" t="n"/>
       <c r="E77" s="3" t="n"/>
-      <c r="F77" s="3" t="n"/>
+      <c r="F77" s="3" t="n">
+        <v>-2446</v>
+      </c>
       <c r="G77" s="3" t="n"/>
       <c r="H77" s="3" t="n"/>
       <c r="I77" s="3" t="n"/>
     </row>
     <row r="78">
+      <c r="A78" t="n">
+        <v>3</v>
+      </c>
+      <c r="B78" t="n">
+        <v>26</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> purchase of investments</t>
+        </is>
+      </c>
       <c r="D78" s="3" t="n"/>
       <c r="E78" s="3" t="n"/>
-      <c r="F78" s="3" t="n"/>
+      <c r="F78" s="3" t="n">
+        <v>-97919</v>
+      </c>
       <c r="G78" s="3" t="n"/>
       <c r="H78" s="3" t="n"/>
       <c r="I78" s="3" t="n"/>
     </row>
     <row r="79">
+      <c r="A79" t="n">
+        <v>3</v>
+      </c>
+      <c r="B79" t="n">
+        <v>27</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from sale of investments</t>
+        </is>
+      </c>
       <c r="D79" s="3" t="n"/>
       <c r="E79" s="3" t="n"/>
-      <c r="F79" s="3" t="n"/>
+      <c r="F79" s="3" t="n">
+        <v>97936</v>
+      </c>
       <c r="G79" s="3" t="n"/>
       <c r="H79" s="3" t="n"/>
       <c r="I79" s="3" t="n"/>
     </row>
     <row r="80">
-      <c r="D80" s="3" t="n"/>
+      <c r="A80" t="n">
+        <v>3</v>
+      </c>
+      <c r="B80" t="n">
+        <v>28</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from refranchising</t>
+        </is>
+      </c>
+      <c r="D80" s="3" t="n">
+        <v>46869</v>
+      </c>
       <c r="E80" s="3" t="n"/>
       <c r="F80" s="3" t="n"/>
       <c r="G80" s="3" t="n"/>
@@ -1556,7 +2385,20 @@
       <c r="I80" s="3" t="n"/>
     </row>
     <row r="81">
-      <c r="D81" s="3" t="n"/>
+      <c r="A81" t="n">
+        <v>3</v>
+      </c>
+      <c r="B81" t="n">
+        <v>29</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from sale of property and equipment</t>
+        </is>
+      </c>
+      <c r="D81" s="3" t="n">
+        <v>1553</v>
+      </c>
       <c r="E81" s="3" t="n"/>
       <c r="F81" s="3" t="n"/>
       <c r="G81" s="3" t="n"/>
@@ -1564,31 +2406,93 @@
       <c r="I81" s="3" t="n"/>
     </row>
     <row r="82">
-      <c r="D82" s="3" t="n"/>
-      <c r="E82" s="3" t="n"/>
-      <c r="F82" s="3" t="n"/>
+      <c r="A82" t="n">
+        <v>3</v>
+      </c>
+      <c r="B82" t="n">
+        <v>30</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from sale-leaseback transactions</t>
+        </is>
+      </c>
+      <c r="D82" s="3" t="n">
+        <v>10095</v>
+      </c>
+      <c r="E82" s="3" t="n">
+        <v>12900</v>
+      </c>
+      <c r="F82" s="3" t="n">
+        <v>6132</v>
+      </c>
       <c r="G82" s="3" t="n"/>
       <c r="H82" s="3" t="n"/>
       <c r="I82" s="3" t="n"/>
     </row>
     <row r="83">
-      <c r="D83" s="3" t="n"/>
-      <c r="E83" s="3" t="n"/>
-      <c r="F83" s="3" t="n"/>
+      <c r="A83" t="n">
+        <v>3</v>
+      </c>
+      <c r="B83" t="n">
+        <v>31</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net cash used in investing activities</t>
+        </is>
+      </c>
+      <c r="D83" s="3" t="n">
+        <v>-165415</v>
+      </c>
+      <c r="E83" s="3" t="n">
+        <v>-211317</v>
+      </c>
+      <c r="F83" s="3" t="n">
+        <v>-188307</v>
+      </c>
       <c r="G83" s="3" t="n"/>
       <c r="H83" s="3" t="n"/>
       <c r="I83" s="3" t="n"/>
     </row>
     <row r="84">
-      <c r="D84" s="3" t="n"/>
-      <c r="E84" s="3" t="n"/>
+      <c r="A84" t="n">
+        <v>3</v>
+      </c>
+      <c r="B84" t="n">
+        <v>33</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from issuance of long-term debt</t>
+        </is>
+      </c>
+      <c r="D84" s="3" t="n">
+        <v>299070</v>
+      </c>
+      <c r="E84" s="3" t="n">
+        <v>100000</v>
+      </c>
       <c r="F84" s="3" t="n"/>
       <c r="G84" s="3" t="n"/>
       <c r="H84" s="3" t="n"/>
       <c r="I84" s="3" t="n"/>
     </row>
     <row r="85">
-      <c r="D85" s="3" t="n"/>
+      <c r="A85" t="n">
+        <v>3</v>
+      </c>
+      <c r="B85" t="n">
+        <v>34</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> repayments of long-term debt</t>
+        </is>
+      </c>
+      <c r="D85" s="3" t="n">
+        <v>-6301</v>
+      </c>
       <c r="E85" s="3" t="n"/>
       <c r="F85" s="3" t="n"/>
       <c r="G85" s="3" t="n"/>
@@ -1596,81 +2500,247 @@
       <c r="I85" s="3" t="n"/>
     </row>
     <row r="86">
-      <c r="D86" s="3" t="n"/>
-      <c r="E86" s="3" t="n"/>
+      <c r="A86" t="n">
+        <v>3</v>
+      </c>
+      <c r="B86" t="n">
+        <v>35</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> capitalized debt issuance costs</t>
+        </is>
+      </c>
+      <c r="D86" s="3" t="n">
+        <v>-363</v>
+      </c>
+      <c r="E86" s="3" t="n">
+        <v>-193</v>
+      </c>
       <c r="F86" s="3" t="n"/>
       <c r="G86" s="3" t="n"/>
       <c r="H86" s="3" t="n"/>
       <c r="I86" s="3" t="n"/>
     </row>
     <row r="87">
+      <c r="A87" t="n">
+        <v>3</v>
+      </c>
+      <c r="B87" t="n">
+        <v>36</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> payment of deferred acquisition holdback</t>
+        </is>
+      </c>
       <c r="D87" s="3" t="n"/>
-      <c r="E87" s="3" t="n"/>
-      <c r="F87" s="3" t="n"/>
+      <c r="E87" s="3" t="n">
+        <v>-270</v>
+      </c>
+      <c r="F87" s="3" t="n">
+        <v>-4112</v>
+      </c>
       <c r="G87" s="3" t="n"/>
       <c r="H87" s="3" t="n"/>
       <c r="I87" s="3" t="n"/>
     </row>
     <row r="88">
-      <c r="D88" s="3" t="n"/>
-      <c r="E88" s="3" t="n"/>
-      <c r="F88" s="3" t="n"/>
+      <c r="A88" t="n">
+        <v>3</v>
+      </c>
+      <c r="B88" t="n">
+        <v>37</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> repurchase of stock</t>
+        </is>
+      </c>
+      <c r="D88" s="3" t="n">
+        <v>-405513</v>
+      </c>
+      <c r="E88" s="3" t="n">
+        <v>-159503</v>
+      </c>
+      <c r="F88" s="3" t="n">
+        <v>-339409</v>
+      </c>
       <c r="G88" s="3" t="n"/>
       <c r="H88" s="3" t="n"/>
       <c r="I88" s="3" t="n"/>
     </row>
     <row r="89">
-      <c r="D89" s="3" t="n"/>
-      <c r="E89" s="3" t="n"/>
-      <c r="F89" s="3" t="n"/>
+      <c r="A89" t="n">
+        <v>3</v>
+      </c>
+      <c r="B89" t="n">
+        <v>39</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> exercise of employee stock options</t>
+        </is>
+      </c>
+      <c r="D89" s="3" t="n">
+        <v>288</v>
+      </c>
+      <c r="E89" s="3" t="n">
+        <v>1116</v>
+      </c>
+      <c r="F89" s="3" t="n">
+        <v>573</v>
+      </c>
       <c r="G89" s="3" t="n"/>
       <c r="H89" s="3" t="n"/>
       <c r="I89" s="3" t="n"/>
     </row>
     <row r="90">
-      <c r="D90" s="3" t="n"/>
-      <c r="E90" s="3" t="n"/>
-      <c r="F90" s="3" t="n"/>
+      <c r="A90" t="n">
+        <v>3</v>
+      </c>
+      <c r="B90" t="n">
+        <v>40</v>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
+        </is>
+      </c>
+      <c r="D90" s="3" t="n">
+        <v>2057</v>
+      </c>
+      <c r="E90" s="3" t="n">
+        <v>3089</v>
+      </c>
+      <c r="F90" s="3" t="n">
+        <v>8100</v>
+      </c>
       <c r="G90" s="3" t="n"/>
       <c r="H90" s="3" t="n"/>
       <c r="I90" s="3" t="n"/>
     </row>
     <row r="91">
-      <c r="D91" s="3" t="n"/>
-      <c r="E91" s="3" t="n"/>
-      <c r="F91" s="3" t="n"/>
+      <c r="A91" t="n">
+        <v>3</v>
+      </c>
+      <c r="B91" t="n">
+        <v>41</v>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from issuance of common stock under employee benefit plans</t>
+        </is>
+      </c>
+      <c r="D91" s="3" t="n">
+        <v>3525</v>
+      </c>
+      <c r="E91" s="3" t="n">
+        <v>3247</v>
+      </c>
+      <c r="F91" s="3" t="n">
+        <v>2842</v>
+      </c>
       <c r="G91" s="3" t="n"/>
       <c r="H91" s="3" t="n"/>
       <c r="I91" s="3" t="n"/>
     </row>
     <row r="92">
-      <c r="D92" s="3" t="n"/>
-      <c r="E92" s="3" t="n"/>
-      <c r="F92" s="3" t="n"/>
+      <c r="A92" t="n">
+        <v>3</v>
+      </c>
+      <c r="B92" t="n">
+        <v>42</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net cash used in financing activities</t>
+        </is>
+      </c>
+      <c r="D92" s="3" t="n">
+        <v>-107237</v>
+      </c>
+      <c r="E92" s="3" t="n">
+        <v>-52514</v>
+      </c>
+      <c r="F92" s="3" t="n">
+        <v>-332006</v>
+      </c>
       <c r="G92" s="3" t="n"/>
       <c r="H92" s="3" t="n"/>
       <c r="I92" s="3" t="n"/>
     </row>
     <row r="93">
-      <c r="D93" s="3" t="n"/>
-      <c r="E93" s="3" t="n"/>
-      <c r="F93" s="3" t="n"/>
+      <c r="A93" t="n">
+        <v>3</v>
+      </c>
+      <c r="B93" t="n">
+        <v>43</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net increase (decrease) in cash and cash equivalents</t>
+        </is>
+      </c>
+      <c r="D93" s="3" t="n">
+        <v>45393</v>
+      </c>
+      <c r="E93" s="3" t="n">
+        <v>71248</v>
+      </c>
+      <c r="F93" s="3" t="n">
+        <v>-171896</v>
+      </c>
       <c r="G93" s="3" t="n"/>
       <c r="H93" s="3" t="n"/>
       <c r="I93" s="3" t="n"/>
     </row>
     <row r="94">
-      <c r="D94" s="3" t="n"/>
-      <c r="E94" s="3" t="n"/>
-      <c r="F94" s="3" t="n"/>
+      <c r="A94" t="n">
+        <v>3</v>
+      </c>
+      <c r="B94" t="n">
+        <v>44</v>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cash and cash equivalents at beginning of period</t>
+        </is>
+      </c>
+      <c r="D94" s="3" t="n">
+        <v>196493</v>
+      </c>
+      <c r="E94" s="3" t="n">
+        <v>125245</v>
+      </c>
+      <c r="F94" s="3" t="n">
+        <v>297141</v>
+      </c>
       <c r="G94" s="3" t="n"/>
       <c r="H94" s="3" t="n"/>
       <c r="I94" s="3" t="n"/>
     </row>
     <row r="95">
-      <c r="D95" s="3" t="n"/>
-      <c r="E95" s="3" t="n"/>
-      <c r="F95" s="3" t="n"/>
+      <c r="A95" t="n">
+        <v>3</v>
+      </c>
+      <c r="B95" t="n">
+        <v>45</v>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cash and cash equivalents at end of 1he period accompanying notes are an integral part of the consolidated financial statements.</t>
+        </is>
+      </c>
+      <c r="D95" s="3" t="n">
+        <v>241886</v>
+      </c>
+      <c r="E95" s="3" t="n">
+        <v>196493</v>
+      </c>
+      <c r="F95" s="3" t="n">
+        <v>125245</v>
+      </c>
       <c r="G95" s="3" t="n"/>
       <c r="H95" s="3" t="n"/>
       <c r="I95" s="3" t="n"/>
@@ -8573,7 +9643,7 @@
     <row r="4268"/>
     <row r="4269"/>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improving the column recognizer function
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -490,17 +490,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>december 30. 2015</t>
+          <t>september 30. 2015</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>december 30. 2014</t>
+          <t>september 30. 2014</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>2013</t>
+          <t>december 31. 2013</t>
         </is>
       </c>
       <c r="G1" s="1" t="n"/>

</xml_diff>

<commit_message>
code from 2 years ago idk what it does
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -490,21 +490,29 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>september 30. 2015</t>
+          <t>11M</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>september 30. 2014</t>
+          <t>1/31/2023</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>december 31. 2013</t>
+          <t>1/31/2022</t>
         </is>
       </c>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>1/31/2021</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>1/31/2020</t>
+        </is>
+      </c>
       <c r="I1" s="1" t="n"/>
     </row>
     <row r="2">
@@ -512,22 +520,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents</t>
+          <t xml:space="preserve"> operating revenue</t>
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>241886</v>
+        <v>32681000</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
-      <c r="H2" s="3" t="n"/>
+        <v>26974000</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>26914000</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>16675000</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>10918000</v>
+      </c>
       <c r="I2" s="3" t="n"/>
     </row>
     <row r="3">
@@ -535,22 +549,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> trade accounts receivable net</t>
+          <t xml:space="preserve"> cost of revenue</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>38211</v>
+        <v>11561000</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>36584</v>
-      </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
-      <c r="H3" s="3" t="n"/>
+        <v>11618000</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>9439000</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>6279000</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>4150000</v>
+      </c>
       <c r="I3" s="3" t="n"/>
     </row>
     <row r="4">
@@ -558,22 +578,28 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other accounts receivable</t>
+          <t xml:space="preserve"> gross operating profit</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>77575</v>
+        <v>21120000</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>70069</v>
-      </c>
-      <c r="F4" s="3" t="n"/>
-      <c r="G4" s="3" t="n"/>
-      <c r="H4" s="3" t="n"/>
+        <v>15356000</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>17475000</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>10396000</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>6768000</v>
+      </c>
       <c r="I4" s="3" t="n"/>
     </row>
     <row r="5">
@@ -585,18 +611,24 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> inventories</t>
+          <t xml:space="preserve"> selling general and administrati</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>22482</v>
+        <v>2510000</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>22811</v>
-      </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
-      <c r="H5" s="3" t="n"/>
+        <v>2440000</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>2166000</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>1940000</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <v>1093000</v>
+      </c>
       <c r="I5" s="3" t="n"/>
     </row>
     <row r="6">
@@ -608,18 +640,24 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> prepaid and other</t>
+          <t xml:space="preserve"> research &amp; developinient</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>59457</v>
+        <v>7812000</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>51588</v>
-      </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="n"/>
+        <v>7339000</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>5268000</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>3924000</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>2829000</v>
+      </c>
       <c r="I6" s="3" t="n"/>
     </row>
     <row r="7">
@@ -627,22 +665,28 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> veferred income taxes</t>
+          <t xml:space="preserve"> operating net non income operating interest inc.</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>34479</v>
+        <v>10798000</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>28621</v>
-      </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
-      <c r="H7" s="3" t="n"/>
+        <v>5577000</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>10041000</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>4532000</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>2846000</v>
+      </c>
       <c r="I7" s="3" t="n"/>
     </row>
     <row r="8">
@@ -654,16 +698,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> assets held for sale</t>
+          <t xml:space="preserve"> interest income non operating</t>
         </is>
       </c>
       <c r="D8" s="3" t="n">
-        <v>28699</v>
-      </c>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
-      <c r="H8" s="3" t="n"/>
+        <v>541000</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>267000</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>29000</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>57000</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>178000</v>
+      </c>
       <c r="I8" s="3" t="n"/>
     </row>
     <row r="9">
@@ -675,18 +727,24 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current assets</t>
+          <t xml:space="preserve"> interest other income expense expense non operating</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>502789</v>
+        <v>261000</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>406166</v>
-      </c>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="n"/>
-      <c r="H9" s="3" t="n"/>
+        <v>262000</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>236000</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>184000</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>52000</v>
+      </c>
       <c r="I9" s="3" t="n"/>
     </row>
     <row r="10">
@@ -698,14 +756,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> property and equipment net</t>
+          <t xml:space="preserve"> v special charges 0.</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
-        <v>776248</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>787294</v>
+        <v>-1353000</v>
       </c>
       <c r="F10" s="3" t="n"/>
       <c r="G10" s="3" t="n"/>
@@ -721,14 +779,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> goodwill</t>
+          <t xml:space="preserve"> restructuring &amp; mergers acq. 0.</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>121791</v>
+        <v>0</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>120778</v>
+        <v>1353000</v>
       </c>
       <c r="F11" s="3" t="n"/>
       <c r="G11" s="3" t="n"/>
@@ -744,18 +802,24 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other intangible assets net</t>
+          <t xml:space="preserve"> other non operating income ex</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>63877</v>
+        <v>13000</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>70940</v>
-      </c>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="3" t="n"/>
-      <c r="H12" s="3" t="n"/>
+        <v>-48000</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>107000</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>-2000</v>
+      </c>
       <c r="I12" s="3" t="n"/>
     </row>
     <row r="13">
@@ -767,18 +831,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deposits and other</t>
+          <t xml:space="preserve"> pretax income</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>10613</v>
+        <v>11091000</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>5508</v>
-      </c>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
-      <c r="H13" s="3" t="n"/>
+        <v>4181000</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>9941000</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>4409000</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>2970000</v>
+      </c>
       <c r="I13" s="3" t="n"/>
     </row>
     <row r="14">
@@ -790,18 +860,24 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total other assets</t>
+          <t xml:space="preserve"> tax net provision income common stockhold</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>196281</v>
+        <v>765000</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>197226</v>
-      </c>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
-      <c r="H14" s="3" t="n"/>
+        <v>-187000</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>189000</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>77000</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>174000</v>
+      </c>
       <c r="I14" s="3" t="n"/>
     </row>
     <row r="15">
@@ -813,18 +889,24 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total assets</t>
+          <t xml:space="preserve"> vy net income</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>1475318</v>
+        <v>10326000</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>1390686</v>
-      </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
-      <c r="H15" s="3" t="n"/>
+        <v>4368000</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>9752000</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>4332000</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>2796000</v>
+      </c>
       <c r="I15" s="3" t="n"/>
     </row>
     <row r="16">
@@ -832,22 +914,28 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable</t>
+          <t xml:space="preserve"> v net income including non.</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>19805</v>
+        <v>10326000</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>19511</v>
-      </c>
-      <c r="F16" s="3" t="n"/>
-      <c r="G16" s="3" t="n"/>
-      <c r="H16" s="3" t="n"/>
+        <v>4368000</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>9752000</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>4332000</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>2796000</v>
+      </c>
       <c r="I16" s="3" t="n"/>
     </row>
     <row r="17">
@@ -855,22 +943,28 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accrued</t>
+          <t xml:space="preserve"> net income continuous op</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>359464</v>
+        <v>10326000</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>333201</v>
-      </c>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
-      <c r="H17" s="3" t="n"/>
+        <v>4368000</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>9752000</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>4332000</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>2796000</v>
+      </c>
       <c r="I17" s="3" t="n"/>
     </row>
     <row r="18">
@@ -878,20 +972,28 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cunent portion of long-term debt</t>
+          <t xml:space="preserve"> diluted ni available to com stock...</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>17229</v>
-      </c>
-      <c r="E18" s="3" t="n"/>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="n"/>
-      <c r="H18" s="3" t="n"/>
+        <v>10326000</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>4368000</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>9752000</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>4332000</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>2796000</v>
+      </c>
       <c r="I18" s="3" t="n"/>
     </row>
     <row r="19">
@@ -899,20 +1001,26 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> liabilities associated with assets held for sale</t>
+          <t xml:space="preserve"> basic eps boi</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>2945</v>
-      </c>
-      <c r="E19" s="3" t="n"/>
+        <v>4.18</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>1.76</v>
+      </c>
       <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
-      <c r="H19" s="3" t="n"/>
+      <c r="G19" s="3" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>1.15</v>
+      </c>
       <c r="I19" s="3" t="n"/>
     </row>
     <row r="20">
@@ -920,22 +1028,28 @@
         <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current liabilities</t>
+          <t xml:space="preserve"> diluted eps</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
-        <v>399443</v>
+        <v>4.14</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>352712</v>
-      </c>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
-      <c r="H20" s="3" t="n"/>
+        <v>1.74</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>1.13</v>
+      </c>
       <c r="I20" s="3" t="n"/>
     </row>
     <row r="21">
@@ -943,22 +1057,28 @@
         <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> long-term debt</t>
+          <t xml:space="preserve"> basic average shares</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>388971</v>
+        <v>2473000</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>99784</v>
-      </c>
-      <c r="F21" s="3" t="n"/>
-      <c r="G21" s="3" t="n"/>
-      <c r="H21" s="3" t="n"/>
+        <v>2487000</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>2496000</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>2468000</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>2436000</v>
+      </c>
       <c r="I21" s="3" t="n"/>
     </row>
     <row r="22">
@@ -966,22 +1086,28 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred rent</t>
+          <t xml:space="preserve"> diluted average shares</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
-        <v>62610</v>
+        <v>2491500</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>67390</v>
-      </c>
-      <c r="F22" s="3" t="n"/>
-      <c r="G22" s="3" t="n"/>
-      <c r="H22" s="3" t="n"/>
+        <v>2507000</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>2535000</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>2512000</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>2472000</v>
+      </c>
       <c r="I22" s="3" t="n"/>
     </row>
     <row r="23">
@@ -989,22 +1115,28 @@
         <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred income taxes</t>
+          <t xml:space="preserve"> total operating income as reported</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>70447</v>
+        <v>10798000</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>76589</v>
-      </c>
-      <c r="F23" s="3" t="n"/>
-      <c r="G23" s="3" t="n"/>
-      <c r="H23" s="3" t="n"/>
+        <v>4224000</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>10041000</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>4532000</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>2846000</v>
+      </c>
       <c r="I23" s="3" t="n"/>
     </row>
     <row r="24">
@@ -1012,22 +1144,28 @@
         <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
+          <t xml:space="preserve"> total expenses</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
-        <v>52566</v>
+        <v>21883000</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>58027</v>
-      </c>
-      <c r="F24" s="3" t="n"/>
-      <c r="G24" s="3" t="n"/>
-      <c r="H24" s="3" t="n"/>
+        <v>21397000</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>16873000</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>12143000</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>8072000</v>
+      </c>
       <c r="I24" s="3" t="n"/>
     </row>
     <row r="25">
@@ -1035,39 +1173,32 @@
         <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total liabilities</t>
+          <t xml:space="preserve"> net income from continuing &amp; dis...</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>974037</v>
+        <v>10326000</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>654502</v>
-      </c>
-      <c r="F25" s="3" t="n"/>
-      <c r="G25" s="3" t="n"/>
-      <c r="H25" s="3" t="n"/>
+        <v>4368000</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>9752000</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>4332000</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>2796000</v>
+      </c>
       <c r="I25" s="3" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" t="n">
-        <v>33</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> redeemable noncontrolling interest</t>
-        </is>
-      </c>
-      <c r="D26" s="3" t="n">
-        <v>3981</v>
-      </c>
+      <c r="D26" s="3" t="n"/>
       <c r="E26" s="3" t="n"/>
       <c r="F26" s="3" t="n"/>
       <c r="G26" s="3" t="n"/>
@@ -1075,483 +1206,159 @@
       <c r="I26" s="3" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" t="n">
-        <v>1</v>
-      </c>
-      <c r="B27" t="n">
-        <v>40</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> treasury stock carried at cost; shares at december and shares at</t>
-        </is>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>-1111586</v>
-      </c>
-      <c r="E27" s="3" t="n">
-        <v>-706073</v>
-      </c>
+      <c r="D27" s="3" t="n"/>
+      <c r="E27" s="3" t="n"/>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
       <c r="H27" s="3" t="n"/>
       <c r="I27" s="3" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" t="n">
-        <v>44</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> additional paid-in capital</t>
-        </is>
-      </c>
-      <c r="D28" s="3" t="n">
-        <v>235393</v>
-      </c>
-      <c r="E28" s="3" t="n">
-        <v>214437</v>
-      </c>
+      <c r="D28" s="3" t="n"/>
+      <c r="E28" s="3" t="n"/>
       <c r="F28" s="3" t="n"/>
       <c r="G28" s="3" t="n"/>
       <c r="H28" s="3" t="n"/>
       <c r="I28" s="3" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" t="n">
-        <v>45</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accumulated other comprehensive income (loss)</t>
-        </is>
-      </c>
-      <c r="D29" s="3" t="n">
-        <v>-5029</v>
-      </c>
-      <c r="E29" s="3" t="n">
-        <v>-1360</v>
-      </c>
+      <c r="D29" s="3" t="n"/>
+      <c r="E29" s="3" t="n"/>
       <c r="F29" s="3" t="n"/>
       <c r="G29" s="3" t="n"/>
       <c r="H29" s="3" t="n"/>
       <c r="I29" s="3" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" t="n">
-        <v>46</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> retained ca:uings</t>
-        </is>
-      </c>
-      <c r="D30" s="3" t="n">
-        <v>1378519</v>
-      </c>
-      <c r="E30" s="3" t="n">
-        <v>1229177</v>
-      </c>
+      <c r="D30" s="3" t="n"/>
+      <c r="E30" s="3" t="n"/>
       <c r="F30" s="3" t="n"/>
       <c r="G30" s="3" t="n"/>
       <c r="H30" s="3" t="n"/>
       <c r="I30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" t="n">
-        <v>47</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total stockholders' equity</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="n">
-        <v>497300</v>
-      </c>
-      <c r="E31" s="3" t="n">
-        <v>736184</v>
-      </c>
+      <c r="D31" s="3" t="n"/>
+      <c r="E31" s="3" t="n"/>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="3" t="n"/>
       <c r="I31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" t="n">
-        <v>48</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total liabilities redeemable the accompanying noncontrolling notes interest are an and integral stockholders' part of equity the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>1475318</v>
-      </c>
-      <c r="E32" s="3" t="n">
-        <v>1390686</v>
-      </c>
+      <c r="D32" s="3" t="n"/>
+      <c r="E32" s="3" t="n"/>
       <c r="F32" s="3" t="n"/>
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="3" t="n"/>
       <c r="I32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>2</v>
-      </c>
-      <c r="B33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> bakery-cafe sales net</t>
-        </is>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>2358794</v>
-      </c>
-      <c r="E33" s="3" t="n">
-        <v>2230370</v>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>2108908</v>
-      </c>
+      <c r="D33" s="3" t="n"/>
+      <c r="E33" s="3" t="n"/>
+      <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="3" t="n"/>
       <c r="I33" s="3" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>2</v>
-      </c>
-      <c r="B34" t="n">
-        <v>3</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> franchise royalties and fees</t>
-        </is>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>138563</v>
-      </c>
-      <c r="E34" s="3" t="n">
-        <v>123686</v>
-      </c>
-      <c r="F34" s="3" t="n">
-        <v>112641</v>
-      </c>
+      <c r="D34" s="3" t="n"/>
+      <c r="E34" s="3" t="n"/>
+      <c r="F34" s="3" t="n"/>
       <c r="G34" s="3" t="n"/>
       <c r="H34" s="3" t="n"/>
       <c r="I34" s="3" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>2</v>
-      </c>
-      <c r="B35" t="n">
-        <v>4</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> fresh dough and other product sales to franchisees</t>
-        </is>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>184223</v>
-      </c>
-      <c r="E35" s="3" t="n">
-        <v>175139</v>
-      </c>
-      <c r="F35" s="3" t="n">
-        <v>163453</v>
-      </c>
+      <c r="D35" s="3" t="n"/>
+      <c r="E35" s="3" t="n"/>
+      <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
       <c r="H35" s="3" t="n"/>
       <c r="I35" s="3" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>2</v>
-      </c>
-      <c r="B36" t="n">
-        <v>5</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total</t>
-        </is>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>2681580</v>
-      </c>
-      <c r="E36" s="3" t="n">
-        <v>2529195</v>
-      </c>
-      <c r="F36" s="3" t="n">
-        <v>2385002</v>
-      </c>
+      <c r="D36" s="3" t="n"/>
+      <c r="E36" s="3" t="n"/>
+      <c r="F36" s="3" t="n"/>
       <c r="G36" s="3" t="n"/>
       <c r="H36" s="3" t="n"/>
       <c r="I36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>2</v>
-      </c>
-      <c r="B37" t="n">
-        <v>11</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cost of food and paper products</t>
-        </is>
-      </c>
-      <c r="D37" s="3" t="n">
-        <v>715502</v>
-      </c>
-      <c r="E37" s="3" t="n">
-        <v>669860</v>
-      </c>
-      <c r="F37" s="3" t="n">
-        <v>625622</v>
-      </c>
+      <c r="D37" s="3" t="n"/>
+      <c r="E37" s="3" t="n"/>
+      <c r="F37" s="3" t="n"/>
       <c r="G37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="I37" s="3" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>2</v>
-      </c>
-      <c r="B38" t="n">
-        <v>12</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> labor</t>
-        </is>
-      </c>
-      <c r="D38" s="3" t="n">
-        <v>754646</v>
-      </c>
-      <c r="E38" s="3" t="n">
-        <v>685576</v>
-      </c>
-      <c r="F38" s="3" t="n">
-        <v>625457</v>
-      </c>
+      <c r="D38" s="3" t="n"/>
+      <c r="E38" s="3" t="n"/>
+      <c r="F38" s="3" t="n"/>
       <c r="G38" s="3" t="n"/>
       <c r="H38" s="3" t="n"/>
       <c r="I38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>2</v>
-      </c>
-      <c r="B39" t="n">
-        <v>13</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> occupancy</t>
-        </is>
-      </c>
-      <c r="D39" s="3" t="n">
-        <v>169998</v>
-      </c>
-      <c r="E39" s="3" t="n">
-        <v>159794</v>
-      </c>
-      <c r="F39" s="3" t="n">
-        <v>148816</v>
-      </c>
+      <c r="D39" s="3" t="n"/>
+      <c r="E39" s="3" t="n"/>
+      <c r="F39" s="3" t="n"/>
       <c r="G39" s="3" t="n"/>
       <c r="H39" s="3" t="n"/>
       <c r="I39" s="3" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>2</v>
-      </c>
-      <c r="B40" t="n">
-        <v>14</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other operating expenses</t>
-        </is>
-      </c>
-      <c r="D40" s="3" t="n">
-        <v>334635</v>
-      </c>
-      <c r="E40" s="3" t="n">
-        <v>314879</v>
-      </c>
-      <c r="F40" s="3" t="n">
-        <v>295539</v>
-      </c>
+      <c r="D40" s="3" t="n"/>
+      <c r="E40" s="3" t="n"/>
+      <c r="F40" s="3" t="n"/>
       <c r="G40" s="3" t="n"/>
       <c r="H40" s="3" t="n"/>
       <c r="I40" s="3" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>2</v>
-      </c>
-      <c r="B41" t="n">
-        <v>15</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total bakery-cafe expenses</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="n">
-        <v>1974781</v>
-      </c>
-      <c r="E41" s="3" t="n">
-        <v>1830109</v>
-      </c>
-      <c r="F41" s="3" t="n">
-        <v>1695434</v>
-      </c>
+      <c r="D41" s="3" t="n"/>
+      <c r="E41" s="3" t="n"/>
+      <c r="F41" s="3" t="n"/>
       <c r="G41" s="3" t="n"/>
       <c r="H41" s="3" t="n"/>
       <c r="I41" s="3" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>2</v>
-      </c>
-      <c r="B42" t="n">
-        <v>16</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> fresh dough and other product cost of sales to franchisees</t>
-        </is>
-      </c>
-      <c r="D42" s="3" t="n">
-        <v>160706</v>
-      </c>
-      <c r="E42" s="3" t="n">
-        <v>152267</v>
-      </c>
-      <c r="F42" s="3" t="n">
-        <v>142160</v>
-      </c>
+      <c r="D42" s="3" t="n"/>
+      <c r="E42" s="3" t="n"/>
+      <c r="F42" s="3" t="n"/>
       <c r="G42" s="3" t="n"/>
       <c r="H42" s="3" t="n"/>
       <c r="I42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>2</v>
-      </c>
-      <c r="B43" t="n">
-        <v>17</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
-        </is>
-      </c>
-      <c r="D43" s="3" t="n">
-        <v>135398</v>
-      </c>
-      <c r="E43" s="3" t="n">
-        <v>124109</v>
-      </c>
-      <c r="F43" s="3" t="n">
-        <v>106523</v>
-      </c>
+      <c r="D43" s="3" t="n"/>
+      <c r="E43" s="3" t="n"/>
+      <c r="F43" s="3" t="n"/>
       <c r="G43" s="3" t="n"/>
       <c r="H43" s="3" t="n"/>
       <c r="I43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>2</v>
-      </c>
-      <c r="B44" t="n">
-        <v>18</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> general and administrative expenses</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="n">
-        <v>142904</v>
-      </c>
-      <c r="E44" s="3" t="n">
-        <v>138060</v>
-      </c>
-      <c r="F44" s="3" t="n">
-        <v>123335</v>
-      </c>
+      <c r="D44" s="3" t="n"/>
+      <c r="E44" s="3" t="n"/>
+      <c r="F44" s="3" t="n"/>
       <c r="G44" s="3" t="n"/>
       <c r="H44" s="3" t="n"/>
       <c r="I44" s="3" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>2</v>
-      </c>
-      <c r="B45" t="n">
-        <v>19</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> pre-opening</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="n">
-        <v>9089</v>
-      </c>
-      <c r="E45" s="3" t="n">
-        <v>8707</v>
-      </c>
-      <c r="F45" s="3" t="n">
-        <v>7794</v>
-      </c>
+      <c r="D45" s="3" t="n"/>
+      <c r="E45" s="3" t="n"/>
+      <c r="F45" s="3" t="n"/>
       <c r="G45" s="3" t="n"/>
       <c r="H45" s="3" t="n"/>
       <c r="I45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>2</v>
-      </c>
-      <c r="B46" t="n">
-        <v>21</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> refranchising loss</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="n">
-        <v>17108</v>
-      </c>
+      <c r="D46" s="3" t="n"/>
       <c r="E46" s="3" t="n"/>
       <c r="F46" s="3" t="n"/>
       <c r="G46" s="3" t="n"/>
@@ -1559,195 +1366,63 @@
       <c r="I46" s="3" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>2</v>
-      </c>
-      <c r="B47" t="n">
-        <v>22</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total and</t>
-        </is>
-      </c>
-      <c r="D47" s="3" t="n">
-        <v>2439986</v>
-      </c>
-      <c r="E47" s="3" t="n">
-        <v>2253252</v>
-      </c>
-      <c r="F47" s="3" t="n">
-        <v>2075246</v>
-      </c>
+      <c r="D47" s="3" t="n"/>
+      <c r="E47" s="3" t="n"/>
+      <c r="F47" s="3" t="n"/>
       <c r="G47" s="3" t="n"/>
       <c r="H47" s="3" t="n"/>
       <c r="I47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>2</v>
-      </c>
-      <c r="B48" t="n">
-        <v>24</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> operating profit</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="n">
-        <v>241594</v>
-      </c>
-      <c r="E48" s="3" t="n">
-        <v>275943</v>
-      </c>
-      <c r="F48" s="3" t="n">
-        <v>309756</v>
-      </c>
+      <c r="D48" s="3" t="n"/>
+      <c r="E48" s="3" t="n"/>
+      <c r="F48" s="3" t="n"/>
       <c r="G48" s="3" t="n"/>
       <c r="H48" s="3" t="n"/>
       <c r="I48" s="3" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>2</v>
-      </c>
-      <c r="B49" t="n">
-        <v>25</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> interest</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="n">
-        <v>3830</v>
-      </c>
-      <c r="E49" s="3" t="n">
-        <v>1824</v>
-      </c>
-      <c r="F49" s="3" t="n">
-        <v>1053</v>
-      </c>
+      <c r="D49" s="3" t="n"/>
+      <c r="E49" s="3" t="n"/>
+      <c r="F49" s="3" t="n"/>
       <c r="G49" s="3" t="n"/>
       <c r="H49" s="3" t="n"/>
       <c r="I49" s="3" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>2</v>
-      </c>
-      <c r="B50" t="n">
-        <v>27</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other (income)</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="n">
-        <v>1192</v>
-      </c>
-      <c r="E50" s="3" t="n">
-        <v>-3175</v>
-      </c>
-      <c r="F50" s="3" t="n">
-        <v>-4017</v>
-      </c>
+      <c r="D50" s="3" t="n"/>
+      <c r="E50" s="3" t="n"/>
+      <c r="F50" s="3" t="n"/>
       <c r="G50" s="3" t="n"/>
       <c r="H50" s="3" t="n"/>
       <c r="I50" s="3" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>2</v>
-      </c>
-      <c r="B51" t="n">
-        <v>29</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> income before income taxes</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="n">
-        <v>236572</v>
-      </c>
-      <c r="E51" s="3" t="n">
-        <v>277294</v>
-      </c>
-      <c r="F51" s="3" t="n">
-        <v>312720</v>
-      </c>
+      <c r="D51" s="3" t="n"/>
+      <c r="E51" s="3" t="n"/>
+      <c r="F51" s="3" t="n"/>
       <c r="G51" s="3" t="n"/>
       <c r="H51" s="3" t="n"/>
       <c r="I51" s="3" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>2</v>
-      </c>
-      <c r="B52" t="n">
-        <v>30</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> income taxes</t>
-        </is>
-      </c>
-      <c r="D52" s="3" t="n">
-        <v>87247</v>
-      </c>
-      <c r="E52" s="3" t="n">
-        <v>98001</v>
-      </c>
-      <c r="F52" s="3" t="n">
-        <v>116551</v>
-      </c>
+      <c r="D52" s="3" t="n"/>
+      <c r="E52" s="3" t="n"/>
+      <c r="F52" s="3" t="n"/>
       <c r="G52" s="3" t="n"/>
       <c r="H52" s="3" t="n"/>
       <c r="I52" s="3" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>2</v>
-      </c>
-      <c r="B53" t="n">
-        <v>31</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="n">
-        <v>149325</v>
-      </c>
-      <c r="E53" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F53" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D53" s="3" t="n"/>
+      <c r="E53" s="3" t="n"/>
+      <c r="F53" s="3" t="n"/>
       <c r="G53" s="3" t="n"/>
       <c r="H53" s="3" t="n"/>
       <c r="I53" s="3" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>2</v>
-      </c>
-      <c r="B54" t="n">
-        <v>32</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> less: net loss attributable to noncontrolling interest</t>
-        </is>
-      </c>
-      <c r="D54" s="3" t="n">
-        <v>-17</v>
-      </c>
+      <c r="D54" s="3" t="n"/>
       <c r="E54" s="3" t="n"/>
       <c r="F54" s="3" t="n"/>
       <c r="G54" s="3" t="n"/>
@@ -1755,270 +1430,87 @@
       <c r="I54" s="3" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>2</v>
-      </c>
-      <c r="B55" t="n">
-        <v>33</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income attributable to panera bread company</t>
-        </is>
-      </c>
-      <c r="D55" s="3" t="n">
-        <v>149342</v>
-      </c>
-      <c r="E55" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F55" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D55" s="3" t="n"/>
+      <c r="E55" s="3" t="n"/>
+      <c r="F55" s="3" t="n"/>
       <c r="G55" s="3" t="n"/>
       <c r="H55" s="3" t="n"/>
       <c r="I55" s="3" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>2</v>
-      </c>
-      <c r="B56" t="n">
-        <v>36</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> basic</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="n">
-        <v>5.81</v>
-      </c>
-      <c r="E56" s="3" t="n">
-        <v>6.67</v>
-      </c>
-      <c r="F56" s="3" t="n">
-        <v>6.85</v>
-      </c>
+      <c r="D56" s="3" t="n"/>
+      <c r="E56" s="3" t="n"/>
+      <c r="F56" s="3" t="n"/>
       <c r="G56" s="3" t="n"/>
       <c r="H56" s="3" t="n"/>
       <c r="I56" s="3" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>2</v>
-      </c>
-      <c r="B57" t="n">
-        <v>37</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> diluted</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="n">
-        <v>5.79</v>
-      </c>
-      <c r="E57" s="3" t="n">
-        <v>6.64</v>
-      </c>
-      <c r="F57" s="3" t="n">
-        <v>6.81</v>
-      </c>
+      <c r="D57" s="3" t="n"/>
+      <c r="E57" s="3" t="n"/>
+      <c r="F57" s="3" t="n"/>
       <c r="G57" s="3" t="n"/>
       <c r="H57" s="3" t="n"/>
       <c r="I57" s="3" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>2</v>
-      </c>
-      <c r="B58" t="n">
-        <v>40</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> basic</t>
-        </is>
-      </c>
-      <c r="D58" s="3" t="n">
-        <v>25685</v>
-      </c>
-      <c r="E58" s="3" t="n">
-        <v>26881</v>
-      </c>
-      <c r="F58" s="3" t="n">
-        <v>28629</v>
-      </c>
+      <c r="D58" s="3" t="n"/>
+      <c r="E58" s="3" t="n"/>
+      <c r="F58" s="3" t="n"/>
       <c r="G58" s="3" t="n"/>
       <c r="H58" s="3" t="n"/>
       <c r="I58" s="3" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>2</v>
-      </c>
-      <c r="B59" t="n">
-        <v>41</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> viluted 1he accompanying notes are an integral part of the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="n">
-        <v>25788</v>
-      </c>
-      <c r="E59" s="3" t="n">
-        <v>26999</v>
-      </c>
-      <c r="F59" s="3" t="n">
-        <v>28794</v>
-      </c>
+      <c r="D59" s="3" t="n"/>
+      <c r="E59" s="3" t="n"/>
+      <c r="F59" s="3" t="n"/>
       <c r="G59" s="3" t="n"/>
       <c r="H59" s="3" t="n"/>
       <c r="I59" s="3" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>3</v>
-      </c>
-      <c r="B60" t="n">
-        <v>2</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income</t>
-        </is>
-      </c>
-      <c r="D60" s="3" t="n">
-        <v>149325</v>
-      </c>
-      <c r="E60" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F60" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D60" s="3" t="n"/>
+      <c r="E60" s="3" t="n"/>
+      <c r="F60" s="3" t="n"/>
       <c r="G60" s="3" t="n"/>
       <c r="H60" s="3" t="n"/>
       <c r="I60" s="3" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>3</v>
-      </c>
-      <c r="B61" t="n">
-        <v>4</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="n">
-        <v>135398</v>
-      </c>
-      <c r="E61" s="3" t="n">
-        <v>124109</v>
-      </c>
-      <c r="F61" s="3" t="n">
-        <v>106523</v>
-      </c>
+      <c r="D61" s="3" t="n"/>
+      <c r="E61" s="3" t="n"/>
+      <c r="F61" s="3" t="n"/>
       <c r="G61" s="3" t="n"/>
       <c r="H61" s="3" t="n"/>
       <c r="I61" s="3" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>3</v>
-      </c>
-      <c r="B62" t="n">
-        <v>5</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> stock-based compensation expense</t>
-        </is>
-      </c>
-      <c r="D62" s="3" t="n">
-        <v>15086</v>
-      </c>
-      <c r="E62" s="3" t="n">
-        <v>10077</v>
-      </c>
-      <c r="F62" s="3" t="n">
-        <v>10703</v>
-      </c>
+      <c r="D62" s="3" t="n"/>
+      <c r="E62" s="3" t="n"/>
+      <c r="F62" s="3" t="n"/>
       <c r="G62" s="3" t="n"/>
       <c r="H62" s="3" t="n"/>
       <c r="I62" s="3" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>3</v>
-      </c>
-      <c r="B63" t="n">
-        <v>6</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
-      </c>
-      <c r="D63" s="3" t="n">
-        <v>-2057</v>
-      </c>
-      <c r="E63" s="3" t="n">
-        <v>-3089</v>
-      </c>
-      <c r="F63" s="3" t="n">
-        <v>-8100</v>
-      </c>
+      <c r="D63" s="3" t="n"/>
+      <c r="E63" s="3" t="n"/>
+      <c r="F63" s="3" t="n"/>
       <c r="G63" s="3" t="n"/>
       <c r="H63" s="3" t="n"/>
       <c r="I63" s="3" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>3</v>
-      </c>
-      <c r="B64" t="n">
-        <v>7</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred income taxes</t>
-        </is>
-      </c>
-      <c r="D64" s="3" t="n">
-        <v>-10991</v>
-      </c>
-      <c r="E64" s="3" t="n">
-        <v>10459</v>
-      </c>
-      <c r="F64" s="3" t="n">
-        <v>10356</v>
-      </c>
+      <c r="D64" s="3" t="n"/>
+      <c r="E64" s="3" t="n"/>
+      <c r="F64" s="3" t="n"/>
       <c r="G64" s="3" t="n"/>
       <c r="H64" s="3" t="n"/>
       <c r="I64" s="3" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>3</v>
-      </c>
-      <c r="B65" t="n">
-        <v>8</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> refranchising loss</t>
-        </is>
-      </c>
-      <c r="D65" s="3" t="n">
-        <v>12942</v>
-      </c>
+      <c r="D65" s="3" t="n"/>
       <c r="E65" s="3" t="n"/>
       <c r="F65" s="3" t="n"/>
       <c r="G65" s="3" t="n"/>
@@ -2026,358 +1518,119 @@
       <c r="I65" s="3" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>3</v>
-      </c>
-      <c r="B66" t="n">
-        <v>9</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other</t>
-        </is>
-      </c>
-      <c r="D66" s="3" t="n">
-        <v>3505</v>
-      </c>
-      <c r="E66" s="3" t="n">
-        <v>4617</v>
-      </c>
-      <c r="F66" s="3" t="n">
-        <v>6353</v>
-      </c>
+      <c r="D66" s="3" t="n"/>
+      <c r="E66" s="3" t="n"/>
+      <c r="F66" s="3" t="n"/>
       <c r="G66" s="3" t="n"/>
       <c r="H66" s="3" t="n"/>
       <c r="I66" s="3" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>3</v>
-      </c>
-      <c r="B67" t="n">
-        <v>12</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> trade and other accounts receivable net</t>
-        </is>
-      </c>
-      <c r="D67" s="3" t="n">
-        <v>-3605</v>
-      </c>
-      <c r="E67" s="3" t="n">
-        <v>-22139</v>
-      </c>
-      <c r="F67" s="3" t="n">
-        <v>3021</v>
-      </c>
+      <c r="D67" s="3" t="n"/>
+      <c r="E67" s="3" t="n"/>
+      <c r="F67" s="3" t="n"/>
       <c r="G67" s="3" t="n"/>
       <c r="H67" s="3" t="n"/>
       <c r="I67" s="3" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>3</v>
-      </c>
-      <c r="B68" t="n">
-        <v>13</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> inventories</t>
-        </is>
-      </c>
-      <c r="D68" s="3" t="n">
-        <v>-1698</v>
-      </c>
-      <c r="E68" s="3" t="n">
-        <v>-895</v>
-      </c>
-      <c r="F68" s="3" t="n">
-        <v>-2186</v>
-      </c>
+      <c r="D68" s="3" t="n"/>
+      <c r="E68" s="3" t="n"/>
+      <c r="F68" s="3" t="n"/>
       <c r="G68" s="3" t="n"/>
       <c r="H68" s="3" t="n"/>
       <c r="I68" s="3" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>3</v>
-      </c>
-      <c r="B69" t="n">
-        <v>14</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> prepaid and other</t>
-        </is>
-      </c>
-      <c r="D69" s="3" t="n">
-        <v>-7191</v>
-      </c>
-      <c r="E69" s="3" t="n">
-        <v>-8524</v>
-      </c>
-      <c r="F69" s="3" t="n">
-        <v>-841</v>
-      </c>
+      <c r="D69" s="3" t="n"/>
+      <c r="E69" s="3" t="n"/>
+      <c r="F69" s="3" t="n"/>
       <c r="G69" s="3" t="n"/>
       <c r="H69" s="3" t="n"/>
       <c r="I69" s="3" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>3</v>
-      </c>
-      <c r="B70" t="n">
-        <v>16</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deposits and other</t>
-        </is>
-      </c>
-      <c r="D70" s="3" t="n">
-        <v>-455</v>
-      </c>
-      <c r="E70" s="3" t="n">
-        <v>239</v>
-      </c>
-      <c r="F70" s="3" t="n">
-        <v>1449</v>
-      </c>
+      <c r="D70" s="3" t="n"/>
+      <c r="E70" s="3" t="n"/>
+      <c r="F70" s="3" t="n"/>
       <c r="G70" s="3" t="n"/>
       <c r="H70" s="3" t="n"/>
       <c r="I70" s="3" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>3</v>
-      </c>
-      <c r="B71" t="n">
-        <v>17</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accounts payable</t>
-        </is>
-      </c>
-      <c r="D71" s="3" t="n">
-        <v>-183</v>
-      </c>
-      <c r="E71" s="3" t="n">
-        <v>1978</v>
-      </c>
-      <c r="F71" s="3" t="n">
-        <v>8162</v>
-      </c>
+      <c r="D71" s="3" t="n"/>
+      <c r="E71" s="3" t="n"/>
+      <c r="F71" s="3" t="n"/>
       <c r="G71" s="3" t="n"/>
       <c r="H71" s="3" t="n"/>
       <c r="I71" s="3" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>3</v>
-      </c>
-      <c r="B72" t="n">
-        <v>18</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accrued</t>
-        </is>
-      </c>
-      <c r="D72" s="3" t="n">
-        <v>31169</v>
-      </c>
-      <c r="E72" s="3" t="n">
-        <v>35288</v>
-      </c>
-      <c r="F72" s="3" t="n">
-        <v>13372</v>
-      </c>
+      <c r="D72" s="3" t="n"/>
+      <c r="E72" s="3" t="n"/>
+      <c r="F72" s="3" t="n"/>
       <c r="G72" s="3" t="n"/>
       <c r="H72" s="3" t="n"/>
       <c r="I72" s="3" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>3</v>
-      </c>
-      <c r="B73" t="n">
-        <v>20</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred rent</t>
-        </is>
-      </c>
-      <c r="D73" s="3" t="n">
-        <v>3751</v>
-      </c>
-      <c r="E73" s="3" t="n">
-        <v>1067</v>
-      </c>
-      <c r="F73" s="3" t="n">
-        <v>5868</v>
-      </c>
+      <c r="D73" s="3" t="n"/>
+      <c r="E73" s="3" t="n"/>
+      <c r="F73" s="3" t="n"/>
       <c r="G73" s="3" t="n"/>
       <c r="H73" s="3" t="n"/>
       <c r="I73" s="3" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>3</v>
-      </c>
-      <c r="B74" t="n">
-        <v>21</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
-        </is>
-      </c>
-      <c r="D74" s="3" t="n">
-        <v>-6951</v>
-      </c>
-      <c r="E74" s="3" t="n">
-        <v>2599</v>
-      </c>
-      <c r="F74" s="3" t="n">
-        <v>-2432</v>
-      </c>
+      <c r="D74" s="3" t="n"/>
+      <c r="E74" s="3" t="n"/>
+      <c r="F74" s="3" t="n"/>
       <c r="G74" s="3" t="n"/>
       <c r="H74" s="3" t="n"/>
       <c r="I74" s="3" t="n"/>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>3</v>
-      </c>
-      <c r="B75" t="n">
-        <v>22</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash provided by operating activities</t>
-        </is>
-      </c>
-      <c r="D75" s="3" t="n">
-        <v>318045</v>
-      </c>
-      <c r="E75" s="3" t="n">
-        <v>335079</v>
-      </c>
-      <c r="F75" s="3" t="n">
-        <v>348417</v>
-      </c>
+      <c r="D75" s="3" t="n"/>
+      <c r="E75" s="3" t="n"/>
+      <c r="F75" s="3" t="n"/>
       <c r="G75" s="3" t="n"/>
       <c r="H75" s="3" t="n"/>
       <c r="I75" s="3" t="n"/>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>3</v>
-      </c>
-      <c r="B76" t="n">
-        <v>24</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> additions to property and equipment</t>
-        </is>
-      </c>
-      <c r="D76" s="3" t="n">
-        <v>-223932</v>
-      </c>
-      <c r="E76" s="3" t="n">
-        <v>-224217</v>
-      </c>
-      <c r="F76" s="3" t="n">
-        <v>-192010</v>
-      </c>
+      <c r="D76" s="3" t="n"/>
+      <c r="E76" s="3" t="n"/>
+      <c r="F76" s="3" t="n"/>
       <c r="G76" s="3" t="n"/>
       <c r="H76" s="3" t="n"/>
       <c r="I76" s="3" t="n"/>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>3</v>
-      </c>
-      <c r="B77" t="n">
-        <v>25</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> acquisitions net of cash acquired</t>
-        </is>
-      </c>
       <c r="D77" s="3" t="n"/>
       <c r="E77" s="3" t="n"/>
-      <c r="F77" s="3" t="n">
-        <v>-2446</v>
-      </c>
+      <c r="F77" s="3" t="n"/>
       <c r="G77" s="3" t="n"/>
       <c r="H77" s="3" t="n"/>
       <c r="I77" s="3" t="n"/>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>3</v>
-      </c>
-      <c r="B78" t="n">
-        <v>26</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> purchase of investments</t>
-        </is>
-      </c>
       <c r="D78" s="3" t="n"/>
       <c r="E78" s="3" t="n"/>
-      <c r="F78" s="3" t="n">
-        <v>-97919</v>
-      </c>
+      <c r="F78" s="3" t="n"/>
       <c r="G78" s="3" t="n"/>
       <c r="H78" s="3" t="n"/>
       <c r="I78" s="3" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" t="n">
-        <v>3</v>
-      </c>
-      <c r="B79" t="n">
-        <v>27</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale of investments</t>
-        </is>
-      </c>
       <c r="D79" s="3" t="n"/>
       <c r="E79" s="3" t="n"/>
-      <c r="F79" s="3" t="n">
-        <v>97936</v>
-      </c>
+      <c r="F79" s="3" t="n"/>
       <c r="G79" s="3" t="n"/>
       <c r="H79" s="3" t="n"/>
       <c r="I79" s="3" t="n"/>
     </row>
     <row r="80">
-      <c r="A80" t="n">
-        <v>3</v>
-      </c>
-      <c r="B80" t="n">
-        <v>28</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from refranchising</t>
-        </is>
-      </c>
-      <c r="D80" s="3" t="n">
-        <v>46869</v>
-      </c>
+      <c r="D80" s="3" t="n"/>
       <c r="E80" s="3" t="n"/>
       <c r="F80" s="3" t="n"/>
       <c r="G80" s="3" t="n"/>
@@ -2385,20 +1638,7 @@
       <c r="I80" s="3" t="n"/>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>3</v>
-      </c>
-      <c r="B81" t="n">
-        <v>29</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale of property and equipment</t>
-        </is>
-      </c>
-      <c r="D81" s="3" t="n">
-        <v>1553</v>
-      </c>
+      <c r="D81" s="3" t="n"/>
       <c r="E81" s="3" t="n"/>
       <c r="F81" s="3" t="n"/>
       <c r="G81" s="3" t="n"/>
@@ -2406,93 +1646,31 @@
       <c r="I81" s="3" t="n"/>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>3</v>
-      </c>
-      <c r="B82" t="n">
-        <v>30</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale-leaseback transactions</t>
-        </is>
-      </c>
-      <c r="D82" s="3" t="n">
-        <v>10095</v>
-      </c>
-      <c r="E82" s="3" t="n">
-        <v>12900</v>
-      </c>
-      <c r="F82" s="3" t="n">
-        <v>6132</v>
-      </c>
+      <c r="D82" s="3" t="n"/>
+      <c r="E82" s="3" t="n"/>
+      <c r="F82" s="3" t="n"/>
       <c r="G82" s="3" t="n"/>
       <c r="H82" s="3" t="n"/>
       <c r="I82" s="3" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>3</v>
-      </c>
-      <c r="B83" t="n">
-        <v>31</v>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash used in investing activities</t>
-        </is>
-      </c>
-      <c r="D83" s="3" t="n">
-        <v>-165415</v>
-      </c>
-      <c r="E83" s="3" t="n">
-        <v>-211317</v>
-      </c>
-      <c r="F83" s="3" t="n">
-        <v>-188307</v>
-      </c>
+      <c r="D83" s="3" t="n"/>
+      <c r="E83" s="3" t="n"/>
+      <c r="F83" s="3" t="n"/>
       <c r="G83" s="3" t="n"/>
       <c r="H83" s="3" t="n"/>
       <c r="I83" s="3" t="n"/>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>3</v>
-      </c>
-      <c r="B84" t="n">
-        <v>33</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from issuance of long-term debt</t>
-        </is>
-      </c>
-      <c r="D84" s="3" t="n">
-        <v>299070</v>
-      </c>
-      <c r="E84" s="3" t="n">
-        <v>100000</v>
-      </c>
+      <c r="D84" s="3" t="n"/>
+      <c r="E84" s="3" t="n"/>
       <c r="F84" s="3" t="n"/>
       <c r="G84" s="3" t="n"/>
       <c r="H84" s="3" t="n"/>
       <c r="I84" s="3" t="n"/>
     </row>
     <row r="85">
-      <c r="A85" t="n">
-        <v>3</v>
-      </c>
-      <c r="B85" t="n">
-        <v>34</v>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> repayments of long-term debt</t>
-        </is>
-      </c>
-      <c r="D85" s="3" t="n">
-        <v>-6301</v>
-      </c>
+      <c r="D85" s="3" t="n"/>
       <c r="E85" s="3" t="n"/>
       <c r="F85" s="3" t="n"/>
       <c r="G85" s="3" t="n"/>
@@ -2500,247 +1678,81 @@
       <c r="I85" s="3" t="n"/>
     </row>
     <row r="86">
-      <c r="A86" t="n">
-        <v>3</v>
-      </c>
-      <c r="B86" t="n">
-        <v>35</v>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> capitalized debt issuance costs</t>
-        </is>
-      </c>
-      <c r="D86" s="3" t="n">
-        <v>-363</v>
-      </c>
-      <c r="E86" s="3" t="n">
-        <v>-193</v>
-      </c>
+      <c r="D86" s="3" t="n"/>
+      <c r="E86" s="3" t="n"/>
       <c r="F86" s="3" t="n"/>
       <c r="G86" s="3" t="n"/>
       <c r="H86" s="3" t="n"/>
       <c r="I86" s="3" t="n"/>
     </row>
     <row r="87">
-      <c r="A87" t="n">
-        <v>3</v>
-      </c>
-      <c r="B87" t="n">
-        <v>36</v>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> payment of deferred acquisition holdback</t>
-        </is>
-      </c>
       <c r="D87" s="3" t="n"/>
-      <c r="E87" s="3" t="n">
-        <v>-270</v>
-      </c>
-      <c r="F87" s="3" t="n">
-        <v>-4112</v>
-      </c>
+      <c r="E87" s="3" t="n"/>
+      <c r="F87" s="3" t="n"/>
       <c r="G87" s="3" t="n"/>
       <c r="H87" s="3" t="n"/>
       <c r="I87" s="3" t="n"/>
     </row>
     <row r="88">
-      <c r="A88" t="n">
-        <v>3</v>
-      </c>
-      <c r="B88" t="n">
-        <v>37</v>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> repurchase of stock</t>
-        </is>
-      </c>
-      <c r="D88" s="3" t="n">
-        <v>-405513</v>
-      </c>
-      <c r="E88" s="3" t="n">
-        <v>-159503</v>
-      </c>
-      <c r="F88" s="3" t="n">
-        <v>-339409</v>
-      </c>
+      <c r="D88" s="3" t="n"/>
+      <c r="E88" s="3" t="n"/>
+      <c r="F88" s="3" t="n"/>
       <c r="G88" s="3" t="n"/>
       <c r="H88" s="3" t="n"/>
       <c r="I88" s="3" t="n"/>
     </row>
     <row r="89">
-      <c r="A89" t="n">
-        <v>3</v>
-      </c>
-      <c r="B89" t="n">
-        <v>39</v>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> exercise of employee stock options</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="n">
-        <v>288</v>
-      </c>
-      <c r="E89" s="3" t="n">
-        <v>1116</v>
-      </c>
-      <c r="F89" s="3" t="n">
-        <v>573</v>
-      </c>
+      <c r="D89" s="3" t="n"/>
+      <c r="E89" s="3" t="n"/>
+      <c r="F89" s="3" t="n"/>
       <c r="G89" s="3" t="n"/>
       <c r="H89" s="3" t="n"/>
       <c r="I89" s="3" t="n"/>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>3</v>
-      </c>
-      <c r="B90" t="n">
-        <v>40</v>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
-      </c>
-      <c r="D90" s="3" t="n">
-        <v>2057</v>
-      </c>
-      <c r="E90" s="3" t="n">
-        <v>3089</v>
-      </c>
-      <c r="F90" s="3" t="n">
-        <v>8100</v>
-      </c>
+      <c r="D90" s="3" t="n"/>
+      <c r="E90" s="3" t="n"/>
+      <c r="F90" s="3" t="n"/>
       <c r="G90" s="3" t="n"/>
       <c r="H90" s="3" t="n"/>
       <c r="I90" s="3" t="n"/>
     </row>
     <row r="91">
-      <c r="A91" t="n">
-        <v>3</v>
-      </c>
-      <c r="B91" t="n">
-        <v>41</v>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from issuance of common stock under employee benefit plans</t>
-        </is>
-      </c>
-      <c r="D91" s="3" t="n">
-        <v>3525</v>
-      </c>
-      <c r="E91" s="3" t="n">
-        <v>3247</v>
-      </c>
-      <c r="F91" s="3" t="n">
-        <v>2842</v>
-      </c>
+      <c r="D91" s="3" t="n"/>
+      <c r="E91" s="3" t="n"/>
+      <c r="F91" s="3" t="n"/>
       <c r="G91" s="3" t="n"/>
       <c r="H91" s="3" t="n"/>
       <c r="I91" s="3" t="n"/>
     </row>
     <row r="92">
-      <c r="A92" t="n">
-        <v>3</v>
-      </c>
-      <c r="B92" t="n">
-        <v>42</v>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash used in financing activities</t>
-        </is>
-      </c>
-      <c r="D92" s="3" t="n">
-        <v>-107237</v>
-      </c>
-      <c r="E92" s="3" t="n">
-        <v>-52514</v>
-      </c>
-      <c r="F92" s="3" t="n">
-        <v>-332006</v>
-      </c>
+      <c r="D92" s="3" t="n"/>
+      <c r="E92" s="3" t="n"/>
+      <c r="F92" s="3" t="n"/>
       <c r="G92" s="3" t="n"/>
       <c r="H92" s="3" t="n"/>
       <c r="I92" s="3" t="n"/>
     </row>
     <row r="93">
-      <c r="A93" t="n">
-        <v>3</v>
-      </c>
-      <c r="B93" t="n">
-        <v>43</v>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net increase (decrease) in cash and cash equivalents</t>
-        </is>
-      </c>
-      <c r="D93" s="3" t="n">
-        <v>45393</v>
-      </c>
-      <c r="E93" s="3" t="n">
-        <v>71248</v>
-      </c>
-      <c r="F93" s="3" t="n">
-        <v>-171896</v>
-      </c>
+      <c r="D93" s="3" t="n"/>
+      <c r="E93" s="3" t="n"/>
+      <c r="F93" s="3" t="n"/>
       <c r="G93" s="3" t="n"/>
       <c r="H93" s="3" t="n"/>
       <c r="I93" s="3" t="n"/>
     </row>
     <row r="94">
-      <c r="A94" t="n">
-        <v>3</v>
-      </c>
-      <c r="B94" t="n">
-        <v>44</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cash and cash equivalents at beginning of period</t>
-        </is>
-      </c>
-      <c r="D94" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="E94" s="3" t="n">
-        <v>125245</v>
-      </c>
-      <c r="F94" s="3" t="n">
-        <v>297141</v>
-      </c>
+      <c r="D94" s="3" t="n"/>
+      <c r="E94" s="3" t="n"/>
+      <c r="F94" s="3" t="n"/>
       <c r="G94" s="3" t="n"/>
       <c r="H94" s="3" t="n"/>
       <c r="I94" s="3" t="n"/>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>3</v>
-      </c>
-      <c r="B95" t="n">
-        <v>45</v>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cash and cash equivalents at end of 1he period accompanying notes are an integral part of the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D95" s="3" t="n">
-        <v>241886</v>
-      </c>
-      <c r="E95" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="F95" s="3" t="n">
-        <v>125245</v>
-      </c>
+      <c r="D95" s="3" t="n"/>
+      <c r="E95" s="3" t="n"/>
+      <c r="F95" s="3" t="n"/>
       <c r="G95" s="3" t="n"/>
       <c r="H95" s="3" t="n"/>
       <c r="I95" s="3" t="n"/>

</xml_diff>

<commit_message>
mostly fixed the column thing
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -490,15 +490,19 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>december 31. 2020</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>december 31. 2020:1</t>
+          <t>December 2019</t>
         </is>
       </c>
-      <c r="F1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2018</t>
+        </is>
+      </c>
       <c r="G1" s="1" t="n"/>
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
@@ -508,20 +512,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents</t>
+          <t xml:space="preserve"> net income (loss)</t>
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>384344</v>
+        <v>862</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>27872</v>
-      </c>
-      <c r="F2" s="3" t="n"/>
+        <v>-775</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>-1063</v>
+      </c>
       <c r="G2" s="3" t="n"/>
       <c r="H2" s="3" t="n"/>
       <c r="I2" s="3" t="n"/>
@@ -531,20 +537,22 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> and respectively</t>
+          <t xml:space="preserve"> depreciation amortization and impairment</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>176617</v>
+        <v>2322</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>148855</v>
-      </c>
-      <c r="F3" s="3" t="n"/>
+        <v>2154</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>1901</v>
+      </c>
       <c r="G3" s="3" t="n"/>
       <c r="H3" s="3" t="n"/>
       <c r="I3" s="3" t="n"/>
@@ -554,20 +562,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> prepaid and other</t>
+          <t xml:space="preserve"> stock-based compensation</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>63224</v>
+        <v>1734</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>52161</v>
-      </c>
-      <c r="F4" s="3" t="n"/>
+        <v>898</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>749</v>
+      </c>
       <c r="G4" s="3" t="n"/>
       <c r="H4" s="3" t="n"/>
       <c r="I4" s="3" t="n"/>
@@ -577,20 +587,22 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current assets</t>
+          <t xml:space="preserve"> amortization of debt discounts and issuance costs</t>
         </is>
       </c>
       <c r="D5" s="3" t="n">
-        <v>624185</v>
+        <v>180</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>228888</v>
-      </c>
-      <c r="F5" s="3" t="n"/>
+        <v>188</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>159</v>
+      </c>
       <c r="G5" s="3" t="n"/>
       <c r="H5" s="3" t="n"/>
       <c r="I5" s="3" t="n"/>
@@ -600,20 +612,22 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> fixed assets net</t>
+          <t xml:space="preserve"> inventory and purchase commitments write-downs</t>
         </is>
       </c>
       <c r="D6" s="3" t="n">
-        <v>628757</v>
+        <v>202</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>636153</v>
-      </c>
-      <c r="F6" s="3" t="n"/>
+        <v>193</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>85</v>
+      </c>
       <c r="G6" s="3" t="n"/>
       <c r="H6" s="3" t="n"/>
       <c r="I6" s="3" t="n"/>
@@ -623,20 +637,22 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> goodwill</t>
+          <t xml:space="preserve"> loss on disposals of fixed assets</t>
         </is>
       </c>
       <c r="D7" s="3" t="n">
-        <v>1431967</v>
+        <v>117</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>1412873</v>
-      </c>
-      <c r="F7" s="3" t="n"/>
+        <v>146</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>162</v>
+      </c>
       <c r="G7" s="3" t="n"/>
       <c r="H7" s="3" t="n"/>
       <c r="I7" s="3" t="n"/>
@@ -646,20 +662,22 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other intangible asse*s net</t>
+          <t xml:space="preserve"> currency net</t>
         </is>
       </c>
       <c r="D8" s="3" t="n">
-        <v>274620</v>
+        <v>114</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>304673</v>
-      </c>
-      <c r="F8" s="3" t="n"/>
+        <v>-48</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>-2</v>
+      </c>
       <c r="G8" s="3" t="n"/>
       <c r="H8" s="3" t="n"/>
       <c r="I8" s="3" t="n"/>
@@ -669,20 +687,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> operating lease right-of-use assets</t>
+          <t xml:space="preserve"> non-cash interest and other operating activities</t>
         </is>
       </c>
       <c r="D9" s="3" t="n">
-        <v>717821</v>
+        <v>228</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>700956</v>
-      </c>
-      <c r="F9" s="3" t="n"/>
+        <v>186</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>49</v>
+      </c>
       <c r="G9" s="3" t="n"/>
       <c r="H9" s="3" t="n"/>
       <c r="I9" s="3" t="n"/>
@@ -692,18 +712,16 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other assets</t>
+          <t xml:space="preserve"> operating cash flow related to repayment of discounted convertible senior notes</t>
         </is>
       </c>
-      <c r="D10" s="3" t="n">
-        <v>49298</v>
-      </c>
+      <c r="D10" s="3" t="n"/>
       <c r="E10" s="3" t="n">
-        <v>46877</v>
+        <v>-188</v>
       </c>
       <c r="F10" s="3" t="n"/>
       <c r="G10" s="3" t="n"/>
@@ -719,16 +737,18 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total assets</t>
+          <t xml:space="preserve"> accounts receivable</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>3726648</v>
+        <v>-652</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>3330420</v>
-      </c>
-      <c r="F11" s="3" t="n"/>
+        <v>-367</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>-497</v>
+      </c>
       <c r="G11" s="3" t="n"/>
       <c r="H11" s="3" t="n"/>
       <c r="I11" s="3" t="n"/>
@@ -738,20 +758,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> current portion of long-term debt</t>
+          <t xml:space="preserve"> inventory</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>10750</v>
+        <v>-422</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>10750</v>
-      </c>
-      <c r="F12" s="3" t="n"/>
+        <v>-429</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>-1023</v>
+      </c>
       <c r="G12" s="3" t="n"/>
       <c r="H12" s="3" t="n"/>
       <c r="I12" s="3" t="n"/>
@@ -761,20 +783,22 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable and accrued expenses</t>
+          <t xml:space="preserve"> operating lease vehicles</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>194551</v>
+        <v>-1072</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>167059</v>
-      </c>
-      <c r="F13" s="3" t="n"/>
+        <v>-764</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>-215</v>
+      </c>
       <c r="G13" s="3" t="n"/>
       <c r="H13" s="3" t="n"/>
       <c r="I13" s="3" t="n"/>
@@ -784,20 +808,22 @@
         <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> current portion of operating lease liabilities</t>
+          <t xml:space="preserve"> expenses current assets</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>87181</v>
+        <v>-251</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>83123</v>
-      </c>
-      <c r="F14" s="3" t="n"/>
+        <v>-288</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>-82</v>
+      </c>
       <c r="G14" s="3" t="n"/>
       <c r="H14" s="3" t="n"/>
       <c r="I14" s="3" t="n"/>
@@ -807,20 +833,22 @@
         <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred</t>
+          <t xml:space="preserve"> other non-current assets</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>197939</v>
+        <v>-344</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>191117</v>
-      </c>
-      <c r="F15" s="3" t="n"/>
+        <v>115</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>-207</v>
+      </c>
       <c r="G15" s="3" t="n"/>
       <c r="H15" s="3" t="n"/>
       <c r="I15" s="3" t="n"/>
@@ -830,20 +858,22 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other current liabilities</t>
+          <t xml:space="preserve"> accounts payable and accrued liabilities</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>40393</v>
+        <v>2102</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>31241</v>
-      </c>
-      <c r="F16" s="3" t="n"/>
+        <v>646</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>1797</v>
+      </c>
       <c r="G16" s="3" t="n"/>
       <c r="H16" s="3" t="n"/>
       <c r="I16" s="3" t="n"/>
@@ -853,20 +883,22 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current liabilities</t>
+          <t xml:space="preserve"> deferred revenue</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>530814</v>
+        <v>321</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>483290</v>
-      </c>
-      <c r="F17" s="3" t="n"/>
+        <v>801</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>406</v>
+      </c>
       <c r="G17" s="3" t="n"/>
       <c r="H17" s="3" t="n"/>
       <c r="I17" s="3" t="n"/>
@@ -876,20 +908,22 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> long-iciu debt net</t>
+          <t xml:space="preserve"> customer deposits</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>1020137</v>
+        <v>7</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>1028049</v>
-      </c>
-      <c r="F18" s="3" t="n"/>
+        <v>-58</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>-96</v>
+      </c>
       <c r="G18" s="3" t="n"/>
       <c r="H18" s="3" t="n"/>
       <c r="I18" s="3" t="n"/>
@@ -899,20 +933,22 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> operating lease liabilities</t>
+          <t xml:space="preserve"> other long-term liabilities</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>729754</v>
+        <v>495</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>685910</v>
-      </c>
-      <c r="F19" s="3" t="n"/>
+        <v>-3</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>-25</v>
+      </c>
       <c r="G19" s="3" t="n"/>
       <c r="H19" s="3" t="n"/>
       <c r="I19" s="3" t="n"/>
@@ -922,20 +958,22 @@
         <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
+          <t xml:space="preserve"> net cash provided by operating activities</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
-        <v>105980</v>
+        <v>5943</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>92865</v>
-      </c>
-      <c r="F20" s="3" t="n"/>
+        <v>2405</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>2098</v>
+      </c>
       <c r="G20" s="3" t="n"/>
       <c r="H20" s="3" t="n"/>
       <c r="I20" s="3" t="n"/>
@@ -945,20 +983,22 @@
         <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred</t>
+          <t xml:space="preserve"> purchases of property and equipment excluding finance leases net of sales</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>10215</v>
+        <v>-3157</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>10098</v>
-      </c>
-      <c r="F21" s="3" t="n"/>
+        <v>-1327</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>-2101</v>
+      </c>
       <c r="G21" s="3" t="n"/>
       <c r="H21" s="3" t="n"/>
       <c r="I21" s="3" t="n"/>
@@ -968,20 +1008,22 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred income taxes</t>
+          <t xml:space="preserve"> purchases solar energy systems net sales</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
-        <v>45951</v>
+        <v>-75</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>58940</v>
-      </c>
-      <c r="F22" s="3" t="n"/>
+        <v>-105</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>-218</v>
+      </c>
       <c r="G22" s="3" t="n"/>
       <c r="H22" s="3" t="n"/>
       <c r="I22" s="3" t="n"/>
@@ -991,18 +1033,18 @@
         <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total liabilities</t>
+          <t xml:space="preserve"> receipt of government grants</t>
         </is>
       </c>
       <c r="D23" s="3" t="n">
-        <v>2442851</v>
+        <v>123</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>2359152</v>
+        <v>46</v>
       </c>
       <c r="F23" s="3" t="n"/>
       <c r="G23" s="3" t="n"/>
@@ -1014,18 +1056,18 @@
         <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> issued and outstanding at december and respectively</t>
+          <t xml:space="preserve"> purchase intangible assets as)</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
-        <v>60</v>
+        <v>-10</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>58</v>
+        <v>-5</v>
       </c>
       <c r="F24" s="3" t="n"/>
       <c r="G24" s="3" t="n"/>
@@ -1037,18 +1079,18 @@
         <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> additional paid-in capital</t>
+          <t xml:space="preserve"> business combinations net of cash acquired</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>910304</v>
+        <v>-13</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>648031</v>
+        <v>-45</v>
       </c>
       <c r="F25" s="3" t="n"/>
       <c r="G25" s="3" t="n"/>
@@ -1060,20 +1102,22 @@
         <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accumulated other comprehensive loss</t>
+          <t xml:space="preserve"> net cash used in investing activities</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
-        <v>-27069</v>
+        <v>-3132</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>-50331</v>
-      </c>
-      <c r="F26" s="3" t="n"/>
+        <v>-1436</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>-2337</v>
+      </c>
       <c r="G26" s="3" t="n"/>
       <c r="H26" s="3" t="n"/>
       <c r="I26" s="3" t="n"/>
@@ -1083,18 +1127,18 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> retained earnings</t>
+          <t xml:space="preserve"> proceeds from issuances of common stock in public offerings net of issuance costs</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>400502</v>
+        <v>12269</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>373510</v>
+        <v>848</v>
       </c>
       <c r="F27" s="3" t="n"/>
       <c r="G27" s="3" t="n"/>
@@ -1106,20 +1150,22 @@
         <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total stockholders’ equity</t>
+          <t xml:space="preserve"> proceeds from issuances of convertible and other debt</t>
         </is>
       </c>
       <c r="D28" s="3" t="n">
-        <v>1283797</v>
+        <v>9713</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>971268</v>
-      </c>
-      <c r="F28" s="3" t="n"/>
+        <v>10669</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>6176</v>
+      </c>
       <c r="G28" s="3" t="n"/>
       <c r="H28" s="3" t="n"/>
       <c r="I28" s="3" t="n"/>
@@ -1129,180 +1175,496 @@
         <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total liabilities and stockholders’ equity see accompanying notes to consolidated financial statements.</t>
+          <t xml:space="preserve"> repayments of convertible and other debt</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>3726648</v>
+        <v>-11623</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>3330420</v>
-      </c>
-      <c r="F29" s="3" t="n"/>
+        <v>-9161</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>-5247</v>
+      </c>
       <c r="G29" s="3" t="n"/>
       <c r="H29" s="3" t="n"/>
       <c r="I29" s="3" t="n"/>
     </row>
     <row r="30">
+      <c r="A30" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="n">
+        <v>38</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> repayments of borrowings issued to related parties</t>
+        </is>
+      </c>
       <c r="D30" s="3" t="n"/>
       <c r="E30" s="3" t="n"/>
-      <c r="F30" s="3" t="n"/>
+      <c r="F30" s="3" t="n">
+        <v>-100</v>
+      </c>
       <c r="G30" s="3" t="n"/>
       <c r="H30" s="3" t="n"/>
       <c r="I30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="D31" s="3" t="n"/>
-      <c r="E31" s="3" t="n"/>
-      <c r="F31" s="3" t="n"/>
+      <c r="A31" t="n">
+        <v>1</v>
+      </c>
+      <c r="B31" t="n">
+        <v>39</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> collateralized lease repayments</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>-240</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>-389</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>-559</v>
+      </c>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="3" t="n"/>
       <c r="I31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="D32" s="3" t="n"/>
-      <c r="E32" s="3" t="n"/>
-      <c r="F32" s="3" t="n"/>
+      <c r="A32" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" t="n">
+        <v>40</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from exercises of stock options and other stock issuances</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>417</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>263</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>296</v>
+      </c>
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="3" t="n"/>
       <c r="I32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="D33" s="3" t="n"/>
-      <c r="E33" s="3" t="n"/>
-      <c r="F33" s="3" t="n"/>
+      <c r="A33" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" t="n">
+        <v>42</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> payments on</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>-338</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <v>-321</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>-181</v>
+      </c>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="3" t="n"/>
       <c r="I33" s="3" t="n"/>
     </row>
     <row r="34">
+      <c r="A34" t="n">
+        <v>1</v>
+      </c>
+      <c r="B34" t="n">
+        <v>43</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> debt issuance costs ©) (1s)</t>
+        </is>
+      </c>
       <c r="D34" s="3" t="n"/>
-      <c r="E34" s="3" t="n"/>
+      <c r="E34" s="3" t="n">
+        <v>-37</v>
+      </c>
       <c r="F34" s="3" t="n"/>
       <c r="G34" s="3" t="n"/>
       <c r="H34" s="3" t="n"/>
       <c r="I34" s="3" t="n"/>
     </row>
     <row r="35">
+      <c r="A35" t="n">
+        <v>1</v>
+      </c>
+      <c r="B35" t="n">
+        <v>44</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> purchase of convertible note hedges</t>
+        </is>
+      </c>
       <c r="D35" s="3" t="n"/>
-      <c r="E35" s="3" t="n"/>
+      <c r="E35" s="3" t="n">
+        <v>-476</v>
+      </c>
       <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
       <c r="H35" s="3" t="n"/>
       <c r="I35" s="3" t="n"/>
     </row>
     <row r="36">
+      <c r="A36" t="n">
+        <v>1</v>
+      </c>
+      <c r="B36" t="n">
+        <v>45</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from issuance of warrants</t>
+        </is>
+      </c>
       <c r="D36" s="3" t="n"/>
-      <c r="E36" s="3" t="n"/>
-      <c r="F36" s="3" t="n"/>
+      <c r="E36" s="3" t="n">
+        <v>174</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>437</v>
+      </c>
       <c r="G36" s="3" t="n"/>
       <c r="H36" s="3" t="n"/>
       <c r="I36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="D37" s="3" t="n"/>
-      <c r="E37" s="3" t="n"/>
+      <c r="A37" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" t="n">
+        <v>46</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> proceeds from investments by noncontrolling interests in subsidiaries</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="E37" s="3" t="n">
+        <v>279</v>
+      </c>
       <c r="F37" s="3" t="n"/>
       <c r="G37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="I37" s="3" t="n"/>
     </row>
     <row r="38">
-      <c r="D38" s="3" t="n"/>
+      <c r="A38" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" t="n">
+        <v>47</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> distributions paid to noncontrolling interests in subsidiaries gl)</t>
+        </is>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>-208</v>
+      </c>
       <c r="E38" s="3" t="n"/>
-      <c r="F38" s="3" t="n"/>
+      <c r="F38" s="3" t="n">
+        <v>-227</v>
+      </c>
       <c r="G38" s="3" t="n"/>
       <c r="H38" s="3" t="n"/>
       <c r="I38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="D39" s="3" t="n"/>
-      <c r="E39" s="3" t="n"/>
-      <c r="F39" s="3" t="n"/>
+      <c r="A39" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="n">
+        <v>48</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> payments for buy-outs of noncontrolling interests in subsidiaries</t>
+        </is>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>-35</v>
+      </c>
+      <c r="E39" s="3" t="n">
+        <v>-9</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>-6</v>
+      </c>
       <c r="G39" s="3" t="n"/>
       <c r="H39" s="3" t="n"/>
       <c r="I39" s="3" t="n"/>
     </row>
     <row r="40">
-      <c r="D40" s="3" t="n"/>
-      <c r="E40" s="3" t="n"/>
-      <c r="F40" s="3" t="n"/>
+      <c r="A40" t="n">
+        <v>1</v>
+      </c>
+      <c r="B40" t="n">
+        <v>49</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net cash provided by financing activities</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="n">
+        <v>9973</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <v>1529</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <v>574</v>
+      </c>
       <c r="G40" s="3" t="n"/>
       <c r="H40" s="3" t="n"/>
       <c r="I40" s="3" t="n"/>
     </row>
     <row r="41">
-      <c r="D41" s="3" t="n"/>
-      <c r="E41" s="3" t="n"/>
-      <c r="F41" s="3" t="n"/>
+      <c r="A41" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" t="n">
+        <v>50</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> effect of exchange rate changes on cash and cash equivalents and restricted cash</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="n">
+        <v>334</v>
+      </c>
+      <c r="E41" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F41" s="3" t="n">
+        <v>-23</v>
+      </c>
       <c r="G41" s="3" t="n"/>
       <c r="H41" s="3" t="n"/>
       <c r="I41" s="3" t="n"/>
     </row>
     <row r="42">
-      <c r="D42" s="3" t="n"/>
-      <c r="E42" s="3" t="n"/>
-      <c r="F42" s="3" t="n"/>
+      <c r="A42" t="n">
+        <v>1</v>
+      </c>
+      <c r="B42" t="n">
+        <v>51</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> net increase in cash and cash equivalents and restricted cash</t>
+        </is>
+      </c>
+      <c r="D42" s="3" t="n">
+        <v>13118</v>
+      </c>
+      <c r="E42" s="3" t="n">
+        <v>2506</v>
+      </c>
+      <c r="F42" s="3" t="n">
+        <v>312</v>
+      </c>
       <c r="G42" s="3" t="n"/>
       <c r="H42" s="3" t="n"/>
       <c r="I42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="D43" s="3" t="n"/>
-      <c r="E43" s="3" t="n"/>
-      <c r="F43" s="3" t="n"/>
+      <c r="A43" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" t="n">
+        <v>52</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cash and cash equivalents and restricted cash beginning of period</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="n">
+        <v>6783</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>4277</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>3965</v>
+      </c>
       <c r="G43" s="3" t="n"/>
       <c r="H43" s="3" t="n"/>
       <c r="I43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="D44" s="3" t="n"/>
-      <c r="E44" s="3" t="n"/>
-      <c r="F44" s="3" t="n"/>
+      <c r="A44" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" t="n">
+        <v>53</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cash and cash equivalents and restricted cash end of period</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="n">
+        <v>19901</v>
+      </c>
+      <c r="E44" s="3" t="n">
+        <v>6783</v>
+      </c>
+      <c r="F44" s="3" t="n">
+        <v>4277</v>
+      </c>
       <c r="G44" s="3" t="n"/>
       <c r="H44" s="3" t="n"/>
       <c r="I44" s="3" t="n"/>
     </row>
     <row r="45">
+      <c r="A45" t="n">
+        <v>1</v>
+      </c>
+      <c r="B45" t="n">
+        <v>55</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> equity issued in connection with business combination</t>
+        </is>
+      </c>
       <c r="D45" s="3" t="n"/>
-      <c r="E45" s="3" t="n"/>
+      <c r="E45" s="3" t="n">
+        <v>207</v>
+      </c>
       <c r="F45" s="3" t="n"/>
       <c r="G45" s="3" t="n"/>
       <c r="H45" s="3" t="n"/>
       <c r="I45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="D46" s="3" t="n"/>
-      <c r="E46" s="3" t="n"/>
-      <c r="F46" s="3" t="n"/>
+      <c r="A46" t="n">
+        <v>1</v>
+      </c>
+      <c r="B46" t="n">
+        <v>56</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> acquisitions of property and equipment included in liabilities</t>
+        </is>
+      </c>
+      <c r="D46" s="3" t="n">
+        <v>1088</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <v>562</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <v>249</v>
+      </c>
       <c r="G46" s="3" t="n"/>
       <c r="H46" s="3" t="n"/>
       <c r="I46" s="3" t="n"/>
     </row>
     <row r="47">
+      <c r="A47" t="n">
+        <v>1</v>
+      </c>
+      <c r="B47" t="n">
+        <v>57</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> estimated fair value of facilities under build-to-suit leases</t>
+        </is>
+      </c>
       <c r="D47" s="3" t="n"/>
       <c r="E47" s="3" t="n"/>
-      <c r="F47" s="3" t="n"/>
+      <c r="F47" s="3" t="n">
+        <v>94</v>
+      </c>
       <c r="G47" s="3" t="n"/>
       <c r="H47" s="3" t="n"/>
       <c r="I47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="D48" s="3" t="n"/>
-      <c r="E48" s="3" t="n"/>
-      <c r="F48" s="3" t="n"/>
+      <c r="A48" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" t="n">
+        <v>59</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cash paid during the period for interest net of amounts capitalized</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="n">
+        <v>444</v>
+      </c>
+      <c r="E48" s="3" t="n">
+        <v>455</v>
+      </c>
+      <c r="F48" s="3" t="n">
+        <v>381</v>
+      </c>
       <c r="G48" s="3" t="n"/>
       <c r="H48" s="3" t="n"/>
       <c r="I48" s="3" t="n"/>
     </row>
     <row r="49">
-      <c r="D49" s="3" t="n"/>
-      <c r="E49" s="3" t="n"/>
-      <c r="F49" s="3" t="n"/>
+      <c r="A49" t="n">
+        <v>1</v>
+      </c>
+      <c r="B49" t="n">
+        <v>60</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> cash paid during the period for taxes net of the refunds accompanying notes are an integral part of these consolidated financial statements.</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="n">
+        <v>115</v>
+      </c>
+      <c r="E49" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="F49" s="3" t="n">
+        <v>35</v>
+      </c>
       <c r="G49" s="3" t="n"/>
       <c r="H49" s="3" t="n"/>
       <c r="I49" s="3" t="n"/>

</xml_diff>

<commit_message>
made this public and added a readme
</commit_message>
<xml_diff>
--- a/Financial Statement Output.xlsx
+++ b/Financial Statement Output.xlsx
@@ -490,20 +490,24 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>september 30. 2015</t>
+          <t>three months ended september 30. 2021</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>september 30. 2014</t>
+          <t>three months ended september 30. 2020</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>december 31. 2013</t>
+          <t>nine months ended september 30. 2021</t>
         </is>
       </c>
-      <c r="G1" s="1" t="n"/>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>nine months ended september 30. 2020</t>
+        </is>
+      </c>
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
     </row>
@@ -512,21 +516,25 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cash and cash equivalents</t>
+          <t xml:space="preserve"> cash cash equivalents and restricted cash beginning of period</t>
         </is>
       </c>
       <c r="D2" s="3" t="n">
-        <v>241886</v>
+        <v>37842</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
+        <v>40667</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>36410</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>42377</v>
+      </c>
       <c r="H2" s="3" t="n"/>
       <c r="I2" s="3" t="n"/>
     </row>
@@ -539,17 +547,21 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> trade accounts receivable net</t>
+          <t xml:space="preserve"> net income</t>
         </is>
       </c>
       <c r="D3" s="3" t="n">
-        <v>38211</v>
+        <v>6331</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>36584</v>
-      </c>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
+        <v>3156</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>14109</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>19041</v>
+      </c>
       <c r="H3" s="3" t="n"/>
       <c r="I3" s="3" t="n"/>
     </row>
@@ -558,21 +570,25 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other accounts receivable</t>
+          <t xml:space="preserve"> lease assets and other</t>
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>77575</v>
+        <v>6523</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>70069</v>
-      </c>
-      <c r="F4" s="3" t="n"/>
-      <c r="G4" s="3" t="n"/>
+        <v>8948</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>17633</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>24494</v>
+      </c>
       <c r="H4" s="3" t="n"/>
       <c r="I4" s="3" t="n"/>
     </row>
@@ -581,111 +597,133 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> stock-based compensation</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>2288</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>3180</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>6646</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>9077</v>
+      </c>
+      <c r="H5" s="3" t="n"/>
+      <c r="I5" s="3" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> other operating expense (income) net</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>416</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="H6" s="3" t="n"/>
+      <c r="I6" s="3" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> other expense (income) net</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>-1051</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>340</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>-1255</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>-2374</v>
+      </c>
+      <c r="H7" s="3" t="n"/>
+      <c r="I7" s="3" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="n">
+        <v>11</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> deferred income taxes</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>295</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>909</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>1082</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>3313</v>
+      </c>
+      <c r="H8" s="3" t="n"/>
+      <c r="I8" s="3" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="n">
+        <v>13</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve"> inventories</t>
         </is>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>22482</v>
-      </c>
-      <c r="E5" s="3" t="n">
-        <v>22811</v>
-      </c>
-      <c r="F5" s="3" t="n"/>
-      <c r="G5" s="3" t="n"/>
-      <c r="H5" s="3" t="n"/>
-      <c r="I5" s="3" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>7</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> prepaid and other</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>59457</v>
-      </c>
-      <c r="E6" s="3" t="n">
-        <v>51588</v>
-      </c>
-      <c r="F6" s="3" t="n"/>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="n"/>
-      <c r="I6" s="3" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" t="n">
-        <v>9</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> veferred income taxes</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>34479</v>
-      </c>
-      <c r="E7" s="3" t="n">
-        <v>28621</v>
-      </c>
-      <c r="F7" s="3" t="n"/>
-      <c r="G7" s="3" t="n"/>
-      <c r="H7" s="3" t="n"/>
-      <c r="I7" s="3" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> assets held for sale</t>
-        </is>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>28699</v>
-      </c>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="n"/>
-      <c r="G8" s="3" t="n"/>
-      <c r="H8" s="3" t="n"/>
-      <c r="I8" s="3" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="n">
-        <v>11</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total current assets</t>
-        </is>
-      </c>
       <c r="D9" s="3" t="n">
-        <v>502789</v>
+        <v>-3899</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>406166</v>
-      </c>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="n"/>
+        <v>-7059</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>-3178</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>-7572</v>
+      </c>
       <c r="H9" s="3" t="n"/>
       <c r="I9" s="3" t="n"/>
     </row>
@@ -694,21 +732,25 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> property and equipment net</t>
+          <t xml:space="preserve"> accounts receivable net and other</t>
         </is>
       </c>
       <c r="D10" s="3" t="n">
-        <v>776248</v>
+        <v>-2016</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>787294</v>
-      </c>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
+        <v>-4890</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>-3608</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>-11607</v>
+      </c>
       <c r="H10" s="3" t="n"/>
       <c r="I10" s="3" t="n"/>
     </row>
@@ -717,21 +759,25 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> goodwill</t>
+          <t xml:space="preserve"> accounts payable</t>
         </is>
       </c>
       <c r="D11" s="3" t="n">
-        <v>121791</v>
+        <v>3658</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>120778</v>
-      </c>
-      <c r="F11" s="3" t="n"/>
-      <c r="G11" s="3" t="n"/>
+        <v>3832</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>4231</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>-4387</v>
+      </c>
       <c r="H11" s="3" t="n"/>
       <c r="I11" s="3" t="n"/>
     </row>
@@ -740,21 +786,25 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other intangible assets net</t>
+          <t xml:space="preserve"> accrued expenses and other</t>
         </is>
       </c>
       <c r="D12" s="3" t="n">
-        <v>63877</v>
+        <v>-310</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>70940</v>
-      </c>
-      <c r="F12" s="3" t="n"/>
-      <c r="G12" s="3" t="n"/>
+        <v>-1465</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>-1375</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>-7210</v>
+      </c>
       <c r="H12" s="3" t="n"/>
       <c r="I12" s="3" t="n"/>
     </row>
@@ -763,21 +813,25 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deposits and other</t>
+          <t xml:space="preserve"> unearned revenue</t>
         </is>
       </c>
       <c r="D13" s="3" t="n">
-        <v>10613</v>
+        <v>78</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>5508</v>
-      </c>
-      <c r="F13" s="3" t="n"/>
-      <c r="G13" s="3" t="n"/>
+        <v>338</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>932</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>1394</v>
+      </c>
       <c r="H13" s="3" t="n"/>
       <c r="I13" s="3" t="n"/>
     </row>
@@ -786,21 +840,25 @@
         <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total other assets</t>
+          <t xml:space="preserve"> net cash provided by (used in) operating activities</t>
         </is>
       </c>
       <c r="D14" s="3" t="n">
-        <v>196281</v>
+        <v>11964</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>197226</v>
-      </c>
-      <c r="F14" s="3" t="n"/>
-      <c r="G14" s="3" t="n"/>
+        <v>7313</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>35633</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>24241</v>
+      </c>
       <c r="H14" s="3" t="n"/>
       <c r="I14" s="3" t="n"/>
     </row>
@@ -809,21 +867,25 @@
         <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total assets</t>
+          <t xml:space="preserve"> purchases of property and equipment</t>
         </is>
       </c>
       <c r="D15" s="3" t="n">
-        <v>1475318</v>
+        <v>-11063</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>1390686</v>
-      </c>
-      <c r="F15" s="3" t="n"/>
-      <c r="G15" s="3" t="n"/>
+        <v>-15748</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>-25317</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>-42118</v>
+      </c>
       <c r="H15" s="3" t="n"/>
       <c r="I15" s="3" t="n"/>
     </row>
@@ -836,17 +898,21 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accounts payable</t>
+          <t xml:space="preserve"> proceeds from property and equipment sales and incentives</t>
         </is>
       </c>
       <c r="D16" s="3" t="n">
-        <v>19805</v>
+        <v>1255</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>19511</v>
-      </c>
-      <c r="F16" s="3" t="n"/>
-      <c r="G16" s="3" t="n"/>
+        <v>997</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>3467</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>3192</v>
+      </c>
       <c r="H16" s="3" t="n"/>
       <c r="I16" s="3" t="n"/>
     </row>
@@ -859,17 +925,21 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accrued</t>
+          <t xml:space="preserve"> acquisitions net of cash acquired and other</t>
         </is>
       </c>
       <c r="D17" s="3" t="n">
-        <v>359464</v>
+        <v>-1735</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>333201</v>
-      </c>
-      <c r="F17" s="3" t="n"/>
-      <c r="G17" s="3" t="n"/>
+        <v>-654</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>-1945</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>-1604</v>
+      </c>
       <c r="H17" s="3" t="n"/>
       <c r="I17" s="3" t="n"/>
     </row>
@@ -878,19 +948,25 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> cunent portion of long-term debt</t>
+          <t xml:space="preserve"> sales and maturities of marketable securities</t>
         </is>
       </c>
       <c r="D18" s="3" t="n">
-        <v>17229</v>
-      </c>
-      <c r="E18" s="3" t="n"/>
-      <c r="F18" s="3" t="n"/>
-      <c r="G18" s="3" t="n"/>
+        <v>13135</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>15808</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>32899</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>46847</v>
+      </c>
       <c r="H18" s="3" t="n"/>
       <c r="I18" s="3" t="n"/>
     </row>
@@ -899,19 +975,25 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> liabilities associated with assets held for sale</t>
+          <t xml:space="preserve"> purchases of marketable securities</t>
         </is>
       </c>
       <c r="D19" s="3" t="n">
-        <v>2945</v>
-      </c>
-      <c r="E19" s="3" t="n"/>
-      <c r="F19" s="3" t="n"/>
-      <c r="G19" s="3" t="n"/>
+        <v>-17468</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>-15231</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>-51678</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>-51891</v>
+      </c>
       <c r="H19" s="3" t="n"/>
       <c r="I19" s="3" t="n"/>
     </row>
@@ -920,21 +1002,25 @@
         <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total current liabilities</t>
+          <t xml:space="preserve"> net cash provided by (used in) investing activities</t>
         </is>
       </c>
       <c r="D20" s="3" t="n">
-        <v>399443</v>
+        <v>-15876</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>352712</v>
-      </c>
-      <c r="F20" s="3" t="n"/>
-      <c r="G20" s="3" t="n"/>
+        <v>-14828</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>-42574</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>-45574</v>
+      </c>
       <c r="H20" s="3" t="n"/>
       <c r="I20" s="3" t="n"/>
     </row>
@@ -947,17 +1033,21 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> long-term debt</t>
+          <t xml:space="preserve"> proceeds from short-term debt and other</t>
         </is>
       </c>
       <c r="D21" s="3" t="n">
-        <v>388971</v>
+        <v>1311</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>99784</v>
-      </c>
-      <c r="F21" s="3" t="n"/>
-      <c r="G21" s="3" t="n"/>
+        <v>2187</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>4361</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>5289</v>
+      </c>
       <c r="H21" s="3" t="n"/>
       <c r="I21" s="3" t="n"/>
     </row>
@@ -970,17 +1060,21 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred rent</t>
+          <t xml:space="preserve"> repayments of short-wii. debt and other</t>
         </is>
       </c>
       <c r="D22" s="3" t="n">
-        <v>62610</v>
+        <v>-1349</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>67390</v>
-      </c>
-      <c r="F22" s="3" t="n"/>
-      <c r="G22" s="3" t="n"/>
+        <v>-1917</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>-3886</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>-5094</v>
+      </c>
       <c r="H22" s="3" t="n"/>
       <c r="I22" s="3" t="n"/>
     </row>
@@ -993,17 +1087,19 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> deferred income taxes</t>
+          <t xml:space="preserve"> proceeds from long-term debt</t>
         </is>
       </c>
-      <c r="D23" s="3" t="n">
-        <v>70447</v>
-      </c>
+      <c r="D23" s="3" t="n"/>
       <c r="E23" s="3" t="n">
-        <v>76589</v>
-      </c>
-      <c r="F23" s="3" t="n"/>
-      <c r="G23" s="3" t="n"/>
+        <v>176</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>9994</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>18803</v>
+      </c>
       <c r="H23" s="3" t="n"/>
       <c r="I23" s="3" t="n"/>
     </row>
@@ -1016,17 +1112,21 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
+          <t xml:space="preserve"> repayments of long-term debt</t>
         </is>
       </c>
       <c r="D24" s="3" t="n">
-        <v>52566</v>
+        <v>-1198</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>58027</v>
-      </c>
-      <c r="F24" s="3" t="n"/>
-      <c r="G24" s="3" t="n"/>
+        <v>-509</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>-1439</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>-589</v>
+      </c>
       <c r="H24" s="3" t="n"/>
       <c r="I24" s="3" t="n"/>
     </row>
@@ -1039,17 +1139,21 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> total liabilities</t>
+          <t xml:space="preserve"> principal repay...ents of finance leases</t>
         </is>
       </c>
       <c r="D25" s="3" t="n">
-        <v>974037</v>
+        <v>-2857</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>654502</v>
-      </c>
-      <c r="F25" s="3" t="n"/>
-      <c r="G25" s="3" t="n"/>
+        <v>-2693</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>-8274</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>-8903</v>
+      </c>
       <c r="H25" s="3" t="n"/>
       <c r="I25" s="3" t="n"/>
     </row>
@@ -1058,19 +1162,25 @@
         <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> redeemable noncontrolling interest</t>
+          <t xml:space="preserve"> principal repayments of financing obligations</t>
         </is>
       </c>
       <c r="D26" s="3" t="n">
-        <v>3981</v>
-      </c>
-      <c r="E26" s="3" t="n"/>
-      <c r="F26" s="3" t="n"/>
-      <c r="G26" s="3" t="n"/>
+        <v>-12</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>-20</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>-44</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>-115</v>
+      </c>
       <c r="H26" s="3" t="n"/>
       <c r="I26" s="3" t="n"/>
     </row>
@@ -1079,21 +1189,25 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> treasury stock carried at cost; shares at december and shares at</t>
+          <t xml:space="preserve"> net cash provided by (used in) financing activities</t>
         </is>
       </c>
       <c r="D27" s="3" t="n">
-        <v>-1111586</v>
+        <v>-4105</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>-706073</v>
-      </c>
-      <c r="F27" s="3" t="n"/>
-      <c r="G27" s="3" t="n"/>
+        <v>-2776</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>712</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>9391</v>
+      </c>
       <c r="H27" s="3" t="n"/>
       <c r="I27" s="3" t="n"/>
     </row>
@@ -1102,21 +1216,25 @@
         <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> additional paid-in capital</t>
+          <t xml:space="preserve"> foreign currency effect on cash cash equivalents and restricted cash</t>
         </is>
       </c>
       <c r="D28" s="3" t="n">
-        <v>235393</v>
+        <v>377</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>214437</v>
-      </c>
-      <c r="F28" s="3" t="n"/>
-      <c r="G28" s="3" t="n"/>
+        <v>-199</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>-258</v>
+      </c>
       <c r="H28" s="3" t="n"/>
       <c r="I28" s="3" t="n"/>
     </row>
@@ -1125,21 +1243,25 @@
         <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> accumulated other comprehensive income (loss)</t>
+          <t xml:space="preserve"> net increase (decrease) in cash cash equivalents and restricted cash</t>
         </is>
       </c>
       <c r="D29" s="3" t="n">
-        <v>-5029</v>
+        <v>-7640</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>-1360</v>
-      </c>
-      <c r="F29" s="3" t="n"/>
-      <c r="G29" s="3" t="n"/>
+        <v>-10490</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>-6208</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>-12200</v>
+      </c>
       <c r="H29" s="3" t="n"/>
       <c r="I29" s="3" t="n"/>
     </row>
@@ -1148,410 +1270,150 @@
         <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> retained ca:uings</t>
+          <t xml:space="preserve"> cash cash equivalents and res1xicted cash see end accompanying of period notes to consolidated financial statements.</t>
         </is>
       </c>
       <c r="D30" s="3" t="n">
-        <v>1378519</v>
+        <v>30202</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>1229177</v>
-      </c>
-      <c r="F30" s="3" t="n"/>
-      <c r="G30" s="3" t="n"/>
+        <v>30177</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>30202</v>
+      </c>
+      <c r="G30" s="3" t="n">
+        <v>30177</v>
+      </c>
       <c r="H30" s="3" t="n"/>
       <c r="I30" s="3" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" t="n">
-        <v>1</v>
-      </c>
-      <c r="B31" t="n">
-        <v>47</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total stockholders' equity</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="n">
-        <v>497300</v>
-      </c>
-      <c r="E31" s="3" t="n">
-        <v>736184</v>
-      </c>
+      <c r="D31" s="3" t="n"/>
+      <c r="E31" s="3" t="n"/>
       <c r="F31" s="3" t="n"/>
       <c r="G31" s="3" t="n"/>
       <c r="H31" s="3" t="n"/>
       <c r="I31" s="3" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" t="n">
-        <v>1</v>
-      </c>
-      <c r="B32" t="n">
-        <v>48</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total liabilities redeemable the accompanying noncontrolling notes interest are an and integral stockholders' part of equity the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>1475318</v>
-      </c>
-      <c r="E32" s="3" t="n">
-        <v>1390686</v>
-      </c>
+      <c r="D32" s="3" t="n"/>
+      <c r="E32" s="3" t="n"/>
       <c r="F32" s="3" t="n"/>
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="3" t="n"/>
       <c r="I32" s="3" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" t="n">
-        <v>2</v>
-      </c>
-      <c r="B33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> bakery-cafe sales net</t>
-        </is>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>2358794</v>
-      </c>
-      <c r="E33" s="3" t="n">
-        <v>2230370</v>
-      </c>
-      <c r="F33" s="3" t="n">
-        <v>2108908</v>
-      </c>
+      <c r="D33" s="3" t="n"/>
+      <c r="E33" s="3" t="n"/>
+      <c r="F33" s="3" t="n"/>
       <c r="G33" s="3" t="n"/>
       <c r="H33" s="3" t="n"/>
       <c r="I33" s="3" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" t="n">
-        <v>2</v>
-      </c>
-      <c r="B34" t="n">
-        <v>3</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> franchise royalties and fees</t>
-        </is>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>138563</v>
-      </c>
-      <c r="E34" s="3" t="n">
-        <v>123686</v>
-      </c>
-      <c r="F34" s="3" t="n">
-        <v>112641</v>
-      </c>
+      <c r="D34" s="3" t="n"/>
+      <c r="E34" s="3" t="n"/>
+      <c r="F34" s="3" t="n"/>
       <c r="G34" s="3" t="n"/>
       <c r="H34" s="3" t="n"/>
       <c r="I34" s="3" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" t="n">
-        <v>2</v>
-      </c>
-      <c r="B35" t="n">
-        <v>4</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> fresh dough and other product sales to franchisees</t>
-        </is>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>184223</v>
-      </c>
-      <c r="E35" s="3" t="n">
-        <v>175139</v>
-      </c>
-      <c r="F35" s="3" t="n">
-        <v>163453</v>
-      </c>
+      <c r="D35" s="3" t="n"/>
+      <c r="E35" s="3" t="n"/>
+      <c r="F35" s="3" t="n"/>
       <c r="G35" s="3" t="n"/>
       <c r="H35" s="3" t="n"/>
       <c r="I35" s="3" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" t="n">
-        <v>2</v>
-      </c>
-      <c r="B36" t="n">
-        <v>5</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total</t>
-        </is>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>2681580</v>
-      </c>
-      <c r="E36" s="3" t="n">
-        <v>2529195</v>
-      </c>
-      <c r="F36" s="3" t="n">
-        <v>2385002</v>
-      </c>
+      <c r="D36" s="3" t="n"/>
+      <c r="E36" s="3" t="n"/>
+      <c r="F36" s="3" t="n"/>
       <c r="G36" s="3" t="n"/>
       <c r="H36" s="3" t="n"/>
       <c r="I36" s="3" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" t="n">
-        <v>2</v>
-      </c>
-      <c r="B37" t="n">
-        <v>11</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cost of food and paper products</t>
-        </is>
-      </c>
-      <c r="D37" s="3" t="n">
-        <v>715502</v>
-      </c>
-      <c r="E37" s="3" t="n">
-        <v>669860</v>
-      </c>
-      <c r="F37" s="3" t="n">
-        <v>625622</v>
-      </c>
+      <c r="D37" s="3" t="n"/>
+      <c r="E37" s="3" t="n"/>
+      <c r="F37" s="3" t="n"/>
       <c r="G37" s="3" t="n"/>
       <c r="H37" s="3" t="n"/>
       <c r="I37" s="3" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" t="n">
-        <v>2</v>
-      </c>
-      <c r="B38" t="n">
-        <v>12</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> labor</t>
-        </is>
-      </c>
-      <c r="D38" s="3" t="n">
-        <v>754646</v>
-      </c>
-      <c r="E38" s="3" t="n">
-        <v>685576</v>
-      </c>
-      <c r="F38" s="3" t="n">
-        <v>625457</v>
-      </c>
+      <c r="D38" s="3" t="n"/>
+      <c r="E38" s="3" t="n"/>
+      <c r="F38" s="3" t="n"/>
       <c r="G38" s="3" t="n"/>
       <c r="H38" s="3" t="n"/>
       <c r="I38" s="3" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" t="n">
-        <v>2</v>
-      </c>
-      <c r="B39" t="n">
-        <v>13</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> occupancy</t>
-        </is>
-      </c>
-      <c r="D39" s="3" t="n">
-        <v>169998</v>
-      </c>
-      <c r="E39" s="3" t="n">
-        <v>159794</v>
-      </c>
-      <c r="F39" s="3" t="n">
-        <v>148816</v>
-      </c>
+      <c r="D39" s="3" t="n"/>
+      <c r="E39" s="3" t="n"/>
+      <c r="F39" s="3" t="n"/>
       <c r="G39" s="3" t="n"/>
       <c r="H39" s="3" t="n"/>
       <c r="I39" s="3" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" t="n">
-        <v>2</v>
-      </c>
-      <c r="B40" t="n">
-        <v>14</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other operating expenses</t>
-        </is>
-      </c>
-      <c r="D40" s="3" t="n">
-        <v>334635</v>
-      </c>
-      <c r="E40" s="3" t="n">
-        <v>314879</v>
-      </c>
-      <c r="F40" s="3" t="n">
-        <v>295539</v>
-      </c>
+      <c r="D40" s="3" t="n"/>
+      <c r="E40" s="3" t="n"/>
+      <c r="F40" s="3" t="n"/>
       <c r="G40" s="3" t="n"/>
       <c r="H40" s="3" t="n"/>
       <c r="I40" s="3" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" t="n">
-        <v>2</v>
-      </c>
-      <c r="B41" t="n">
-        <v>15</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total bakery-cafe expenses</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="n">
-        <v>1974781</v>
-      </c>
-      <c r="E41" s="3" t="n">
-        <v>1830109</v>
-      </c>
-      <c r="F41" s="3" t="n">
-        <v>1695434</v>
-      </c>
+      <c r="D41" s="3" t="n"/>
+      <c r="E41" s="3" t="n"/>
+      <c r="F41" s="3" t="n"/>
       <c r="G41" s="3" t="n"/>
       <c r="H41" s="3" t="n"/>
       <c r="I41" s="3" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>2</v>
-      </c>
-      <c r="B42" t="n">
-        <v>16</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> fresh dough and other product cost of sales to franchisees</t>
-        </is>
-      </c>
-      <c r="D42" s="3" t="n">
-        <v>160706</v>
-      </c>
-      <c r="E42" s="3" t="n">
-        <v>152267</v>
-      </c>
-      <c r="F42" s="3" t="n">
-        <v>142160</v>
-      </c>
+      <c r="D42" s="3" t="n"/>
+      <c r="E42" s="3" t="n"/>
+      <c r="F42" s="3" t="n"/>
       <c r="G42" s="3" t="n"/>
       <c r="H42" s="3" t="n"/>
       <c r="I42" s="3" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" t="n">
-        <v>2</v>
-      </c>
-      <c r="B43" t="n">
-        <v>17</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
-        </is>
-      </c>
-      <c r="D43" s="3" t="n">
-        <v>135398</v>
-      </c>
-      <c r="E43" s="3" t="n">
-        <v>124109</v>
-      </c>
-      <c r="F43" s="3" t="n">
-        <v>106523</v>
-      </c>
+      <c r="D43" s="3" t="n"/>
+      <c r="E43" s="3" t="n"/>
+      <c r="F43" s="3" t="n"/>
       <c r="G43" s="3" t="n"/>
       <c r="H43" s="3" t="n"/>
       <c r="I43" s="3" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" t="n">
-        <v>2</v>
-      </c>
-      <c r="B44" t="n">
-        <v>18</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> general and administrative expenses</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="n">
-        <v>142904</v>
-      </c>
-      <c r="E44" s="3" t="n">
-        <v>138060</v>
-      </c>
-      <c r="F44" s="3" t="n">
-        <v>123335</v>
-      </c>
+      <c r="D44" s="3" t="n"/>
+      <c r="E44" s="3" t="n"/>
+      <c r="F44" s="3" t="n"/>
       <c r="G44" s="3" t="n"/>
       <c r="H44" s="3" t="n"/>
       <c r="I44" s="3" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" t="n">
-        <v>2</v>
-      </c>
-      <c r="B45" t="n">
-        <v>19</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> pre-opening</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="n">
-        <v>9089</v>
-      </c>
-      <c r="E45" s="3" t="n">
-        <v>8707</v>
-      </c>
-      <c r="F45" s="3" t="n">
-        <v>7794</v>
-      </c>
+      <c r="D45" s="3" t="n"/>
+      <c r="E45" s="3" t="n"/>
+      <c r="F45" s="3" t="n"/>
       <c r="G45" s="3" t="n"/>
       <c r="H45" s="3" t="n"/>
       <c r="I45" s="3" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" t="n">
-        <v>2</v>
-      </c>
-      <c r="B46" t="n">
-        <v>21</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> refranchising loss</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="n">
-        <v>17108</v>
-      </c>
+      <c r="D46" s="3" t="n"/>
       <c r="E46" s="3" t="n"/>
       <c r="F46" s="3" t="n"/>
       <c r="G46" s="3" t="n"/>
@@ -1559,195 +1421,63 @@
       <c r="I46" s="3" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" t="n">
-        <v>2</v>
-      </c>
-      <c r="B47" t="n">
-        <v>22</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> total and</t>
-        </is>
-      </c>
-      <c r="D47" s="3" t="n">
-        <v>2439986</v>
-      </c>
-      <c r="E47" s="3" t="n">
-        <v>2253252</v>
-      </c>
-      <c r="F47" s="3" t="n">
-        <v>2075246</v>
-      </c>
+      <c r="D47" s="3" t="n"/>
+      <c r="E47" s="3" t="n"/>
+      <c r="F47" s="3" t="n"/>
       <c r="G47" s="3" t="n"/>
       <c r="H47" s="3" t="n"/>
       <c r="I47" s="3" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" t="n">
-        <v>2</v>
-      </c>
-      <c r="B48" t="n">
-        <v>24</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> operating profit</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="n">
-        <v>241594</v>
-      </c>
-      <c r="E48" s="3" t="n">
-        <v>275943</v>
-      </c>
-      <c r="F48" s="3" t="n">
-        <v>309756</v>
-      </c>
+      <c r="D48" s="3" t="n"/>
+      <c r="E48" s="3" t="n"/>
+      <c r="F48" s="3" t="n"/>
       <c r="G48" s="3" t="n"/>
       <c r="H48" s="3" t="n"/>
       <c r="I48" s="3" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" t="n">
-        <v>2</v>
-      </c>
-      <c r="B49" t="n">
-        <v>25</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> interest</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="n">
-        <v>3830</v>
-      </c>
-      <c r="E49" s="3" t="n">
-        <v>1824</v>
-      </c>
-      <c r="F49" s="3" t="n">
-        <v>1053</v>
-      </c>
+      <c r="D49" s="3" t="n"/>
+      <c r="E49" s="3" t="n"/>
+      <c r="F49" s="3" t="n"/>
       <c r="G49" s="3" t="n"/>
       <c r="H49" s="3" t="n"/>
       <c r="I49" s="3" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" t="n">
-        <v>2</v>
-      </c>
-      <c r="B50" t="n">
-        <v>27</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other (income)</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="n">
-        <v>1192</v>
-      </c>
-      <c r="E50" s="3" t="n">
-        <v>-3175</v>
-      </c>
-      <c r="F50" s="3" t="n">
-        <v>-4017</v>
-      </c>
+      <c r="D50" s="3" t="n"/>
+      <c r="E50" s="3" t="n"/>
+      <c r="F50" s="3" t="n"/>
       <c r="G50" s="3" t="n"/>
       <c r="H50" s="3" t="n"/>
       <c r="I50" s="3" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" t="n">
-        <v>2</v>
-      </c>
-      <c r="B51" t="n">
-        <v>29</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> income before income taxes</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="n">
-        <v>236572</v>
-      </c>
-      <c r="E51" s="3" t="n">
-        <v>277294</v>
-      </c>
-      <c r="F51" s="3" t="n">
-        <v>312720</v>
-      </c>
+      <c r="D51" s="3" t="n"/>
+      <c r="E51" s="3" t="n"/>
+      <c r="F51" s="3" t="n"/>
       <c r="G51" s="3" t="n"/>
       <c r="H51" s="3" t="n"/>
       <c r="I51" s="3" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" t="n">
-        <v>2</v>
-      </c>
-      <c r="B52" t="n">
-        <v>30</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> income taxes</t>
-        </is>
-      </c>
-      <c r="D52" s="3" t="n">
-        <v>87247</v>
-      </c>
-      <c r="E52" s="3" t="n">
-        <v>98001</v>
-      </c>
-      <c r="F52" s="3" t="n">
-        <v>116551</v>
-      </c>
+      <c r="D52" s="3" t="n"/>
+      <c r="E52" s="3" t="n"/>
+      <c r="F52" s="3" t="n"/>
       <c r="G52" s="3" t="n"/>
       <c r="H52" s="3" t="n"/>
       <c r="I52" s="3" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" t="n">
-        <v>2</v>
-      </c>
-      <c r="B53" t="n">
-        <v>31</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="n">
-        <v>149325</v>
-      </c>
-      <c r="E53" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F53" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D53" s="3" t="n"/>
+      <c r="E53" s="3" t="n"/>
+      <c r="F53" s="3" t="n"/>
       <c r="G53" s="3" t="n"/>
       <c r="H53" s="3" t="n"/>
       <c r="I53" s="3" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" t="n">
-        <v>2</v>
-      </c>
-      <c r="B54" t="n">
-        <v>32</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> less: net loss attributable to noncontrolling interest</t>
-        </is>
-      </c>
-      <c r="D54" s="3" t="n">
-        <v>-17</v>
-      </c>
+      <c r="D54" s="3" t="n"/>
       <c r="E54" s="3" t="n"/>
       <c r="F54" s="3" t="n"/>
       <c r="G54" s="3" t="n"/>
@@ -1755,270 +1485,87 @@
       <c r="I54" s="3" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" t="n">
-        <v>2</v>
-      </c>
-      <c r="B55" t="n">
-        <v>33</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income attributable to panera bread company</t>
-        </is>
-      </c>
-      <c r="D55" s="3" t="n">
-        <v>149342</v>
-      </c>
-      <c r="E55" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F55" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D55" s="3" t="n"/>
+      <c r="E55" s="3" t="n"/>
+      <c r="F55" s="3" t="n"/>
       <c r="G55" s="3" t="n"/>
       <c r="H55" s="3" t="n"/>
       <c r="I55" s="3" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" t="n">
-        <v>2</v>
-      </c>
-      <c r="B56" t="n">
-        <v>36</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> basic</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="n">
-        <v>5.81</v>
-      </c>
-      <c r="E56" s="3" t="n">
-        <v>6.67</v>
-      </c>
-      <c r="F56" s="3" t="n">
-        <v>6.85</v>
-      </c>
+      <c r="D56" s="3" t="n"/>
+      <c r="E56" s="3" t="n"/>
+      <c r="F56" s="3" t="n"/>
       <c r="G56" s="3" t="n"/>
       <c r="H56" s="3" t="n"/>
       <c r="I56" s="3" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" t="n">
-        <v>2</v>
-      </c>
-      <c r="B57" t="n">
-        <v>37</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> diluted</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="n">
-        <v>5.79</v>
-      </c>
-      <c r="E57" s="3" t="n">
-        <v>6.64</v>
-      </c>
-      <c r="F57" s="3" t="n">
-        <v>6.81</v>
-      </c>
+      <c r="D57" s="3" t="n"/>
+      <c r="E57" s="3" t="n"/>
+      <c r="F57" s="3" t="n"/>
       <c r="G57" s="3" t="n"/>
       <c r="H57" s="3" t="n"/>
       <c r="I57" s="3" t="n"/>
     </row>
     <row r="58">
-      <c r="A58" t="n">
-        <v>2</v>
-      </c>
-      <c r="B58" t="n">
-        <v>40</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> basic</t>
-        </is>
-      </c>
-      <c r="D58" s="3" t="n">
-        <v>25685</v>
-      </c>
-      <c r="E58" s="3" t="n">
-        <v>26881</v>
-      </c>
-      <c r="F58" s="3" t="n">
-        <v>28629</v>
-      </c>
+      <c r="D58" s="3" t="n"/>
+      <c r="E58" s="3" t="n"/>
+      <c r="F58" s="3" t="n"/>
       <c r="G58" s="3" t="n"/>
       <c r="H58" s="3" t="n"/>
       <c r="I58" s="3" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" t="n">
-        <v>2</v>
-      </c>
-      <c r="B59" t="n">
-        <v>41</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> viluted 1he accompanying notes are an integral part of the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="n">
-        <v>25788</v>
-      </c>
-      <c r="E59" s="3" t="n">
-        <v>26999</v>
-      </c>
-      <c r="F59" s="3" t="n">
-        <v>28794</v>
-      </c>
+      <c r="D59" s="3" t="n"/>
+      <c r="E59" s="3" t="n"/>
+      <c r="F59" s="3" t="n"/>
       <c r="G59" s="3" t="n"/>
       <c r="H59" s="3" t="n"/>
       <c r="I59" s="3" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" t="n">
-        <v>3</v>
-      </c>
-      <c r="B60" t="n">
-        <v>2</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net income</t>
-        </is>
-      </c>
-      <c r="D60" s="3" t="n">
-        <v>149325</v>
-      </c>
-      <c r="E60" s="3" t="n">
-        <v>179293</v>
-      </c>
-      <c r="F60" s="3" t="n">
-        <v>196169</v>
-      </c>
+      <c r="D60" s="3" t="n"/>
+      <c r="E60" s="3" t="n"/>
+      <c r="F60" s="3" t="n"/>
       <c r="G60" s="3" t="n"/>
       <c r="H60" s="3" t="n"/>
       <c r="I60" s="3" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" t="n">
-        <v>3</v>
-      </c>
-      <c r="B61" t="n">
-        <v>4</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> depreciation and amortization</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="n">
-        <v>135398</v>
-      </c>
-      <c r="E61" s="3" t="n">
-        <v>124109</v>
-      </c>
-      <c r="F61" s="3" t="n">
-        <v>106523</v>
-      </c>
+      <c r="D61" s="3" t="n"/>
+      <c r="E61" s="3" t="n"/>
+      <c r="F61" s="3" t="n"/>
       <c r="G61" s="3" t="n"/>
       <c r="H61" s="3" t="n"/>
       <c r="I61" s="3" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" t="n">
-        <v>3</v>
-      </c>
-      <c r="B62" t="n">
-        <v>5</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> stock-based compensation expense</t>
-        </is>
-      </c>
-      <c r="D62" s="3" t="n">
-        <v>15086</v>
-      </c>
-      <c r="E62" s="3" t="n">
-        <v>10077</v>
-      </c>
-      <c r="F62" s="3" t="n">
-        <v>10703</v>
-      </c>
+      <c r="D62" s="3" t="n"/>
+      <c r="E62" s="3" t="n"/>
+      <c r="F62" s="3" t="n"/>
       <c r="G62" s="3" t="n"/>
       <c r="H62" s="3" t="n"/>
       <c r="I62" s="3" t="n"/>
     </row>
     <row r="63">
-      <c r="A63" t="n">
-        <v>3</v>
-      </c>
-      <c r="B63" t="n">
-        <v>6</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
-      </c>
-      <c r="D63" s="3" t="n">
-        <v>-2057</v>
-      </c>
-      <c r="E63" s="3" t="n">
-        <v>-3089</v>
-      </c>
-      <c r="F63" s="3" t="n">
-        <v>-8100</v>
-      </c>
+      <c r="D63" s="3" t="n"/>
+      <c r="E63" s="3" t="n"/>
+      <c r="F63" s="3" t="n"/>
       <c r="G63" s="3" t="n"/>
       <c r="H63" s="3" t="n"/>
       <c r="I63" s="3" t="n"/>
     </row>
     <row r="64">
-      <c r="A64" t="n">
-        <v>3</v>
-      </c>
-      <c r="B64" t="n">
-        <v>7</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred income taxes</t>
-        </is>
-      </c>
-      <c r="D64" s="3" t="n">
-        <v>-10991</v>
-      </c>
-      <c r="E64" s="3" t="n">
-        <v>10459</v>
-      </c>
-      <c r="F64" s="3" t="n">
-        <v>10356</v>
-      </c>
+      <c r="D64" s="3" t="n"/>
+      <c r="E64" s="3" t="n"/>
+      <c r="F64" s="3" t="n"/>
       <c r="G64" s="3" t="n"/>
       <c r="H64" s="3" t="n"/>
       <c r="I64" s="3" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" t="n">
-        <v>3</v>
-      </c>
-      <c r="B65" t="n">
-        <v>8</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> refranchising loss</t>
-        </is>
-      </c>
-      <c r="D65" s="3" t="n">
-        <v>12942</v>
-      </c>
+      <c r="D65" s="3" t="n"/>
       <c r="E65" s="3" t="n"/>
       <c r="F65" s="3" t="n"/>
       <c r="G65" s="3" t="n"/>
@@ -2026,358 +1573,119 @@
       <c r="I65" s="3" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" t="n">
-        <v>3</v>
-      </c>
-      <c r="B66" t="n">
-        <v>9</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other</t>
-        </is>
-      </c>
-      <c r="D66" s="3" t="n">
-        <v>3505</v>
-      </c>
-      <c r="E66" s="3" t="n">
-        <v>4617</v>
-      </c>
-      <c r="F66" s="3" t="n">
-        <v>6353</v>
-      </c>
+      <c r="D66" s="3" t="n"/>
+      <c r="E66" s="3" t="n"/>
+      <c r="F66" s="3" t="n"/>
       <c r="G66" s="3" t="n"/>
       <c r="H66" s="3" t="n"/>
       <c r="I66" s="3" t="n"/>
     </row>
     <row r="67">
-      <c r="A67" t="n">
-        <v>3</v>
-      </c>
-      <c r="B67" t="n">
-        <v>12</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> trade and other accounts receivable net</t>
-        </is>
-      </c>
-      <c r="D67" s="3" t="n">
-        <v>-3605</v>
-      </c>
-      <c r="E67" s="3" t="n">
-        <v>-22139</v>
-      </c>
-      <c r="F67" s="3" t="n">
-        <v>3021</v>
-      </c>
+      <c r="D67" s="3" t="n"/>
+      <c r="E67" s="3" t="n"/>
+      <c r="F67" s="3" t="n"/>
       <c r="G67" s="3" t="n"/>
       <c r="H67" s="3" t="n"/>
       <c r="I67" s="3" t="n"/>
     </row>
     <row r="68">
-      <c r="A68" t="n">
-        <v>3</v>
-      </c>
-      <c r="B68" t="n">
-        <v>13</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> inventories</t>
-        </is>
-      </c>
-      <c r="D68" s="3" t="n">
-        <v>-1698</v>
-      </c>
-      <c r="E68" s="3" t="n">
-        <v>-895</v>
-      </c>
-      <c r="F68" s="3" t="n">
-        <v>-2186</v>
-      </c>
+      <c r="D68" s="3" t="n"/>
+      <c r="E68" s="3" t="n"/>
+      <c r="F68" s="3" t="n"/>
       <c r="G68" s="3" t="n"/>
       <c r="H68" s="3" t="n"/>
       <c r="I68" s="3" t="n"/>
     </row>
     <row r="69">
-      <c r="A69" t="n">
-        <v>3</v>
-      </c>
-      <c r="B69" t="n">
-        <v>14</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> prepaid and other</t>
-        </is>
-      </c>
-      <c r="D69" s="3" t="n">
-        <v>-7191</v>
-      </c>
-      <c r="E69" s="3" t="n">
-        <v>-8524</v>
-      </c>
-      <c r="F69" s="3" t="n">
-        <v>-841</v>
-      </c>
+      <c r="D69" s="3" t="n"/>
+      <c r="E69" s="3" t="n"/>
+      <c r="F69" s="3" t="n"/>
       <c r="G69" s="3" t="n"/>
       <c r="H69" s="3" t="n"/>
       <c r="I69" s="3" t="n"/>
     </row>
     <row r="70">
-      <c r="A70" t="n">
-        <v>3</v>
-      </c>
-      <c r="B70" t="n">
-        <v>16</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deposits and other</t>
-        </is>
-      </c>
-      <c r="D70" s="3" t="n">
-        <v>-455</v>
-      </c>
-      <c r="E70" s="3" t="n">
-        <v>239</v>
-      </c>
-      <c r="F70" s="3" t="n">
-        <v>1449</v>
-      </c>
+      <c r="D70" s="3" t="n"/>
+      <c r="E70" s="3" t="n"/>
+      <c r="F70" s="3" t="n"/>
       <c r="G70" s="3" t="n"/>
       <c r="H70" s="3" t="n"/>
       <c r="I70" s="3" t="n"/>
     </row>
     <row r="71">
-      <c r="A71" t="n">
-        <v>3</v>
-      </c>
-      <c r="B71" t="n">
-        <v>17</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accounts payable</t>
-        </is>
-      </c>
-      <c r="D71" s="3" t="n">
-        <v>-183</v>
-      </c>
-      <c r="E71" s="3" t="n">
-        <v>1978</v>
-      </c>
-      <c r="F71" s="3" t="n">
-        <v>8162</v>
-      </c>
+      <c r="D71" s="3" t="n"/>
+      <c r="E71" s="3" t="n"/>
+      <c r="F71" s="3" t="n"/>
       <c r="G71" s="3" t="n"/>
       <c r="H71" s="3" t="n"/>
       <c r="I71" s="3" t="n"/>
     </row>
     <row r="72">
-      <c r="A72" t="n">
-        <v>3</v>
-      </c>
-      <c r="B72" t="n">
-        <v>18</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> accrued</t>
-        </is>
-      </c>
-      <c r="D72" s="3" t="n">
-        <v>31169</v>
-      </c>
-      <c r="E72" s="3" t="n">
-        <v>35288</v>
-      </c>
-      <c r="F72" s="3" t="n">
-        <v>13372</v>
-      </c>
+      <c r="D72" s="3" t="n"/>
+      <c r="E72" s="3" t="n"/>
+      <c r="F72" s="3" t="n"/>
       <c r="G72" s="3" t="n"/>
       <c r="H72" s="3" t="n"/>
       <c r="I72" s="3" t="n"/>
     </row>
     <row r="73">
-      <c r="A73" t="n">
-        <v>3</v>
-      </c>
-      <c r="B73" t="n">
-        <v>20</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> deferred rent</t>
-        </is>
-      </c>
-      <c r="D73" s="3" t="n">
-        <v>3751</v>
-      </c>
-      <c r="E73" s="3" t="n">
-        <v>1067</v>
-      </c>
-      <c r="F73" s="3" t="n">
-        <v>5868</v>
-      </c>
+      <c r="D73" s="3" t="n"/>
+      <c r="E73" s="3" t="n"/>
+      <c r="F73" s="3" t="n"/>
       <c r="G73" s="3" t="n"/>
       <c r="H73" s="3" t="n"/>
       <c r="I73" s="3" t="n"/>
     </row>
     <row r="74">
-      <c r="A74" t="n">
-        <v>3</v>
-      </c>
-      <c r="B74" t="n">
-        <v>21</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> other long-term liabilities</t>
-        </is>
-      </c>
-      <c r="D74" s="3" t="n">
-        <v>-6951</v>
-      </c>
-      <c r="E74" s="3" t="n">
-        <v>2599</v>
-      </c>
-      <c r="F74" s="3" t="n">
-        <v>-2432</v>
-      </c>
+      <c r="D74" s="3" t="n"/>
+      <c r="E74" s="3" t="n"/>
+      <c r="F74" s="3" t="n"/>
       <c r="G74" s="3" t="n"/>
       <c r="H74" s="3" t="n"/>
       <c r="I74" s="3" t="n"/>
     </row>
     <row r="75">
-      <c r="A75" t="n">
-        <v>3</v>
-      </c>
-      <c r="B75" t="n">
-        <v>22</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash provided by operating activities</t>
-        </is>
-      </c>
-      <c r="D75" s="3" t="n">
-        <v>318045</v>
-      </c>
-      <c r="E75" s="3" t="n">
-        <v>335079</v>
-      </c>
-      <c r="F75" s="3" t="n">
-        <v>348417</v>
-      </c>
+      <c r="D75" s="3" t="n"/>
+      <c r="E75" s="3" t="n"/>
+      <c r="F75" s="3" t="n"/>
       <c r="G75" s="3" t="n"/>
       <c r="H75" s="3" t="n"/>
       <c r="I75" s="3" t="n"/>
     </row>
     <row r="76">
-      <c r="A76" t="n">
-        <v>3</v>
-      </c>
-      <c r="B76" t="n">
-        <v>24</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> additions to property and equipment</t>
-        </is>
-      </c>
-      <c r="D76" s="3" t="n">
-        <v>-223932</v>
-      </c>
-      <c r="E76" s="3" t="n">
-        <v>-224217</v>
-      </c>
-      <c r="F76" s="3" t="n">
-        <v>-192010</v>
-      </c>
+      <c r="D76" s="3" t="n"/>
+      <c r="E76" s="3" t="n"/>
+      <c r="F76" s="3" t="n"/>
       <c r="G76" s="3" t="n"/>
       <c r="H76" s="3" t="n"/>
       <c r="I76" s="3" t="n"/>
     </row>
     <row r="77">
-      <c r="A77" t="n">
-        <v>3</v>
-      </c>
-      <c r="B77" t="n">
-        <v>25</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> acquisitions net of cash acquired</t>
-        </is>
-      </c>
       <c r="D77" s="3" t="n"/>
       <c r="E77" s="3" t="n"/>
-      <c r="F77" s="3" t="n">
-        <v>-2446</v>
-      </c>
+      <c r="F77" s="3" t="n"/>
       <c r="G77" s="3" t="n"/>
       <c r="H77" s="3" t="n"/>
       <c r="I77" s="3" t="n"/>
     </row>
     <row r="78">
-      <c r="A78" t="n">
-        <v>3</v>
-      </c>
-      <c r="B78" t="n">
-        <v>26</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> purchase of investments</t>
-        </is>
-      </c>
       <c r="D78" s="3" t="n"/>
       <c r="E78" s="3" t="n"/>
-      <c r="F78" s="3" t="n">
-        <v>-97919</v>
-      </c>
+      <c r="F78" s="3" t="n"/>
       <c r="G78" s="3" t="n"/>
       <c r="H78" s="3" t="n"/>
       <c r="I78" s="3" t="n"/>
     </row>
     <row r="79">
-      <c r="A79" t="n">
-        <v>3</v>
-      </c>
-      <c r="B79" t="n">
-        <v>27</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale of investments</t>
-        </is>
-      </c>
       <c r="D79" s="3" t="n"/>
       <c r="E79" s="3" t="n"/>
-      <c r="F79" s="3" t="n">
-        <v>97936</v>
-      </c>
+      <c r="F79" s="3" t="n"/>
       <c r="G79" s="3" t="n"/>
       <c r="H79" s="3" t="n"/>
       <c r="I79" s="3" t="n"/>
     </row>
     <row r="80">
-      <c r="A80" t="n">
-        <v>3</v>
-      </c>
-      <c r="B80" t="n">
-        <v>28</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from refranchising</t>
-        </is>
-      </c>
-      <c r="D80" s="3" t="n">
-        <v>46869</v>
-      </c>
+      <c r="D80" s="3" t="n"/>
       <c r="E80" s="3" t="n"/>
       <c r="F80" s="3" t="n"/>
       <c r="G80" s="3" t="n"/>
@@ -2385,20 +1693,7 @@
       <c r="I80" s="3" t="n"/>
     </row>
     <row r="81">
-      <c r="A81" t="n">
-        <v>3</v>
-      </c>
-      <c r="B81" t="n">
-        <v>29</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale of property and equipment</t>
-        </is>
-      </c>
-      <c r="D81" s="3" t="n">
-        <v>1553</v>
-      </c>
+      <c r="D81" s="3" t="n"/>
       <c r="E81" s="3" t="n"/>
       <c r="F81" s="3" t="n"/>
       <c r="G81" s="3" t="n"/>
@@ -2406,93 +1701,31 @@
       <c r="I81" s="3" t="n"/>
     </row>
     <row r="82">
-      <c r="A82" t="n">
-        <v>3</v>
-      </c>
-      <c r="B82" t="n">
-        <v>30</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from sale-leaseback transactions</t>
-        </is>
-      </c>
-      <c r="D82" s="3" t="n">
-        <v>10095</v>
-      </c>
-      <c r="E82" s="3" t="n">
-        <v>12900</v>
-      </c>
-      <c r="F82" s="3" t="n">
-        <v>6132</v>
-      </c>
+      <c r="D82" s="3" t="n"/>
+      <c r="E82" s="3" t="n"/>
+      <c r="F82" s="3" t="n"/>
       <c r="G82" s="3" t="n"/>
       <c r="H82" s="3" t="n"/>
       <c r="I82" s="3" t="n"/>
     </row>
     <row r="83">
-      <c r="A83" t="n">
-        <v>3</v>
-      </c>
-      <c r="B83" t="n">
-        <v>31</v>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash used in investing activities</t>
-        </is>
-      </c>
-      <c r="D83" s="3" t="n">
-        <v>-165415</v>
-      </c>
-      <c r="E83" s="3" t="n">
-        <v>-211317</v>
-      </c>
-      <c r="F83" s="3" t="n">
-        <v>-188307</v>
-      </c>
+      <c r="D83" s="3" t="n"/>
+      <c r="E83" s="3" t="n"/>
+      <c r="F83" s="3" t="n"/>
       <c r="G83" s="3" t="n"/>
       <c r="H83" s="3" t="n"/>
       <c r="I83" s="3" t="n"/>
     </row>
     <row r="84">
-      <c r="A84" t="n">
-        <v>3</v>
-      </c>
-      <c r="B84" t="n">
-        <v>33</v>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from issuance of long-term debt</t>
-        </is>
-      </c>
-      <c r="D84" s="3" t="n">
-        <v>299070</v>
-      </c>
-      <c r="E84" s="3" t="n">
-        <v>100000</v>
-      </c>
+      <c r="D84" s="3" t="n"/>
+      <c r="E84" s="3" t="n"/>
       <c r="F84" s="3" t="n"/>
       <c r="G84" s="3" t="n"/>
       <c r="H84" s="3" t="n"/>
       <c r="I84" s="3" t="n"/>
     </row>
     <row r="85">
-      <c r="A85" t="n">
-        <v>3</v>
-      </c>
-      <c r="B85" t="n">
-        <v>34</v>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> repayments of long-term debt</t>
-        </is>
-      </c>
-      <c r="D85" s="3" t="n">
-        <v>-6301</v>
-      </c>
+      <c r="D85" s="3" t="n"/>
       <c r="E85" s="3" t="n"/>
       <c r="F85" s="3" t="n"/>
       <c r="G85" s="3" t="n"/>
@@ -2500,247 +1733,81 @@
       <c r="I85" s="3" t="n"/>
     </row>
     <row r="86">
-      <c r="A86" t="n">
-        <v>3</v>
-      </c>
-      <c r="B86" t="n">
-        <v>35</v>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> capitalized debt issuance costs</t>
-        </is>
-      </c>
-      <c r="D86" s="3" t="n">
-        <v>-363</v>
-      </c>
-      <c r="E86" s="3" t="n">
-        <v>-193</v>
-      </c>
+      <c r="D86" s="3" t="n"/>
+      <c r="E86" s="3" t="n"/>
       <c r="F86" s="3" t="n"/>
       <c r="G86" s="3" t="n"/>
       <c r="H86" s="3" t="n"/>
       <c r="I86" s="3" t="n"/>
     </row>
     <row r="87">
-      <c r="A87" t="n">
-        <v>3</v>
-      </c>
-      <c r="B87" t="n">
-        <v>36</v>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> payment of deferred acquisition holdback</t>
-        </is>
-      </c>
       <c r="D87" s="3" t="n"/>
-      <c r="E87" s="3" t="n">
-        <v>-270</v>
-      </c>
-      <c r="F87" s="3" t="n">
-        <v>-4112</v>
-      </c>
+      <c r="E87" s="3" t="n"/>
+      <c r="F87" s="3" t="n"/>
       <c r="G87" s="3" t="n"/>
       <c r="H87" s="3" t="n"/>
       <c r="I87" s="3" t="n"/>
     </row>
     <row r="88">
-      <c r="A88" t="n">
-        <v>3</v>
-      </c>
-      <c r="B88" t="n">
-        <v>37</v>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> repurchase of stock</t>
-        </is>
-      </c>
-      <c r="D88" s="3" t="n">
-        <v>-405513</v>
-      </c>
-      <c r="E88" s="3" t="n">
-        <v>-159503</v>
-      </c>
-      <c r="F88" s="3" t="n">
-        <v>-339409</v>
-      </c>
+      <c r="D88" s="3" t="n"/>
+      <c r="E88" s="3" t="n"/>
+      <c r="F88" s="3" t="n"/>
       <c r="G88" s="3" t="n"/>
       <c r="H88" s="3" t="n"/>
       <c r="I88" s="3" t="n"/>
     </row>
     <row r="89">
-      <c r="A89" t="n">
-        <v>3</v>
-      </c>
-      <c r="B89" t="n">
-        <v>39</v>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> exercise of employee stock options</t>
-        </is>
-      </c>
-      <c r="D89" s="3" t="n">
-        <v>288</v>
-      </c>
-      <c r="E89" s="3" t="n">
-        <v>1116</v>
-      </c>
-      <c r="F89" s="3" t="n">
-        <v>573</v>
-      </c>
+      <c r="D89" s="3" t="n"/>
+      <c r="E89" s="3" t="n"/>
+      <c r="F89" s="3" t="n"/>
       <c r="G89" s="3" t="n"/>
       <c r="H89" s="3" t="n"/>
       <c r="I89" s="3" t="n"/>
     </row>
     <row r="90">
-      <c r="A90" t="n">
-        <v>3</v>
-      </c>
-      <c r="B90" t="n">
-        <v>40</v>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> tax benefit from stock-based compensation</t>
-        </is>
-      </c>
-      <c r="D90" s="3" t="n">
-        <v>2057</v>
-      </c>
-      <c r="E90" s="3" t="n">
-        <v>3089</v>
-      </c>
-      <c r="F90" s="3" t="n">
-        <v>8100</v>
-      </c>
+      <c r="D90" s="3" t="n"/>
+      <c r="E90" s="3" t="n"/>
+      <c r="F90" s="3" t="n"/>
       <c r="G90" s="3" t="n"/>
       <c r="H90" s="3" t="n"/>
       <c r="I90" s="3" t="n"/>
     </row>
     <row r="91">
-      <c r="A91" t="n">
-        <v>3</v>
-      </c>
-      <c r="B91" t="n">
-        <v>41</v>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> proceeds from issuance of common stock under employee benefit plans</t>
-        </is>
-      </c>
-      <c r="D91" s="3" t="n">
-        <v>3525</v>
-      </c>
-      <c r="E91" s="3" t="n">
-        <v>3247</v>
-      </c>
-      <c r="F91" s="3" t="n">
-        <v>2842</v>
-      </c>
+      <c r="D91" s="3" t="n"/>
+      <c r="E91" s="3" t="n"/>
+      <c r="F91" s="3" t="n"/>
       <c r="G91" s="3" t="n"/>
       <c r="H91" s="3" t="n"/>
       <c r="I91" s="3" t="n"/>
     </row>
     <row r="92">
-      <c r="A92" t="n">
-        <v>3</v>
-      </c>
-      <c r="B92" t="n">
-        <v>42</v>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net cash used in financing activities</t>
-        </is>
-      </c>
-      <c r="D92" s="3" t="n">
-        <v>-107237</v>
-      </c>
-      <c r="E92" s="3" t="n">
-        <v>-52514</v>
-      </c>
-      <c r="F92" s="3" t="n">
-        <v>-332006</v>
-      </c>
+      <c r="D92" s="3" t="n"/>
+      <c r="E92" s="3" t="n"/>
+      <c r="F92" s="3" t="n"/>
       <c r="G92" s="3" t="n"/>
       <c r="H92" s="3" t="n"/>
       <c r="I92" s="3" t="n"/>
     </row>
     <row r="93">
-      <c r="A93" t="n">
-        <v>3</v>
-      </c>
-      <c r="B93" t="n">
-        <v>43</v>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> net increase (decrease) in cash and cash equivalents</t>
-        </is>
-      </c>
-      <c r="D93" s="3" t="n">
-        <v>45393</v>
-      </c>
-      <c r="E93" s="3" t="n">
-        <v>71248</v>
-      </c>
-      <c r="F93" s="3" t="n">
-        <v>-171896</v>
-      </c>
+      <c r="D93" s="3" t="n"/>
+      <c r="E93" s="3" t="n"/>
+      <c r="F93" s="3" t="n"/>
       <c r="G93" s="3" t="n"/>
       <c r="H93" s="3" t="n"/>
       <c r="I93" s="3" t="n"/>
     </row>
     <row r="94">
-      <c r="A94" t="n">
-        <v>3</v>
-      </c>
-      <c r="B94" t="n">
-        <v>44</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cash and cash equivalents at beginning of period</t>
-        </is>
-      </c>
-      <c r="D94" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="E94" s="3" t="n">
-        <v>125245</v>
-      </c>
-      <c r="F94" s="3" t="n">
-        <v>297141</v>
-      </c>
+      <c r="D94" s="3" t="n"/>
+      <c r="E94" s="3" t="n"/>
+      <c r="F94" s="3" t="n"/>
       <c r="G94" s="3" t="n"/>
       <c r="H94" s="3" t="n"/>
       <c r="I94" s="3" t="n"/>
     </row>
     <row r="95">
-      <c r="A95" t="n">
-        <v>3</v>
-      </c>
-      <c r="B95" t="n">
-        <v>45</v>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cash and cash equivalents at end of 1he period accompanying notes are an integral part of the consolidated financial statements.</t>
-        </is>
-      </c>
-      <c r="D95" s="3" t="n">
-        <v>241886</v>
-      </c>
-      <c r="E95" s="3" t="n">
-        <v>196493</v>
-      </c>
-      <c r="F95" s="3" t="n">
-        <v>125245</v>
-      </c>
+      <c r="D95" s="3" t="n"/>
+      <c r="E95" s="3" t="n"/>
+      <c r="F95" s="3" t="n"/>
       <c r="G95" s="3" t="n"/>
       <c r="H95" s="3" t="n"/>
       <c r="I95" s="3" t="n"/>

</xml_diff>